<commit_message>
divide variable beta 1
</commit_message>
<xml_diff>
--- a/Instructions/Binary Instructions.xlsx
+++ b/Instructions/Binary Instructions.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="98">
   <si>
     <t>0001</t>
   </si>
@@ -319,6 +319,9 @@
   </si>
   <si>
     <t>10111</t>
+  </si>
+  <si>
+    <t>111</t>
   </si>
 </sst>
 </file>
@@ -707,7 +710,7 @@
   <dimension ref="A1:AQ20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+      <selection activeCell="S2" sqref="S2:S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1626,7 +1629,7 @@
         <v>42</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>20</v>
@@ -1647,10 +1650,10 @@
         <v>20</v>
       </c>
       <c r="I8" s="10" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K8" s="10" t="s">
         <v>30</v>
@@ -1675,11 +1678,11 @@
       </c>
       <c r="R8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>11000000000000000000000000001010</v>
+        <v>01001000000000000001100000001010</v>
       </c>
       <c r="S8" s="4" t="str">
         <f t="shared" si="9"/>
-        <v>C000000A</v>
+        <v>4800180A</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>65</v>
@@ -1689,11 +1692,11 @@
       </c>
       <c r="X8" t="str">
         <f t="shared" si="1"/>
-        <v>1100</v>
+        <v>0100</v>
       </c>
       <c r="Y8" t="str">
         <f t="shared" si="2"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="Z8" t="str">
         <f t="shared" si="3"/>
@@ -1705,11 +1708,11 @@
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="5"/>
-        <v>0000</v>
+        <v>0001</v>
       </c>
       <c r="AC8" t="str">
         <f t="shared" si="6"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="AD8" t="str">
         <f t="shared" si="7"/>
@@ -1721,11 +1724,11 @@
       </c>
       <c r="AG8" t="str">
         <f t="shared" si="10"/>
-        <v>C</v>
+        <v>4</v>
       </c>
       <c r="AH8" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AI8" t="str">
         <f t="shared" si="12"/>
@@ -1737,11 +1740,11 @@
       </c>
       <c r="AK8" t="str">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL8" t="str">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AM8" t="str">
         <f t="shared" si="16"/>
@@ -1762,29 +1765,61 @@
       <c r="A9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="7"/>
-      <c r="N9" s="7"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="7"/>
-      <c r="Q9" s="7"/>
+      <c r="B9" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>30</v>
+      </c>
       <c r="R9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="S9" s="4" t="e">
+        <v>11000000000000000000000000001010</v>
+      </c>
+      <c r="S9" s="4" t="str">
         <f t="shared" si="9"/>
-        <v>#N/A</v>
+        <v>C000000A</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>66</v>
@@ -1794,67 +1829,67 @@
       </c>
       <c r="X9" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>1100</v>
       </c>
       <c r="Y9" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="Z9" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="AA9" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="AB9" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="AC9" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="AD9" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="AE9" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="AG9" t="e">
+        <v>1010</v>
+      </c>
+      <c r="AG9" t="str">
         <f t="shared" si="10"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AH9" t="e">
+        <v>C</v>
+      </c>
+      <c r="AH9" t="str">
         <f t="shared" si="11"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AI9" t="e">
+        <v>0</v>
+      </c>
+      <c r="AI9" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AJ9" t="e">
+        <v>0</v>
+      </c>
+      <c r="AJ9" t="str">
         <f t="shared" si="13"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AK9" t="e">
+        <v>0</v>
+      </c>
+      <c r="AK9" t="str">
         <f t="shared" si="14"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AL9" t="e">
+        <v>0</v>
+      </c>
+      <c r="AL9" t="str">
         <f t="shared" si="15"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AM9" t="e">
+        <v>0</v>
+      </c>
+      <c r="AM9" t="str">
         <f t="shared" si="16"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AN9" t="e">
+        <v>0</v>
+      </c>
+      <c r="AN9" t="str">
         <f t="shared" si="17"/>
-        <v>#N/A</v>
+        <v>A</v>
       </c>
       <c r="AP9" s="1" t="s">
         <v>15</v>
@@ -1867,29 +1902,61 @@
       <c r="A10" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-      <c r="L10" s="11"/>
-      <c r="M10" s="7"/>
-      <c r="N10" s="7"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="7"/>
-      <c r="Q10" s="7"/>
+      <c r="B10" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="L10" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N10" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P10" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q10" s="7" t="s">
+        <v>30</v>
+      </c>
       <c r="R10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="S10" s="4" t="e">
+        <v>00110000111001000000000000000000</v>
+      </c>
+      <c r="S10" s="4" t="str">
         <f t="shared" si="9"/>
-        <v>#N/A</v>
+        <v>30E40000</v>
       </c>
       <c r="U10" s="1" t="s">
         <v>67</v>
@@ -1899,67 +1966,67 @@
       </c>
       <c r="X10" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0011</v>
       </c>
       <c r="Y10" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="Z10" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>1110</v>
       </c>
       <c r="AA10" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>0100</v>
       </c>
       <c r="AB10" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="AC10" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="AD10" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="AE10" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="AG10" t="e">
+        <v>0000</v>
+      </c>
+      <c r="AG10" t="str">
         <f t="shared" si="10"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AH10" t="e">
+        <v>3</v>
+      </c>
+      <c r="AH10" t="str">
         <f t="shared" si="11"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AI10" t="e">
+        <v>0</v>
+      </c>
+      <c r="AI10" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AJ10" t="e">
+        <v>E</v>
+      </c>
+      <c r="AJ10" t="str">
         <f t="shared" si="13"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AK10" t="e">
+        <v>4</v>
+      </c>
+      <c r="AK10" t="str">
         <f t="shared" si="14"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AL10" t="e">
+        <v>0</v>
+      </c>
+      <c r="AL10" t="str">
         <f t="shared" si="15"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AM10" t="e">
+        <v>0</v>
+      </c>
+      <c r="AM10" t="str">
         <f t="shared" si="16"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AN10" t="e">
+        <v>0</v>
+      </c>
+      <c r="AN10" t="str">
         <f t="shared" si="17"/>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AP10" s="1" t="s">
         <v>16</v>
@@ -2581,10 +2648,10 @@
     <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B16">
       <formula1>5</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D16 H2:I16 M2:N16">
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:N16 H2:I16 C2:D16">
       <formula1>3</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:G16 J2:L16 O2:Q16">
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:Q16 J2:L16 E2:G16">
       <formula1>1</formula1>
     </dataValidation>
     <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A16">

</xml_diff>

<commit_message>
divide variable beta 2
</commit_message>
<xml_diff>
--- a/Instructions/Binary Instructions.xlsx
+++ b/Instructions/Binary Instructions.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="99">
   <si>
     <t>0001</t>
   </si>
@@ -321,17 +321,27 @@
     <t>10111</t>
   </si>
   <si>
-    <t>111</t>
+    <t>00000</t>
+  </si>
+  <si>
+    <t>10001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0070C0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -402,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -427,6 +437,14 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -710,7 +728,7 @@
   <dimension ref="A1:AQ20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:S10"/>
+      <selection activeCell="S2" sqref="S2:S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,7 +962,7 @@
         <v>36</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>20</v>
@@ -993,11 +1011,11 @@
       </c>
       <c r="R3" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>00010000001010000000000000001100</v>
+        <v>01001000001010000000000000001100</v>
       </c>
       <c r="S3" s="4" t="str">
         <f t="shared" ref="S3:S16" si="9">AG3&amp;AH3&amp;AI3&amp;AJ3&amp;AK3&amp;AL3&amp;AM3&amp;AN3</f>
-        <v>1028000C</v>
+        <v>4828000C</v>
       </c>
       <c r="U3" s="1" t="s">
         <v>60</v>
@@ -1007,11 +1025,11 @@
       </c>
       <c r="X3" t="str">
         <f t="shared" si="1"/>
-        <v>0001</v>
+        <v>0100</v>
       </c>
       <c r="Y3" t="str">
         <f t="shared" si="2"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="Z3" t="str">
         <f t="shared" si="3"/>
@@ -1039,11 +1057,11 @@
       </c>
       <c r="AG3" t="str">
         <f t="shared" ref="AG3:AG16" si="10">INDEX(AQ:AQ,MATCH(X3,AP:AP,0))</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AH3" t="str">
         <f t="shared" ref="AH3:AH16" si="11">INDEX(AQ:AQ,MATCH(Y3,AP:AP,0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AI3" t="str">
         <f t="shared" ref="AI3:AI16" si="12">INDEX(AQ:AQ,MATCH(Z3,AP:AP,0))</f>
@@ -1087,7 +1105,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>31</v>
@@ -1130,11 +1148,11 @@
       </c>
       <c r="R4" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>01001000001100000000000000001010</v>
+        <v>01001000010100000000000000001010</v>
       </c>
       <c r="S4" s="4" t="str">
         <f t="shared" si="9"/>
-        <v>4830000A</v>
+        <v>4850000A</v>
       </c>
       <c r="U4" s="1" t="s">
         <v>61</v>
@@ -1152,7 +1170,7 @@
       </c>
       <c r="Z4" t="str">
         <f t="shared" si="3"/>
-        <v>0011</v>
+        <v>0101</v>
       </c>
       <c r="AA4" t="str">
         <f t="shared" si="4"/>
@@ -1184,7 +1202,7 @@
       </c>
       <c r="AI4" t="str">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AJ4" t="str">
         <f t="shared" si="13"/>
@@ -1217,61 +1235,61 @@
       <c r="A5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="M5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="N5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="O5" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="P5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q5" s="7" t="s">
+      <c r="B5" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I5" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="K5" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="L5" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="N5" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="P5" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="21" t="s">
         <v>30</v>
       </c>
       <c r="R5" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>00001000001010000001001000001100</v>
+        <v>00010000001010000000000000001100</v>
       </c>
       <c r="S5" s="4" t="str">
         <f t="shared" si="9"/>
-        <v>0828120C</v>
+        <v>1028000C</v>
       </c>
       <c r="U5" s="1" t="s">
         <v>62</v>
@@ -1281,11 +1299,11 @@
       </c>
       <c r="X5" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>0001</v>
       </c>
       <c r="Y5" t="str">
         <f t="shared" si="2"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="Z5" t="str">
         <f t="shared" si="3"/>
@@ -1297,11 +1315,11 @@
       </c>
       <c r="AB5" t="str">
         <f t="shared" si="5"/>
-        <v>0001</v>
+        <v>0000</v>
       </c>
       <c r="AC5" t="str">
         <f t="shared" si="6"/>
-        <v>0010</v>
+        <v>0000</v>
       </c>
       <c r="AD5" t="str">
         <f t="shared" si="7"/>
@@ -1313,11 +1331,11 @@
       </c>
       <c r="AG5" t="str">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH5" t="str">
         <f t="shared" si="11"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AI5" t="str">
         <f t="shared" si="12"/>
@@ -1329,11 +1347,11 @@
       </c>
       <c r="AK5" t="str">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL5" t="str">
         <f t="shared" si="15"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AM5" t="str">
         <f t="shared" si="16"/>
@@ -1354,52 +1372,52 @@
       <c r="A6" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="M6" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="O6" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="P6" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q6" s="6" t="s">
+      <c r="C6" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H6" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="M6" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="N6" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="O6" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="P6" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q6" s="21" t="s">
         <v>30</v>
       </c>
       <c r="R6" s="3" t="str">
@@ -1491,61 +1509,61 @@
       <c r="A7" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E7" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="L7" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="O7" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="P7" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q7" s="6" t="s">
+      <c r="C7" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F7" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="O7" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" s="25" t="s">
         <v>30</v>
       </c>
       <c r="R7" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>00001000001010000001010000001100</v>
+        <v>00001000001010000001001000001100</v>
       </c>
       <c r="S7" s="4" t="str">
         <f t="shared" si="9"/>
-        <v>0828140C</v>
+        <v>0828120C</v>
       </c>
       <c r="U7" s="1" t="s">
         <v>64</v>
@@ -1575,7 +1593,7 @@
       </c>
       <c r="AC7" t="str">
         <f t="shared" si="6"/>
-        <v>0100</v>
+        <v>0010</v>
       </c>
       <c r="AD7" t="str">
         <f t="shared" si="7"/>
@@ -1607,7 +1625,7 @@
       </c>
       <c r="AL7" t="str">
         <f t="shared" si="15"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AM7" t="str">
         <f t="shared" si="16"/>
@@ -1628,61 +1646,61 @@
       <c r="A8" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="C8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="K8" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L8" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="M8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q8" s="6" t="s">
+      <c r="C8" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I8" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="L8" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="O8" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="P8" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q8" s="21" t="s">
         <v>30</v>
       </c>
       <c r="R8" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>01001000000000000001100000001010</v>
+        <v>01001000001100000000000000001010</v>
       </c>
       <c r="S8" s="4" t="str">
         <f t="shared" si="9"/>
-        <v>4800180A</v>
+        <v>4830000A</v>
       </c>
       <c r="U8" s="1" t="s">
         <v>65</v>
@@ -1700,7 +1718,7 @@
       </c>
       <c r="Z8" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>0011</v>
       </c>
       <c r="AA8" t="str">
         <f t="shared" si="4"/>
@@ -1708,11 +1726,11 @@
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="5"/>
-        <v>0001</v>
+        <v>0000</v>
       </c>
       <c r="AC8" t="str">
         <f t="shared" si="6"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="AD8" t="str">
         <f t="shared" si="7"/>
@@ -1732,7 +1750,7 @@
       </c>
       <c r="AI8" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AJ8" t="str">
         <f t="shared" si="13"/>
@@ -1740,11 +1758,11 @@
       </c>
       <c r="AK8" t="str">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL8" t="str">
         <f t="shared" si="15"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AM8" t="str">
         <f t="shared" si="16"/>
@@ -1765,61 +1783,61 @@
       <c r="A9" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="12" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="J9" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="L9" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="P9" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q9" s="6" t="s">
+      <c r="B9" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J9" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="L9" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="M9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="O9" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="P9" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q9" s="21" t="s">
         <v>30</v>
       </c>
       <c r="R9" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>11000000000000000000000000001010</v>
+        <v>00000000000000000000000000000000</v>
       </c>
       <c r="S9" s="4" t="str">
         <f t="shared" si="9"/>
-        <v>C000000A</v>
+        <v>00000000</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>66</v>
@@ -1829,7 +1847,7 @@
       </c>
       <c r="X9" t="str">
         <f t="shared" si="1"/>
-        <v>1100</v>
+        <v>0000</v>
       </c>
       <c r="Y9" t="str">
         <f t="shared" si="2"/>
@@ -1857,11 +1875,11 @@
       </c>
       <c r="AE9" t="str">
         <f t="shared" si="8"/>
-        <v>1010</v>
+        <v>0000</v>
       </c>
       <c r="AG9" t="str">
         <f t="shared" si="10"/>
-        <v>C</v>
+        <v>0</v>
       </c>
       <c r="AH9" t="str">
         <f t="shared" si="11"/>
@@ -1889,7 +1907,7 @@
       </c>
       <c r="AN9" t="str">
         <f t="shared" si="17"/>
-        <v>A</v>
+        <v>0</v>
       </c>
       <c r="AP9" s="1" t="s">
         <v>15</v>
@@ -1902,61 +1920,61 @@
       <c r="A10" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="H10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="L10" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="M10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="N10" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="O10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="P10" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q10" s="7" t="s">
+      <c r="B10" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="L10" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="M10" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="N10" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="O10" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="P10" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q10" s="21" t="s">
         <v>30</v>
       </c>
       <c r="R10" s="3" t="str">
         <f t="shared" si="0"/>
-        <v>00110000111001000000000000000000</v>
+        <v>10001000001010000001010000001100</v>
       </c>
       <c r="S10" s="4" t="str">
         <f t="shared" si="9"/>
-        <v>30E40000</v>
+        <v>8828140C</v>
       </c>
       <c r="U10" s="1" t="s">
         <v>67</v>
@@ -1966,27 +1984,27 @@
       </c>
       <c r="X10" t="str">
         <f t="shared" si="1"/>
-        <v>0011</v>
+        <v>1000</v>
       </c>
       <c r="Y10" t="str">
         <f t="shared" si="2"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="Z10" t="str">
         <f t="shared" si="3"/>
-        <v>1110</v>
+        <v>0010</v>
       </c>
       <c r="AA10" t="str">
         <f t="shared" si="4"/>
-        <v>0100</v>
+        <v>1000</v>
       </c>
       <c r="AB10" t="str">
         <f t="shared" si="5"/>
-        <v>0000</v>
+        <v>0001</v>
       </c>
       <c r="AC10" t="str">
         <f t="shared" si="6"/>
-        <v>0000</v>
+        <v>0100</v>
       </c>
       <c r="AD10" t="str">
         <f t="shared" si="7"/>
@@ -1994,31 +2012,31 @@
       </c>
       <c r="AE10" t="str">
         <f t="shared" si="8"/>
-        <v>0000</v>
+        <v>1100</v>
       </c>
       <c r="AG10" t="str">
         <f t="shared" si="10"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="AH10" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AI10" t="str">
         <f t="shared" si="12"/>
-        <v>E</v>
+        <v>2</v>
       </c>
       <c r="AJ10" t="str">
         <f t="shared" si="13"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AK10" t="str">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL10" t="str">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AM10" t="str">
         <f t="shared" si="16"/>
@@ -2026,7 +2044,7 @@
       </c>
       <c r="AN10" t="str">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>C</v>
       </c>
       <c r="AP10" s="1" t="s">
         <v>16</v>
@@ -2039,93 +2057,125 @@
       <c r="A11" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="7"/>
-      <c r="N11" s="7"/>
-      <c r="O11" s="7"/>
-      <c r="P11" s="7"/>
-      <c r="Q11" s="7"/>
+      <c r="B11" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G11" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I11" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="L11" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="M11" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="N11" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="O11" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="P11" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q11" s="21" t="s">
+        <v>30</v>
+      </c>
       <c r="R11" s="3" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="S11" s="4" t="e">
+        <v>01001000000000000001100000001010</v>
+      </c>
+      <c r="S11" s="4" t="str">
         <f t="shared" si="9"/>
-        <v>#N/A</v>
+        <v>4800180A</v>
       </c>
       <c r="X11" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0100</v>
       </c>
       <c r="Y11" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>1000</v>
       </c>
       <c r="Z11" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="AA11" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="AB11" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>0001</v>
       </c>
       <c r="AC11" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>1000</v>
       </c>
       <c r="AD11" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="AE11" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="AG11" t="e">
+        <v>1010</v>
+      </c>
+      <c r="AG11" t="str">
         <f t="shared" si="10"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AH11" t="e">
+        <v>4</v>
+      </c>
+      <c r="AH11" t="str">
         <f t="shared" si="11"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AI11" t="e">
+        <v>8</v>
+      </c>
+      <c r="AI11" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AJ11" t="e">
+        <v>0</v>
+      </c>
+      <c r="AJ11" t="str">
         <f t="shared" si="13"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AK11" t="e">
+        <v>0</v>
+      </c>
+      <c r="AK11" t="str">
         <f t="shared" si="14"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AL11" t="e">
+        <v>1</v>
+      </c>
+      <c r="AL11" t="str">
         <f t="shared" si="15"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AM11" t="e">
+        <v>8</v>
+      </c>
+      <c r="AM11" t="str">
         <f t="shared" si="16"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AN11" t="e">
+        <v>0</v>
+      </c>
+      <c r="AN11" t="str">
         <f t="shared" si="17"/>
-        <v>#N/A</v>
+        <v>A</v>
       </c>
       <c r="AP11" s="1" t="s">
         <v>17</v>
@@ -2138,93 +2188,125 @@
       <c r="A12" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="7"/>
-      <c r="N12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="Q12" s="7"/>
+      <c r="B12" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I12" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="M12" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="N12" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="O12" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="P12" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q12" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="R12" s="3" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="S12" s="4" t="e">
+        <v>00011000010010000001010000010100</v>
+      </c>
+      <c r="S12" s="4" t="str">
         <f t="shared" si="9"/>
-        <v>#N/A</v>
+        <v>18481414</v>
       </c>
       <c r="X12" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0001</v>
       </c>
       <c r="Y12" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>1000</v>
       </c>
       <c r="Z12" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>0100</v>
       </c>
       <c r="AA12" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>1000</v>
       </c>
       <c r="AB12" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>0001</v>
       </c>
       <c r="AC12" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0100</v>
       </c>
       <c r="AD12" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0001</v>
       </c>
       <c r="AE12" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="AG12" t="e">
+        <v>0100</v>
+      </c>
+      <c r="AG12" t="str">
         <f t="shared" si="10"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AH12" t="e">
+        <v>1</v>
+      </c>
+      <c r="AH12" t="str">
         <f t="shared" si="11"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AI12" t="e">
+        <v>8</v>
+      </c>
+      <c r="AI12" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AJ12" t="e">
+        <v>4</v>
+      </c>
+      <c r="AJ12" t="str">
         <f t="shared" si="13"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AK12" t="e">
+        <v>8</v>
+      </c>
+      <c r="AK12" t="str">
         <f t="shared" si="14"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AL12" t="e">
+        <v>1</v>
+      </c>
+      <c r="AL12" t="str">
         <f t="shared" si="15"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AM12" t="e">
+        <v>4</v>
+      </c>
+      <c r="AM12" t="str">
         <f t="shared" si="16"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AN12" t="e">
+        <v>1</v>
+      </c>
+      <c r="AN12" t="str">
         <f t="shared" si="17"/>
-        <v>#N/A</v>
+        <v>4</v>
       </c>
       <c r="AP12" s="1" t="s">
         <v>71</v>
@@ -2237,93 +2319,125 @@
       <c r="A13" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="7"/>
-      <c r="N13" s="7"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="7"/>
-      <c r="Q13" s="7"/>
+      <c r="B13" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I13" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="L13" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="M13" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="N13" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="O13" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="P13" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q13" s="25" t="s">
+        <v>30</v>
+      </c>
       <c r="R13" s="3" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="S13" s="4" t="e">
+        <v>00110001001001001101001000010010</v>
+      </c>
+      <c r="S13" s="4" t="str">
         <f t="shared" si="9"/>
-        <v>#N/A</v>
+        <v>3124D212</v>
       </c>
       <c r="X13" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>0011</v>
       </c>
       <c r="Y13" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0001</v>
       </c>
       <c r="Z13" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>0010</v>
       </c>
       <c r="AA13" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>0100</v>
       </c>
       <c r="AB13" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>1101</v>
       </c>
       <c r="AC13" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0010</v>
       </c>
       <c r="AD13" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0001</v>
       </c>
       <c r="AE13" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="AG13" t="e">
+        <v>0010</v>
+      </c>
+      <c r="AG13" t="str">
         <f t="shared" si="10"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AH13" t="e">
+        <v>3</v>
+      </c>
+      <c r="AH13" t="str">
         <f t="shared" si="11"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AI13" t="e">
+        <v>1</v>
+      </c>
+      <c r="AI13" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AJ13" t="e">
+        <v>2</v>
+      </c>
+      <c r="AJ13" t="str">
         <f t="shared" si="13"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AK13" t="e">
+        <v>4</v>
+      </c>
+      <c r="AK13" t="str">
         <f t="shared" si="14"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AL13" t="e">
+        <v>D</v>
+      </c>
+      <c r="AL13" t="str">
         <f t="shared" si="15"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AM13" t="e">
+        <v>2</v>
+      </c>
+      <c r="AM13" t="str">
         <f t="shared" si="16"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AN13" t="e">
+        <v>1</v>
+      </c>
+      <c r="AN13" t="str">
         <f t="shared" si="17"/>
-        <v>#N/A</v>
+        <v>2</v>
       </c>
       <c r="AP13" s="1" t="s">
         <v>72</v>
@@ -2336,93 +2450,125 @@
       <c r="A14" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="10"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="6"/>
-      <c r="N14" s="6"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6"/>
-      <c r="Q14" s="6"/>
+      <c r="B14" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="J14" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="K14" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="L14" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="M14" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="O14" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="P14" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q14" s="21" t="s">
+        <v>30</v>
+      </c>
       <c r="R14" s="3" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="S14" s="4" t="e">
+        <v>11000000000000000000000000001010</v>
+      </c>
+      <c r="S14" s="4" t="str">
         <f t="shared" si="9"/>
-        <v>#N/A</v>
+        <v>C000000A</v>
       </c>
       <c r="X14" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>1100</v>
       </c>
       <c r="Y14" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="Z14" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="AA14" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="AB14" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="AC14" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="AD14" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="AE14" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="AG14" t="e">
+        <v>1010</v>
+      </c>
+      <c r="AG14" t="str">
         <f t="shared" si="10"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AH14" t="e">
+        <v>C</v>
+      </c>
+      <c r="AH14" t="str">
         <f t="shared" si="11"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AI14" t="e">
+        <v>0</v>
+      </c>
+      <c r="AI14" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AJ14" t="e">
+        <v>0</v>
+      </c>
+      <c r="AJ14" t="str">
         <f t="shared" si="13"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AK14" t="e">
+        <v>0</v>
+      </c>
+      <c r="AK14" t="str">
         <f t="shared" si="14"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AL14" t="e">
+        <v>0</v>
+      </c>
+      <c r="AL14" t="str">
         <f t="shared" si="15"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AM14" t="e">
+        <v>0</v>
+      </c>
+      <c r="AM14" t="str">
         <f t="shared" si="16"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AN14" t="e">
+        <v>0</v>
+      </c>
+      <c r="AN14" t="str">
         <f t="shared" si="17"/>
-        <v>#N/A</v>
+        <v>A</v>
       </c>
       <c r="AP14" s="1" t="s">
         <v>70</v>
@@ -2435,22 +2581,22 @@
       <c r="A15" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="7"/>
-      <c r="N15" s="7"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="7"/>
-      <c r="Q15" s="7"/>
+      <c r="B15" s="18"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="19"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="19"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20"/>
+      <c r="K15" s="20"/>
+      <c r="L15" s="20"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
       <c r="R15" s="3" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -2648,10 +2794,10 @@
     <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B16">
       <formula1>5</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:N16 H2:I16 C2:D16">
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D16 H2:I16 M2:N16">
       <formula1>3</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2:Q16 J2:L16 E2:G16">
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:G16 J2:L16 O2:Q16">
       <formula1>1</formula1>
     </dataValidation>
     <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A16">

</xml_diff>

<commit_message>
divide variable beta 3
</commit_message>
<xml_diff>
--- a/Instructions/Binary Instructions.xlsx
+++ b/Instructions/Binary Instructions.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="99">
   <si>
     <t>0001</t>
   </si>
@@ -321,10 +321,10 @@
     <t>10111</t>
   </si>
   <si>
-    <t>00000</t>
-  </si>
-  <si>
     <t>10001</t>
+  </si>
+  <si>
+    <t>110</t>
   </si>
 </sst>
 </file>
@@ -725,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ20"/>
+  <dimension ref="A1:AQ19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:S14"/>
+      <selection activeCell="S2" sqref="S2:S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1056,35 +1056,35 @@
         <v>1100</v>
       </c>
       <c r="AG3" t="str">
-        <f t="shared" ref="AG3:AG16" si="10">INDEX(AQ:AQ,MATCH(X3,AP:AP,0))</f>
+        <f>INDEX(AQ:AQ,MATCH(X3,AP:AP,0))</f>
         <v>4</v>
       </c>
       <c r="AH3" t="str">
-        <f t="shared" ref="AH3:AH16" si="11">INDEX(AQ:AQ,MATCH(Y3,AP:AP,0))</f>
+        <f>INDEX(AQ:AQ,MATCH(Y3,AP:AP,0))</f>
         <v>8</v>
       </c>
       <c r="AI3" t="str">
-        <f t="shared" ref="AI3:AI16" si="12">INDEX(AQ:AQ,MATCH(Z3,AP:AP,0))</f>
+        <f>INDEX(AQ:AQ,MATCH(Z3,AP:AP,0))</f>
         <v>2</v>
       </c>
       <c r="AJ3" t="str">
-        <f t="shared" ref="AJ3:AJ16" si="13">INDEX(AQ:AQ,MATCH(AA3,AP:AP,0))</f>
+        <f>INDEX(AQ:AQ,MATCH(AA3,AP:AP,0))</f>
         <v>8</v>
       </c>
       <c r="AK3" t="str">
-        <f t="shared" ref="AK3:AK16" si="14">INDEX(AQ:AQ,MATCH(AB3,AP:AP,0))</f>
+        <f>INDEX(AQ:AQ,MATCH(AB3,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AL3" t="str">
-        <f t="shared" ref="AL3:AL16" si="15">INDEX(AQ:AQ,MATCH(AC3,AP:AP,0))</f>
+        <f>INDEX(AQ:AQ,MATCH(AC3,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AM3" t="str">
-        <f t="shared" ref="AM3:AM16" si="16">INDEX(AQ:AQ,MATCH(AD3,AP:AP,0))</f>
+        <f>INDEX(AQ:AQ,MATCH(AD3,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AN3" t="str">
-        <f t="shared" ref="AN3:AN16" si="17">INDEX(AQ:AQ,MATCH(AE3,AP:AP,0))</f>
+        <f>INDEX(AQ:AQ,MATCH(AE3,AP:AP,0))</f>
         <v>C</v>
       </c>
       <c r="AP3" s="1" t="s">
@@ -1193,35 +1193,35 @@
         <v>1010</v>
       </c>
       <c r="AG4" t="str">
-        <f t="shared" si="10"/>
+        <f>INDEX(AQ:AQ,MATCH(X4,AP:AP,0))</f>
         <v>4</v>
       </c>
       <c r="AH4" t="str">
-        <f t="shared" si="11"/>
+        <f>INDEX(AQ:AQ,MATCH(Y4,AP:AP,0))</f>
         <v>8</v>
       </c>
       <c r="AI4" t="str">
-        <f t="shared" si="12"/>
+        <f>INDEX(AQ:AQ,MATCH(Z4,AP:AP,0))</f>
         <v>5</v>
       </c>
       <c r="AJ4" t="str">
-        <f t="shared" si="13"/>
+        <f>INDEX(AQ:AQ,MATCH(AA4,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AK4" t="str">
-        <f t="shared" si="14"/>
+        <f>INDEX(AQ:AQ,MATCH(AB4,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AL4" t="str">
-        <f t="shared" si="15"/>
+        <f>INDEX(AQ:AQ,MATCH(AC4,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AM4" t="str">
-        <f t="shared" si="16"/>
+        <f>INDEX(AQ:AQ,MATCH(AD4,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AN4" t="str">
-        <f t="shared" si="17"/>
+        <f>INDEX(AQ:AQ,MATCH(AE4,AP:AP,0))</f>
         <v>A</v>
       </c>
       <c r="AP4" s="1" t="s">
@@ -1330,35 +1330,35 @@
         <v>1100</v>
       </c>
       <c r="AG5" t="str">
-        <f t="shared" si="10"/>
+        <f>INDEX(AQ:AQ,MATCH(X5,AP:AP,0))</f>
         <v>1</v>
       </c>
       <c r="AH5" t="str">
-        <f t="shared" si="11"/>
+        <f>INDEX(AQ:AQ,MATCH(Y5,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AI5" t="str">
-        <f t="shared" si="12"/>
+        <f>INDEX(AQ:AQ,MATCH(Z5,AP:AP,0))</f>
         <v>2</v>
       </c>
       <c r="AJ5" t="str">
-        <f t="shared" si="13"/>
+        <f>INDEX(AQ:AQ,MATCH(AA5,AP:AP,0))</f>
         <v>8</v>
       </c>
       <c r="AK5" t="str">
-        <f t="shared" si="14"/>
+        <f>INDEX(AQ:AQ,MATCH(AB5,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AL5" t="str">
-        <f t="shared" si="15"/>
+        <f>INDEX(AQ:AQ,MATCH(AC5,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AM5" t="str">
-        <f t="shared" si="16"/>
+        <f>INDEX(AQ:AQ,MATCH(AD5,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AN5" t="str">
-        <f t="shared" si="17"/>
+        <f>INDEX(AQ:AQ,MATCH(AE5,AP:AP,0))</f>
         <v>C</v>
       </c>
       <c r="AP5" s="1" t="s">
@@ -1467,35 +1467,35 @@
         <v>1010</v>
       </c>
       <c r="AG6" t="str">
-        <f t="shared" si="10"/>
+        <f>INDEX(AQ:AQ,MATCH(X6,AP:AP,0))</f>
         <v>4</v>
       </c>
       <c r="AH6" t="str">
-        <f t="shared" si="11"/>
+        <f>INDEX(AQ:AQ,MATCH(Y6,AP:AP,0))</f>
         <v>8</v>
       </c>
       <c r="AI6" t="str">
-        <f t="shared" si="12"/>
+        <f>INDEX(AQ:AQ,MATCH(Z6,AP:AP,0))</f>
         <v>3</v>
       </c>
       <c r="AJ6" t="str">
-        <f t="shared" si="13"/>
+        <f>INDEX(AQ:AQ,MATCH(AA6,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AK6" t="str">
-        <f t="shared" si="14"/>
+        <f>INDEX(AQ:AQ,MATCH(AB6,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AL6" t="str">
-        <f t="shared" si="15"/>
+        <f>INDEX(AQ:AQ,MATCH(AC6,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AM6" t="str">
-        <f t="shared" si="16"/>
+        <f>INDEX(AQ:AQ,MATCH(AD6,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AN6" t="str">
-        <f t="shared" si="17"/>
+        <f>INDEX(AQ:AQ,MATCH(AE6,AP:AP,0))</f>
         <v>A</v>
       </c>
       <c r="AP6" s="1" t="s">
@@ -1604,35 +1604,35 @@
         <v>1100</v>
       </c>
       <c r="AG7" t="str">
-        <f t="shared" si="10"/>
+        <f>INDEX(AQ:AQ,MATCH(X7,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AH7" t="str">
-        <f t="shared" si="11"/>
+        <f>INDEX(AQ:AQ,MATCH(Y7,AP:AP,0))</f>
         <v>8</v>
       </c>
       <c r="AI7" t="str">
-        <f t="shared" si="12"/>
+        <f>INDEX(AQ:AQ,MATCH(Z7,AP:AP,0))</f>
         <v>2</v>
       </c>
       <c r="AJ7" t="str">
-        <f t="shared" si="13"/>
+        <f>INDEX(AQ:AQ,MATCH(AA7,AP:AP,0))</f>
         <v>8</v>
       </c>
       <c r="AK7" t="str">
-        <f t="shared" si="14"/>
+        <f>INDEX(AQ:AQ,MATCH(AB7,AP:AP,0))</f>
         <v>1</v>
       </c>
       <c r="AL7" t="str">
-        <f t="shared" si="15"/>
+        <f>INDEX(AQ:AQ,MATCH(AC7,AP:AP,0))</f>
         <v>2</v>
       </c>
       <c r="AM7" t="str">
-        <f t="shared" si="16"/>
+        <f>INDEX(AQ:AQ,MATCH(AD7,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AN7" t="str">
-        <f t="shared" si="17"/>
+        <f>INDEX(AQ:AQ,MATCH(AE7,AP:AP,0))</f>
         <v>C</v>
       </c>
       <c r="AP7" s="1" t="s">
@@ -1741,35 +1741,35 @@
         <v>1010</v>
       </c>
       <c r="AG8" t="str">
-        <f t="shared" si="10"/>
+        <f>INDEX(AQ:AQ,MATCH(X8,AP:AP,0))</f>
         <v>4</v>
       </c>
       <c r="AH8" t="str">
-        <f t="shared" si="11"/>
+        <f>INDEX(AQ:AQ,MATCH(Y8,AP:AP,0))</f>
         <v>8</v>
       </c>
       <c r="AI8" t="str">
-        <f t="shared" si="12"/>
+        <f>INDEX(AQ:AQ,MATCH(Z8,AP:AP,0))</f>
         <v>3</v>
       </c>
       <c r="AJ8" t="str">
-        <f t="shared" si="13"/>
+        <f>INDEX(AQ:AQ,MATCH(AA8,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AK8" t="str">
-        <f t="shared" si="14"/>
+        <f>INDEX(AQ:AQ,MATCH(AB8,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AL8" t="str">
-        <f t="shared" si="15"/>
+        <f>INDEX(AQ:AQ,MATCH(AC8,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AM8" t="str">
-        <f t="shared" si="16"/>
+        <f>INDEX(AQ:AQ,MATCH(AD8,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AN8" t="str">
-        <f t="shared" si="17"/>
+        <f>INDEX(AQ:AQ,MATCH(AE8,AP:AP,0))</f>
         <v>A</v>
       </c>
       <c r="AP8" s="1" t="s">
@@ -1790,13 +1790,13 @@
         <v>20</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G9" s="19" t="s">
         <v>30</v>
@@ -1805,13 +1805,13 @@
         <v>20</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="J9" s="20" t="s">
         <v>30</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L9" s="20" t="s">
         <v>30</v>
@@ -1820,10 +1820,10 @@
         <v>20</v>
       </c>
       <c r="N9" s="21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="O9" s="21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P9" s="21" t="s">
         <v>30</v>
@@ -1832,12 +1832,12 @@
         <v>30</v>
       </c>
       <c r="R9" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>00000000000000000000000000000000</v>
+        <f t="shared" ref="R9:R15" si="10">B9&amp;C9&amp;D9&amp;E9&amp;F9&amp;G9&amp;H9&amp;I9&amp;J9&amp;K9&amp;L9&amp;M9&amp;N9&amp;O9&amp;P9&amp;Q9</f>
+        <v>10001000001010000001010000001100</v>
       </c>
       <c r="S9" s="4" t="str">
-        <f t="shared" si="9"/>
-        <v>00000000</v>
+        <f t="shared" ref="S9:S15" si="11">AG9&amp;AH9&amp;AI9&amp;AJ9&amp;AK9&amp;AL9&amp;AM9&amp;AN9</f>
+        <v>8828140C</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>66</v>
@@ -1847,27 +1847,27 @@
       </c>
       <c r="X9" t="str">
         <f t="shared" si="1"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="Y9" t="str">
         <f t="shared" si="2"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="Z9" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>0010</v>
       </c>
       <c r="AA9" t="str">
         <f t="shared" si="4"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="AB9" t="str">
         <f t="shared" si="5"/>
-        <v>0000</v>
+        <v>0001</v>
       </c>
       <c r="AC9" t="str">
         <f t="shared" si="6"/>
-        <v>0000</v>
+        <v>0100</v>
       </c>
       <c r="AD9" t="str">
         <f t="shared" si="7"/>
@@ -1875,39 +1875,39 @@
       </c>
       <c r="AE9" t="str">
         <f t="shared" si="8"/>
-        <v>0000</v>
+        <v>1100</v>
       </c>
       <c r="AG9" t="str">
-        <f t="shared" si="10"/>
-        <v>0</v>
+        <f>INDEX(AQ:AQ,MATCH(X9,AP:AP,0))</f>
+        <v>8</v>
       </c>
       <c r="AH9" t="str">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>INDEX(AQ:AQ,MATCH(Y9,AP:AP,0))</f>
+        <v>8</v>
       </c>
       <c r="AI9" t="str">
-        <f t="shared" si="12"/>
-        <v>0</v>
+        <f>INDEX(AQ:AQ,MATCH(Z9,AP:AP,0))</f>
+        <v>2</v>
       </c>
       <c r="AJ9" t="str">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f>INDEX(AQ:AQ,MATCH(AA9,AP:AP,0))</f>
+        <v>8</v>
       </c>
       <c r="AK9" t="str">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f>INDEX(AQ:AQ,MATCH(AB9,AP:AP,0))</f>
+        <v>1</v>
       </c>
       <c r="AL9" t="str">
-        <f t="shared" si="15"/>
-        <v>0</v>
+        <f>INDEX(AQ:AQ,MATCH(AC9,AP:AP,0))</f>
+        <v>4</v>
       </c>
       <c r="AM9" t="str">
-        <f t="shared" si="16"/>
+        <f>INDEX(AQ:AQ,MATCH(AD9,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AN9" t="str">
-        <f t="shared" si="17"/>
-        <v>0</v>
+        <f>INDEX(AQ:AQ,MATCH(AE9,AP:AP,0))</f>
+        <v>C</v>
       </c>
       <c r="AP9" s="1" t="s">
         <v>15</v>
@@ -1921,19 +1921,19 @@
         <v>88</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>98</v>
+        <v>66</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G10" s="19" t="s">
         <v>30</v>
@@ -1945,10 +1945,10 @@
         <v>18</v>
       </c>
       <c r="J10" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L10" s="20" t="s">
         <v>30</v>
@@ -1960,21 +1960,21 @@
         <v>18</v>
       </c>
       <c r="O10" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P10" s="21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q10" s="21" t="s">
         <v>30</v>
       </c>
       <c r="R10" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>10001000001010000001010000001100</v>
+        <f t="shared" si="10"/>
+        <v>01001000000000000001100000001010</v>
       </c>
       <c r="S10" s="4" t="str">
-        <f t="shared" si="9"/>
-        <v>8828140C</v>
+        <f t="shared" si="11"/>
+        <v>4800180A</v>
       </c>
       <c r="U10" s="1" t="s">
         <v>67</v>
@@ -1984,7 +1984,7 @@
       </c>
       <c r="X10" t="str">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>0100</v>
       </c>
       <c r="Y10" t="str">
         <f t="shared" si="2"/>
@@ -1992,11 +1992,11 @@
       </c>
       <c r="Z10" t="str">
         <f t="shared" si="3"/>
-        <v>0010</v>
+        <v>0000</v>
       </c>
       <c r="AA10" t="str">
         <f t="shared" si="4"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="AB10" t="str">
         <f t="shared" si="5"/>
@@ -2004,7 +2004,7 @@
       </c>
       <c r="AC10" t="str">
         <f t="shared" si="6"/>
-        <v>0100</v>
+        <v>1000</v>
       </c>
       <c r="AD10" t="str">
         <f t="shared" si="7"/>
@@ -2012,39 +2012,39 @@
       </c>
       <c r="AE10" t="str">
         <f t="shared" si="8"/>
-        <v>1100</v>
+        <v>1010</v>
       </c>
       <c r="AG10" t="str">
-        <f t="shared" si="10"/>
+        <f>INDEX(AQ:AQ,MATCH(X10,AP:AP,0))</f>
+        <v>4</v>
+      </c>
+      <c r="AH10" t="str">
+        <f>INDEX(AQ:AQ,MATCH(Y10,AP:AP,0))</f>
         <v>8</v>
       </c>
-      <c r="AH10" t="str">
-        <f t="shared" si="11"/>
+      <c r="AI10" t="str">
+        <f>INDEX(AQ:AQ,MATCH(Z10,AP:AP,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AJ10" t="str">
+        <f>INDEX(AQ:AQ,MATCH(AA10,AP:AP,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AK10" t="str">
+        <f>INDEX(AQ:AQ,MATCH(AB10,AP:AP,0))</f>
+        <v>1</v>
+      </c>
+      <c r="AL10" t="str">
+        <f>INDEX(AQ:AQ,MATCH(AC10,AP:AP,0))</f>
         <v>8</v>
       </c>
-      <c r="AI10" t="str">
-        <f t="shared" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AJ10" t="str">
-        <f t="shared" si="13"/>
-        <v>8</v>
-      </c>
-      <c r="AK10" t="str">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="AL10" t="str">
-        <f t="shared" si="15"/>
-        <v>4</v>
-      </c>
       <c r="AM10" t="str">
-        <f t="shared" si="16"/>
+        <f>INDEX(AQ:AQ,MATCH(AD10,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AN10" t="str">
-        <f t="shared" si="17"/>
-        <v>C</v>
+        <f>INDEX(AQ:AQ,MATCH(AE10,AP:AP,0))</f>
+        <v>A</v>
       </c>
       <c r="AP10" s="1" t="s">
         <v>16</v>
@@ -2058,13 +2058,13 @@
         <v>90</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>20</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>30</v>
@@ -2073,19 +2073,19 @@
         <v>30</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H11" s="20" t="s">
         <v>20</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="J11" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L11" s="20" t="s">
         <v>30</v>
@@ -2094,28 +2094,28 @@
         <v>20</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="O11" s="21" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P11" s="21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q11" s="21" t="s">
         <v>30</v>
       </c>
       <c r="R11" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>01001000000000000001100000001010</v>
+        <f t="shared" si="10"/>
+        <v>00001000001001000011010000011100</v>
       </c>
       <c r="S11" s="4" t="str">
-        <f t="shared" si="9"/>
-        <v>4800180A</v>
+        <f t="shared" si="11"/>
+        <v>0824341C</v>
       </c>
       <c r="X11" t="str">
         <f t="shared" si="1"/>
-        <v>0100</v>
+        <v>0000</v>
       </c>
       <c r="Y11" t="str">
         <f t="shared" si="2"/>
@@ -2123,59 +2123,59 @@
       </c>
       <c r="Z11" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>0010</v>
       </c>
       <c r="AA11" t="str">
         <f t="shared" si="4"/>
-        <v>0000</v>
+        <v>0100</v>
       </c>
       <c r="AB11" t="str">
         <f t="shared" si="5"/>
-        <v>0001</v>
+        <v>0011</v>
       </c>
       <c r="AC11" t="str">
         <f t="shared" si="6"/>
-        <v>1000</v>
+        <v>0100</v>
       </c>
       <c r="AD11" t="str">
         <f t="shared" si="7"/>
-        <v>0000</v>
+        <v>0001</v>
       </c>
       <c r="AE11" t="str">
         <f t="shared" si="8"/>
-        <v>1010</v>
+        <v>1100</v>
       </c>
       <c r="AG11" t="str">
-        <f t="shared" si="10"/>
+        <f>INDEX(AQ:AQ,MATCH(X11,AP:AP,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AH11" t="str">
+        <f>INDEX(AQ:AQ,MATCH(Y11,AP:AP,0))</f>
+        <v>8</v>
+      </c>
+      <c r="AI11" t="str">
+        <f>INDEX(AQ:AQ,MATCH(Z11,AP:AP,0))</f>
+        <v>2</v>
+      </c>
+      <c r="AJ11" t="str">
+        <f>INDEX(AQ:AQ,MATCH(AA11,AP:AP,0))</f>
         <v>4</v>
       </c>
-      <c r="AH11" t="str">
-        <f t="shared" si="11"/>
-        <v>8</v>
-      </c>
-      <c r="AI11" t="str">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="AJ11" t="str">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
       <c r="AK11" t="str">
-        <f t="shared" si="14"/>
+        <f>INDEX(AQ:AQ,MATCH(AB11,AP:AP,0))</f>
+        <v>3</v>
+      </c>
+      <c r="AL11" t="str">
+        <f>INDEX(AQ:AQ,MATCH(AC11,AP:AP,0))</f>
+        <v>4</v>
+      </c>
+      <c r="AM11" t="str">
+        <f>INDEX(AQ:AQ,MATCH(AD11,AP:AP,0))</f>
         <v>1</v>
       </c>
-      <c r="AL11" t="str">
-        <f t="shared" si="15"/>
-        <v>8</v>
-      </c>
-      <c r="AM11" t="str">
-        <f t="shared" si="16"/>
-        <v>0</v>
-      </c>
       <c r="AN11" t="str">
-        <f t="shared" si="17"/>
-        <v>A</v>
+        <f>INDEX(AQ:AQ,MATCH(AE11,AP:AP,0))</f>
+        <v>C</v>
       </c>
       <c r="AP11" s="1" t="s">
         <v>17</v>
@@ -2189,19 +2189,19 @@
         <v>91</v>
       </c>
       <c r="B12" s="22" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C12" s="23" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>30</v>
       </c>
       <c r="F12" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G12" s="23" t="s">
         <v>30</v>
@@ -2210,13 +2210,13 @@
         <v>20</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="J12" s="24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K12" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L12" s="24" t="s">
         <v>30</v>
@@ -2225,28 +2225,28 @@
         <v>20</v>
       </c>
       <c r="N12" s="25" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="O12" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P12" s="25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Q12" s="25" t="s">
         <v>30</v>
       </c>
       <c r="R12" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>00011000010010000001010000010100</v>
+        <f t="shared" si="10"/>
+        <v>01001000000000000011100000011010</v>
       </c>
       <c r="S12" s="4" t="str">
-        <f t="shared" si="9"/>
-        <v>18481414</v>
+        <f t="shared" si="11"/>
+        <v>4800381A</v>
       </c>
       <c r="X12" t="str">
         <f t="shared" si="1"/>
-        <v>0001</v>
+        <v>0100</v>
       </c>
       <c r="Y12" t="str">
         <f t="shared" si="2"/>
@@ -2254,19 +2254,19 @@
       </c>
       <c r="Z12" t="str">
         <f t="shared" si="3"/>
-        <v>0100</v>
+        <v>0000</v>
       </c>
       <c r="AA12" t="str">
         <f t="shared" si="4"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="AB12" t="str">
         <f t="shared" si="5"/>
-        <v>0001</v>
+        <v>0011</v>
       </c>
       <c r="AC12" t="str">
         <f t="shared" si="6"/>
-        <v>0100</v>
+        <v>1000</v>
       </c>
       <c r="AD12" t="str">
         <f t="shared" si="7"/>
@@ -2274,39 +2274,39 @@
       </c>
       <c r="AE12" t="str">
         <f t="shared" si="8"/>
-        <v>0100</v>
+        <v>1010</v>
       </c>
       <c r="AG12" t="str">
-        <f t="shared" si="10"/>
+        <f>INDEX(AQ:AQ,MATCH(X12,AP:AP,0))</f>
+        <v>4</v>
+      </c>
+      <c r="AH12" t="str">
+        <f>INDEX(AQ:AQ,MATCH(Y12,AP:AP,0))</f>
+        <v>8</v>
+      </c>
+      <c r="AI12" t="str">
+        <f>INDEX(AQ:AQ,MATCH(Z12,AP:AP,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AJ12" t="str">
+        <f>INDEX(AQ:AQ,MATCH(AA12,AP:AP,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AK12" t="str">
+        <f>INDEX(AQ:AQ,MATCH(AB12,AP:AP,0))</f>
+        <v>3</v>
+      </c>
+      <c r="AL12" t="str">
+        <f>INDEX(AQ:AQ,MATCH(AC12,AP:AP,0))</f>
+        <v>8</v>
+      </c>
+      <c r="AM12" t="str">
+        <f>INDEX(AQ:AQ,MATCH(AD12,AP:AP,0))</f>
         <v>1</v>
       </c>
-      <c r="AH12" t="str">
-        <f t="shared" si="11"/>
-        <v>8</v>
-      </c>
-      <c r="AI12" t="str">
-        <f t="shared" si="12"/>
-        <v>4</v>
-      </c>
-      <c r="AJ12" t="str">
-        <f t="shared" si="13"/>
-        <v>8</v>
-      </c>
-      <c r="AK12" t="str">
-        <f t="shared" si="14"/>
-        <v>1</v>
-      </c>
-      <c r="AL12" t="str">
-        <f t="shared" si="15"/>
-        <v>4</v>
-      </c>
-      <c r="AM12" t="str">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
       <c r="AN12" t="str">
-        <f t="shared" si="17"/>
-        <v>4</v>
+        <f>INDEX(AQ:AQ,MATCH(AE12,AP:AP,0))</f>
+        <v>A</v>
       </c>
       <c r="AP12" s="1" t="s">
         <v>71</v>
@@ -2320,13 +2320,13 @@
         <v>92</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>30</v>
@@ -2335,28 +2335,28 @@
         <v>30</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>33</v>
+        <v>87</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K13" s="24" t="s">
         <v>30</v>
       </c>
       <c r="L13" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M13" s="25" t="s">
         <v>20</v>
       </c>
       <c r="N13" s="25" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="O13" s="25" t="s">
         <v>30</v>
@@ -2368,36 +2368,36 @@
         <v>30</v>
       </c>
       <c r="R13" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>00110001001001001101001000010010</v>
+        <f t="shared" si="10"/>
+        <v>01001000000000000011100000011010</v>
       </c>
       <c r="S13" s="4" t="str">
-        <f t="shared" si="9"/>
-        <v>3124D212</v>
+        <f t="shared" si="11"/>
+        <v>4800381A</v>
       </c>
       <c r="X13" t="str">
         <f t="shared" si="1"/>
-        <v>0011</v>
+        <v>0100</v>
       </c>
       <c r="Y13" t="str">
         <f t="shared" si="2"/>
-        <v>0001</v>
+        <v>1000</v>
       </c>
       <c r="Z13" t="str">
         <f t="shared" si="3"/>
-        <v>0010</v>
+        <v>0000</v>
       </c>
       <c r="AA13" t="str">
         <f t="shared" si="4"/>
-        <v>0100</v>
+        <v>0000</v>
       </c>
       <c r="AB13" t="str">
         <f t="shared" si="5"/>
-        <v>1101</v>
+        <v>0011</v>
       </c>
       <c r="AC13" t="str">
         <f t="shared" si="6"/>
-        <v>0010</v>
+        <v>1000</v>
       </c>
       <c r="AD13" t="str">
         <f t="shared" si="7"/>
@@ -2405,39 +2405,39 @@
       </c>
       <c r="AE13" t="str">
         <f t="shared" si="8"/>
-        <v>0010</v>
+        <v>1010</v>
       </c>
       <c r="AG13" t="str">
-        <f t="shared" si="10"/>
+        <f>INDEX(AQ:AQ,MATCH(X13,AP:AP,0))</f>
+        <v>4</v>
+      </c>
+      <c r="AH13" t="str">
+        <f>INDEX(AQ:AQ,MATCH(Y13,AP:AP,0))</f>
+        <v>8</v>
+      </c>
+      <c r="AI13" t="str">
+        <f>INDEX(AQ:AQ,MATCH(Z13,AP:AP,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AJ13" t="str">
+        <f>INDEX(AQ:AQ,MATCH(AA13,AP:AP,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AK13" t="str">
+        <f>INDEX(AQ:AQ,MATCH(AB13,AP:AP,0))</f>
         <v>3</v>
       </c>
-      <c r="AH13" t="str">
-        <f t="shared" si="11"/>
+      <c r="AL13" t="str">
+        <f>INDEX(AQ:AQ,MATCH(AC13,AP:AP,0))</f>
+        <v>8</v>
+      </c>
+      <c r="AM13" t="str">
+        <f>INDEX(AQ:AQ,MATCH(AD13,AP:AP,0))</f>
         <v>1</v>
       </c>
-      <c r="AI13" t="str">
-        <f t="shared" si="12"/>
-        <v>2</v>
-      </c>
-      <c r="AJ13" t="str">
-        <f t="shared" si="13"/>
-        <v>4</v>
-      </c>
-      <c r="AK13" t="str">
-        <f t="shared" si="14"/>
-        <v>D</v>
-      </c>
-      <c r="AL13" t="str">
-        <f t="shared" si="15"/>
-        <v>2</v>
-      </c>
-      <c r="AM13" t="str">
-        <f t="shared" si="16"/>
-        <v>1</v>
-      </c>
       <c r="AN13" t="str">
-        <f t="shared" si="17"/>
-        <v>2</v>
+        <f>INDEX(AQ:AQ,MATCH(AE13,AP:AP,0))</f>
+        <v>A</v>
       </c>
       <c r="AP13" s="1" t="s">
         <v>72</v>
@@ -2450,69 +2450,69 @@
       <c r="A14" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="B14" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C14" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="I14" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="J14" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="K14" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="L14" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="M14" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="N14" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="O14" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="P14" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q14" s="21" t="s">
+      <c r="B14" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="I14" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="J14" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="K14" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="L14" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="M14" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="O14" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="P14" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q14" s="25" t="s">
         <v>30</v>
       </c>
       <c r="R14" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v>11000000000000000000000000001010</v>
+        <f t="shared" si="10"/>
+        <v>00110001000001001110001000010010</v>
       </c>
       <c r="S14" s="4" t="str">
-        <f t="shared" si="9"/>
-        <v>C000000A</v>
+        <f t="shared" si="11"/>
+        <v>3104E212</v>
       </c>
       <c r="X14" t="str">
         <f t="shared" si="1"/>
-        <v>1100</v>
+        <v>0011</v>
       </c>
       <c r="Y14" t="str">
         <f t="shared" si="2"/>
-        <v>0000</v>
+        <v>0001</v>
       </c>
       <c r="Z14" t="str">
         <f t="shared" si="3"/>
@@ -2520,55 +2520,55 @@
       </c>
       <c r="AA14" t="str">
         <f t="shared" si="4"/>
-        <v>0000</v>
+        <v>0100</v>
       </c>
       <c r="AB14" t="str">
         <f t="shared" si="5"/>
-        <v>0000</v>
+        <v>1110</v>
       </c>
       <c r="AC14" t="str">
         <f t="shared" si="6"/>
-        <v>0000</v>
+        <v>0010</v>
       </c>
       <c r="AD14" t="str">
         <f t="shared" si="7"/>
-        <v>0000</v>
+        <v>0001</v>
       </c>
       <c r="AE14" t="str">
         <f t="shared" si="8"/>
-        <v>1010</v>
+        <v>0010</v>
       </c>
       <c r="AG14" t="str">
-        <f t="shared" si="10"/>
-        <v>C</v>
+        <f>INDEX(AQ:AQ,MATCH(X14,AP:AP,0))</f>
+        <v>3</v>
       </c>
       <c r="AH14" t="str">
-        <f t="shared" si="11"/>
-        <v>0</v>
+        <f>INDEX(AQ:AQ,MATCH(Y14,AP:AP,0))</f>
+        <v>1</v>
       </c>
       <c r="AI14" t="str">
-        <f t="shared" si="12"/>
+        <f>INDEX(AQ:AQ,MATCH(Z14,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AJ14" t="str">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f>INDEX(AQ:AQ,MATCH(AA14,AP:AP,0))</f>
+        <v>4</v>
       </c>
       <c r="AK14" t="str">
-        <f t="shared" si="14"/>
-        <v>0</v>
+        <f>INDEX(AQ:AQ,MATCH(AB14,AP:AP,0))</f>
+        <v>E</v>
       </c>
       <c r="AL14" t="str">
-        <f t="shared" si="15"/>
-        <v>0</v>
+        <f>INDEX(AQ:AQ,MATCH(AC14,AP:AP,0))</f>
+        <v>2</v>
       </c>
       <c r="AM14" t="str">
-        <f t="shared" si="16"/>
-        <v>0</v>
+        <f>INDEX(AQ:AQ,MATCH(AD14,AP:AP,0))</f>
+        <v>1</v>
       </c>
       <c r="AN14" t="str">
-        <f t="shared" si="17"/>
-        <v>A</v>
+        <f>INDEX(AQ:AQ,MATCH(AE14,AP:AP,0))</f>
+        <v>2</v>
       </c>
       <c r="AP14" s="1" t="s">
         <v>70</v>
@@ -2581,93 +2581,125 @@
       <c r="A15" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="B15" s="18"/>
-      <c r="C15" s="19"/>
-      <c r="D15" s="19"/>
-      <c r="E15" s="19"/>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20"/>
-      <c r="K15" s="20"/>
-      <c r="L15" s="20"/>
-      <c r="M15" s="21"/>
-      <c r="N15" s="21"/>
-      <c r="O15" s="21"/>
-      <c r="P15" s="21"/>
-      <c r="Q15" s="21"/>
+      <c r="B15" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" s="20" t="s">
+        <v>87</v>
+      </c>
+      <c r="J15" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="L15" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="M15" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="N15" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="O15" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="P15" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q15" s="21" t="s">
+        <v>30</v>
+      </c>
       <c r="R15" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="S15" s="4" t="e">
-        <f t="shared" si="9"/>
-        <v>#N/A</v>
+        <f t="shared" si="10"/>
+        <v>11000000000000000011010000001010</v>
+      </c>
+      <c r="S15" s="4" t="str">
+        <f t="shared" si="11"/>
+        <v>C000340A</v>
       </c>
       <c r="X15" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>1100</v>
       </c>
       <c r="Y15" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="Z15" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="AA15" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="AB15" t="str">
         <f t="shared" si="5"/>
-        <v/>
+        <v>0011</v>
       </c>
       <c r="AC15" t="str">
         <f t="shared" si="6"/>
-        <v/>
+        <v>0100</v>
       </c>
       <c r="AD15" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="AE15" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="AG15" t="e">
-        <f t="shared" si="10"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AH15" t="e">
-        <f t="shared" si="11"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AI15" t="e">
-        <f t="shared" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AJ15" t="e">
-        <f t="shared" si="13"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AK15" t="e">
-        <f t="shared" si="14"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AL15" t="e">
-        <f t="shared" si="15"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AM15" t="e">
-        <f t="shared" si="16"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AN15" t="e">
-        <f t="shared" si="17"/>
-        <v>#N/A</v>
+        <v>1010</v>
+      </c>
+      <c r="AG15" t="str">
+        <f>INDEX(AQ:AQ,MATCH(X15,AP:AP,0))</f>
+        <v>C</v>
+      </c>
+      <c r="AH15" t="str">
+        <f>INDEX(AQ:AQ,MATCH(Y15,AP:AP,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AI15" t="str">
+        <f>INDEX(AQ:AQ,MATCH(Z15,AP:AP,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AJ15" t="str">
+        <f>INDEX(AQ:AQ,MATCH(AA15,AP:AP,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AK15" t="str">
+        <f>INDEX(AQ:AQ,MATCH(AB15,AP:AP,0))</f>
+        <v>3</v>
+      </c>
+      <c r="AL15" t="str">
+        <f>INDEX(AQ:AQ,MATCH(AC15,AP:AP,0))</f>
+        <v>4</v>
+      </c>
+      <c r="AM15" t="str">
+        <f>INDEX(AQ:AQ,MATCH(AD15,AP:AP,0))</f>
+        <v>0</v>
+      </c>
+      <c r="AN15" t="str">
+        <f>INDEX(AQ:AQ,MATCH(AE15,AP:AP,0))</f>
+        <v>A</v>
       </c>
       <c r="AP15" s="1" t="s">
         <v>73</v>
@@ -2680,30 +2712,24 @@
       <c r="A16" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="7"/>
-      <c r="N16" s="7"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="7"/>
-      <c r="Q16" s="7"/>
-      <c r="R16" s="3" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="S16" s="4" t="e">
-        <f t="shared" si="9"/>
-        <v>#N/A</v>
-      </c>
+      <c r="B16" s="18"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="19"/>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="20"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="4"/>
       <c r="X16" t="str">
         <f t="shared" si="1"/>
         <v/>
@@ -2737,35 +2763,35 @@
         <v/>
       </c>
       <c r="AG16" t="e">
-        <f t="shared" si="10"/>
+        <f>INDEX(AQ:AQ,MATCH(X16,AP:AP,0))</f>
         <v>#N/A</v>
       </c>
       <c r="AH16" t="e">
-        <f t="shared" si="11"/>
+        <f>INDEX(AQ:AQ,MATCH(Y16,AP:AP,0))</f>
         <v>#N/A</v>
       </c>
       <c r="AI16" t="e">
-        <f t="shared" si="12"/>
+        <f>INDEX(AQ:AQ,MATCH(Z16,AP:AP,0))</f>
         <v>#N/A</v>
       </c>
       <c r="AJ16" t="e">
-        <f t="shared" si="13"/>
+        <f>INDEX(AQ:AQ,MATCH(AA16,AP:AP,0))</f>
         <v>#N/A</v>
       </c>
       <c r="AK16" t="e">
-        <f t="shared" si="14"/>
+        <f>INDEX(AQ:AQ,MATCH(AB16,AP:AP,0))</f>
         <v>#N/A</v>
       </c>
       <c r="AL16" t="e">
-        <f t="shared" si="15"/>
+        <f>INDEX(AQ:AQ,MATCH(AC16,AP:AP,0))</f>
         <v>#N/A</v>
       </c>
       <c r="AM16" t="e">
-        <f t="shared" si="16"/>
+        <f>INDEX(AQ:AQ,MATCH(AD16,AP:AP,0))</f>
         <v>#N/A</v>
       </c>
       <c r="AN16" t="e">
-        <f t="shared" si="17"/>
+        <f>INDEX(AQ:AQ,MATCH(AE16,AP:AP,0))</f>
         <v>#N/A</v>
       </c>
       <c r="AP16" s="1" t="s">
@@ -2783,21 +2809,21 @@
         <v>78</v>
       </c>
     </row>
+    <row r="18" spans="18:43" x14ac:dyDescent="0.25">
+      <c r="V18" s="5"/>
+    </row>
     <row r="19" spans="18:43" x14ac:dyDescent="0.25">
-      <c r="V19" s="5"/>
-    </row>
-    <row r="20" spans="18:43" x14ac:dyDescent="0.25">
-      <c r="R20" s="1"/>
+      <c r="R19" s="1"/>
     </row>
   </sheetData>
   <dataValidations count="4">
     <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B16">
       <formula1>5</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D16 H2:I16 M2:N16">
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D16 M2:N16 H2:I16">
       <formula1>3</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:G16 J2:L16 O2:Q16">
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:G16 O2:Q16 J2:L16">
       <formula1>1</formula1>
     </dataValidation>
     <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A16">

</xml_diff>

<commit_message>
divide variable beta 4
</commit_message>
<xml_diff>
--- a/Instructions/Binary Instructions.xlsx
+++ b/Instructions/Binary Instructions.xlsx
@@ -728,7 +728,7 @@
   <dimension ref="A1:AQ19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:S15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,7 +873,7 @@
         <v>30</v>
       </c>
       <c r="R2" s="3" t="str">
-        <f t="shared" ref="R2:R16" si="0">B2&amp;C2&amp;D2&amp;E2&amp;F2&amp;G2&amp;H2&amp;I2&amp;J2&amp;K2&amp;L2&amp;M2&amp;N2&amp;O2&amp;P2&amp;Q2</f>
+        <f t="shared" ref="R2:R8" si="0">B2&amp;C2&amp;D2&amp;E2&amp;F2&amp;G2&amp;H2&amp;I2&amp;J2&amp;K2&amp;L2&amp;M2&amp;N2&amp;O2&amp;P2&amp;Q2</f>
         <v>10111000001100000001100000000000</v>
       </c>
       <c r="S2" s="4" t="str">
@@ -919,35 +919,35 @@
         <v>0000</v>
       </c>
       <c r="AG2" t="str">
-        <f>INDEX(AQ:AQ,MATCH(X2,AP:AP,0))</f>
+        <f t="shared" ref="AG2:AG16" si="9">INDEX(AQ:AQ,MATCH(X2,AP:AP,0))</f>
         <v>B</v>
       </c>
       <c r="AH2" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Y2,AP:AP,0))</f>
+        <f t="shared" ref="AH2:AH16" si="10">INDEX(AQ:AQ,MATCH(Y2,AP:AP,0))</f>
         <v>8</v>
       </c>
       <c r="AI2" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Z2,AP:AP,0))</f>
+        <f t="shared" ref="AI2:AI16" si="11">INDEX(AQ:AQ,MATCH(Z2,AP:AP,0))</f>
         <v>3</v>
       </c>
       <c r="AJ2" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AA2,AP:AP,0))</f>
+        <f t="shared" ref="AJ2:AJ16" si="12">INDEX(AQ:AQ,MATCH(AA2,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AK2" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AB2,AP:AP,0))</f>
+        <f t="shared" ref="AK2:AK16" si="13">INDEX(AQ:AQ,MATCH(AB2,AP:AP,0))</f>
         <v>1</v>
       </c>
       <c r="AL2" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AC2,AP:AP,0))</f>
+        <f t="shared" ref="AL2:AL16" si="14">INDEX(AQ:AQ,MATCH(AC2,AP:AP,0))</f>
         <v>8</v>
       </c>
       <c r="AM2" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AD2,AP:AP,0))</f>
+        <f t="shared" ref="AM2:AM16" si="15">INDEX(AQ:AQ,MATCH(AD2,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AN2" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AE2,AP:AP,0))</f>
+        <f t="shared" ref="AN2:AN16" si="16">INDEX(AQ:AQ,MATCH(AE2,AP:AP,0))</f>
         <v>0</v>
       </c>
       <c r="AP2" s="1" t="s">
@@ -1014,7 +1014,7 @@
         <v>01001000001010000000000000001100</v>
       </c>
       <c r="S3" s="4" t="str">
-        <f t="shared" ref="S3:S16" si="9">AG3&amp;AH3&amp;AI3&amp;AJ3&amp;AK3&amp;AL3&amp;AM3&amp;AN3</f>
+        <f t="shared" ref="S3:S8" si="17">AG3&amp;AH3&amp;AI3&amp;AJ3&amp;AK3&amp;AL3&amp;AM3&amp;AN3</f>
         <v>4828000C</v>
       </c>
       <c r="U3" s="1" t="s">
@@ -1056,35 +1056,35 @@
         <v>1100</v>
       </c>
       <c r="AG3" t="str">
-        <f>INDEX(AQ:AQ,MATCH(X3,AP:AP,0))</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AH3" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Y3,AP:AP,0))</f>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="AI3" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Z3,AP:AP,0))</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="AJ3" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AA3,AP:AP,0))</f>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="AK3" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AB3,AP:AP,0))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AL3" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AC3,AP:AP,0))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AM3" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AD3,AP:AP,0))</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AN3" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AE3,AP:AP,0))</f>
+        <f t="shared" si="16"/>
         <v>C</v>
       </c>
       <c r="AP3" s="1" t="s">
@@ -1151,7 +1151,7 @@
         <v>01001000010100000000000000001010</v>
       </c>
       <c r="S4" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>4850000A</v>
       </c>
       <c r="U4" s="1" t="s">
@@ -1193,35 +1193,35 @@
         <v>1010</v>
       </c>
       <c r="AG4" t="str">
-        <f>INDEX(AQ:AQ,MATCH(X4,AP:AP,0))</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AH4" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Y4,AP:AP,0))</f>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="AI4" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Z4,AP:AP,0))</f>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="AJ4" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AA4,AP:AP,0))</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AK4" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AB4,AP:AP,0))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AL4" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AC4,AP:AP,0))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AM4" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AD4,AP:AP,0))</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AN4" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AE4,AP:AP,0))</f>
+        <f t="shared" si="16"/>
         <v>A</v>
       </c>
       <c r="AP4" s="1" t="s">
@@ -1288,7 +1288,7 @@
         <v>00010000001010000000000000001100</v>
       </c>
       <c r="S5" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>1028000C</v>
       </c>
       <c r="U5" s="1" t="s">
@@ -1330,35 +1330,35 @@
         <v>1100</v>
       </c>
       <c r="AG5" t="str">
-        <f>INDEX(AQ:AQ,MATCH(X5,AP:AP,0))</f>
+        <f t="shared" si="9"/>
         <v>1</v>
       </c>
       <c r="AH5" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Y5,AP:AP,0))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI5" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Z5,AP:AP,0))</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="AJ5" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AA5,AP:AP,0))</f>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="AK5" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AB5,AP:AP,0))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AL5" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AC5,AP:AP,0))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AM5" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AD5,AP:AP,0))</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AN5" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AE5,AP:AP,0))</f>
+        <f t="shared" si="16"/>
         <v>C</v>
       </c>
       <c r="AP5" s="1" t="s">
@@ -1425,7 +1425,7 @@
         <v>01001000001100000000000000001010</v>
       </c>
       <c r="S6" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>4830000A</v>
       </c>
       <c r="U6" s="1" t="s">
@@ -1467,35 +1467,35 @@
         <v>1010</v>
       </c>
       <c r="AG6" t="str">
-        <f>INDEX(AQ:AQ,MATCH(X6,AP:AP,0))</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AH6" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Y6,AP:AP,0))</f>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="AI6" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Z6,AP:AP,0))</f>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="AJ6" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AA6,AP:AP,0))</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AK6" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AB6,AP:AP,0))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AL6" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AC6,AP:AP,0))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AM6" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AD6,AP:AP,0))</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AN6" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AE6,AP:AP,0))</f>
+        <f t="shared" si="16"/>
         <v>A</v>
       </c>
       <c r="AP6" s="1" t="s">
@@ -1562,7 +1562,7 @@
         <v>00001000001010000001001000001100</v>
       </c>
       <c r="S7" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>0828120C</v>
       </c>
       <c r="U7" s="1" t="s">
@@ -1604,35 +1604,35 @@
         <v>1100</v>
       </c>
       <c r="AG7" t="str">
-        <f>INDEX(AQ:AQ,MATCH(X7,AP:AP,0))</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AH7" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Y7,AP:AP,0))</f>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="AI7" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Z7,AP:AP,0))</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="AJ7" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AA7,AP:AP,0))</f>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="AK7" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AB7,AP:AP,0))</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AL7" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AC7,AP:AP,0))</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="AM7" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AD7,AP:AP,0))</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AN7" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AE7,AP:AP,0))</f>
+        <f t="shared" si="16"/>
         <v>C</v>
       </c>
       <c r="AP7" s="1" t="s">
@@ -1699,7 +1699,7 @@
         <v>01001000001100000000000000001010</v>
       </c>
       <c r="S8" s="4" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="17"/>
         <v>4830000A</v>
       </c>
       <c r="U8" s="1" t="s">
@@ -1741,35 +1741,35 @@
         <v>1010</v>
       </c>
       <c r="AG8" t="str">
-        <f>INDEX(AQ:AQ,MATCH(X8,AP:AP,0))</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AH8" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Y8,AP:AP,0))</f>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="AI8" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Z8,AP:AP,0))</f>
+        <f t="shared" si="11"/>
         <v>3</v>
       </c>
       <c r="AJ8" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AA8,AP:AP,0))</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AK8" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AB8,AP:AP,0))</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AL8" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AC8,AP:AP,0))</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="AM8" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AD8,AP:AP,0))</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AN8" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AE8,AP:AP,0))</f>
+        <f t="shared" si="16"/>
         <v>A</v>
       </c>
       <c r="AP8" s="1" t="s">
@@ -1832,11 +1832,11 @@
         <v>30</v>
       </c>
       <c r="R9" s="3" t="str">
-        <f t="shared" ref="R9:R15" si="10">B9&amp;C9&amp;D9&amp;E9&amp;F9&amp;G9&amp;H9&amp;I9&amp;J9&amp;K9&amp;L9&amp;M9&amp;N9&amp;O9&amp;P9&amp;Q9</f>
+        <f t="shared" ref="R9:R15" si="18">B9&amp;C9&amp;D9&amp;E9&amp;F9&amp;G9&amp;H9&amp;I9&amp;J9&amp;K9&amp;L9&amp;M9&amp;N9&amp;O9&amp;P9&amp;Q9</f>
         <v>10001000001010000001010000001100</v>
       </c>
       <c r="S9" s="4" t="str">
-        <f t="shared" ref="S9:S15" si="11">AG9&amp;AH9&amp;AI9&amp;AJ9&amp;AK9&amp;AL9&amp;AM9&amp;AN9</f>
+        <f t="shared" ref="S9:S15" si="19">AG9&amp;AH9&amp;AI9&amp;AJ9&amp;AK9&amp;AL9&amp;AM9&amp;AN9</f>
         <v>8828140C</v>
       </c>
       <c r="U9" s="1" t="s">
@@ -1878,35 +1878,35 @@
         <v>1100</v>
       </c>
       <c r="AG9" t="str">
-        <f>INDEX(AQ:AQ,MATCH(X9,AP:AP,0))</f>
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
       <c r="AH9" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Y9,AP:AP,0))</f>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="AI9" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Z9,AP:AP,0))</f>
+        <f t="shared" si="11"/>
         <v>2</v>
       </c>
       <c r="AJ9" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AA9,AP:AP,0))</f>
+        <f t="shared" si="12"/>
         <v>8</v>
       </c>
       <c r="AK9" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AB9,AP:AP,0))</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AL9" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AC9,AP:AP,0))</f>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="AM9" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AD9,AP:AP,0))</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AN9" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AE9,AP:AP,0))</f>
+        <f t="shared" si="16"/>
         <v>C</v>
       </c>
       <c r="AP9" s="1" t="s">
@@ -1969,11 +1969,11 @@
         <v>30</v>
       </c>
       <c r="R10" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>01001000000000000001100000001010</v>
       </c>
       <c r="S10" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>4800180A</v>
       </c>
       <c r="U10" s="1" t="s">
@@ -2015,35 +2015,35 @@
         <v>1010</v>
       </c>
       <c r="AG10" t="str">
-        <f>INDEX(AQ:AQ,MATCH(X10,AP:AP,0))</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AH10" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Y10,AP:AP,0))</f>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="AI10" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Z10,AP:AP,0))</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ10" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AA10,AP:AP,0))</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AK10" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AB10,AP:AP,0))</f>
+        <f t="shared" si="13"/>
         <v>1</v>
       </c>
       <c r="AL10" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AC10,AP:AP,0))</f>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="AM10" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AD10,AP:AP,0))</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AN10" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AE10,AP:AP,0))</f>
+        <f t="shared" si="16"/>
         <v>A</v>
       </c>
       <c r="AP10" s="1" t="s">
@@ -2064,31 +2064,31 @@
         <v>20</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>18</v>
+        <v>87</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H11" s="20" t="s">
         <v>20</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>87</v>
+        <v>18</v>
       </c>
       <c r="J11" s="20" t="s">
         <v>30</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L11" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M11" s="21" t="s">
         <v>20</v>
@@ -2106,12 +2106,12 @@
         <v>30</v>
       </c>
       <c r="R11" s="3" t="str">
-        <f t="shared" si="10"/>
-        <v>00001000001001000011010000011100</v>
+        <f t="shared" si="18"/>
+        <v>00001000011010000001001000011100</v>
       </c>
       <c r="S11" s="4" t="str">
-        <f t="shared" si="11"/>
-        <v>0824341C</v>
+        <f t="shared" si="19"/>
+        <v>0868121C</v>
       </c>
       <c r="X11" t="str">
         <f t="shared" si="1"/>
@@ -2123,19 +2123,19 @@
       </c>
       <c r="Z11" t="str">
         <f t="shared" si="3"/>
-        <v>0010</v>
+        <v>0110</v>
       </c>
       <c r="AA11" t="str">
         <f t="shared" si="4"/>
-        <v>0100</v>
+        <v>1000</v>
       </c>
       <c r="AB11" t="str">
         <f t="shared" si="5"/>
-        <v>0011</v>
+        <v>0001</v>
       </c>
       <c r="AC11" t="str">
         <f t="shared" si="6"/>
-        <v>0100</v>
+        <v>0010</v>
       </c>
       <c r="AD11" t="str">
         <f t="shared" si="7"/>
@@ -2146,35 +2146,35 @@
         <v>1100</v>
       </c>
       <c r="AG11" t="str">
-        <f>INDEX(AQ:AQ,MATCH(X11,AP:AP,0))</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AH11" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Y11,AP:AP,0))</f>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="AI11" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Z11,AP:AP,0))</f>
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="AJ11" t="str">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+      <c r="AK11" t="str">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AL11" t="str">
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
-      <c r="AJ11" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AA11,AP:AP,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AK11" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AB11,AP:AP,0))</f>
-        <v>3</v>
-      </c>
-      <c r="AL11" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AC11,AP:AP,0))</f>
-        <v>4</v>
-      </c>
       <c r="AM11" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AD11,AP:AP,0))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="AN11" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AE11,AP:AP,0))</f>
+        <f t="shared" si="16"/>
         <v>C</v>
       </c>
       <c r="AP11" s="1" t="s">
@@ -2195,10 +2195,10 @@
         <v>20</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="E12" s="23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F12" s="23" t="s">
         <v>30</v>
@@ -2237,12 +2237,12 @@
         <v>30</v>
       </c>
       <c r="R12" s="3" t="str">
-        <f t="shared" si="10"/>
-        <v>01001000000000000011100000011010</v>
+        <f t="shared" si="18"/>
+        <v>01001000011100000011100000011010</v>
       </c>
       <c r="S12" s="4" t="str">
-        <f t="shared" si="11"/>
-        <v>4800381A</v>
+        <f t="shared" si="19"/>
+        <v>4870381A</v>
       </c>
       <c r="X12" t="str">
         <f t="shared" si="1"/>
@@ -2254,7 +2254,7 @@
       </c>
       <c r="Z12" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>0111</v>
       </c>
       <c r="AA12" t="str">
         <f t="shared" si="4"/>
@@ -2277,35 +2277,35 @@
         <v>1010</v>
       </c>
       <c r="AG12" t="str">
-        <f>INDEX(AQ:AQ,MATCH(X12,AP:AP,0))</f>
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
       <c r="AH12" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Y12,AP:AP,0))</f>
+        <f t="shared" si="10"/>
         <v>8</v>
       </c>
       <c r="AI12" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Z12,AP:AP,0))</f>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>7</v>
       </c>
       <c r="AJ12" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AA12,AP:AP,0))</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AK12" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AB12,AP:AP,0))</f>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
       <c r="AL12" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AC12,AP:AP,0))</f>
+        <f t="shared" si="14"/>
         <v>8</v>
       </c>
       <c r="AM12" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AD12,AP:AP,0))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="AN12" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AE12,AP:AP,0))</f>
+        <f t="shared" si="16"/>
         <v>A</v>
       </c>
       <c r="AP12" s="1" t="s">
@@ -2320,19 +2320,19 @@
         <v>92</v>
       </c>
       <c r="B13" s="22" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C13" s="23" t="s">
         <v>20</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>30</v>
       </c>
       <c r="F13" s="23" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G13" s="23" t="s">
         <v>30</v>
@@ -2341,13 +2341,13 @@
         <v>20</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>87</v>
+        <v>18</v>
       </c>
       <c r="J13" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K13" s="24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L13" s="24" t="s">
         <v>30</v>
@@ -2356,28 +2356,28 @@
         <v>20</v>
       </c>
       <c r="N13" s="25" t="s">
-        <v>87</v>
+        <v>39</v>
       </c>
       <c r="O13" s="25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P13" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q13" s="25" t="s">
         <v>30</v>
       </c>
       <c r="R13" s="3" t="str">
-        <f t="shared" si="10"/>
-        <v>01001000000000000011100000011010</v>
+        <f t="shared" si="18"/>
+        <v>00011000011010000001010000010100</v>
       </c>
       <c r="S13" s="4" t="str">
-        <f t="shared" si="11"/>
-        <v>4800381A</v>
+        <f t="shared" si="19"/>
+        <v>18681414</v>
       </c>
       <c r="X13" t="str">
         <f t="shared" si="1"/>
-        <v>0100</v>
+        <v>0001</v>
       </c>
       <c r="Y13" t="str">
         <f t="shared" si="2"/>
@@ -2385,19 +2385,19 @@
       </c>
       <c r="Z13" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>0110</v>
       </c>
       <c r="AA13" t="str">
         <f t="shared" si="4"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="AB13" t="str">
         <f t="shared" si="5"/>
-        <v>0011</v>
+        <v>0001</v>
       </c>
       <c r="AC13" t="str">
         <f t="shared" si="6"/>
-        <v>1000</v>
+        <v>0100</v>
       </c>
       <c r="AD13" t="str">
         <f t="shared" si="7"/>
@@ -2405,39 +2405,39 @@
       </c>
       <c r="AE13" t="str">
         <f t="shared" si="8"/>
-        <v>1010</v>
+        <v>0100</v>
       </c>
       <c r="AG13" t="str">
-        <f>INDEX(AQ:AQ,MATCH(X13,AP:AP,0))</f>
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="AH13" t="str">
+        <f t="shared" si="10"/>
+        <v>8</v>
+      </c>
+      <c r="AI13" t="str">
+        <f t="shared" si="11"/>
+        <v>6</v>
+      </c>
+      <c r="AJ13" t="str">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+      <c r="AK13" t="str">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="AL13" t="str">
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
-      <c r="AH13" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Y13,AP:AP,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AI13" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Z13,AP:AP,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AJ13" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AA13,AP:AP,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AK13" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AB13,AP:AP,0))</f>
-        <v>3</v>
-      </c>
-      <c r="AL13" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AC13,AP:AP,0))</f>
-        <v>8</v>
-      </c>
       <c r="AM13" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AD13,AP:AP,0))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="AN13" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AE13,AP:AP,0))</f>
-        <v>A</v>
+        <f t="shared" si="16"/>
+        <v>4</v>
       </c>
       <c r="AP13" s="1" t="s">
         <v>72</v>
@@ -2499,11 +2499,11 @@
         <v>30</v>
       </c>
       <c r="R14" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>00110001000001001110001000010010</v>
       </c>
       <c r="S14" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>3104E212</v>
       </c>
       <c r="X14" t="str">
@@ -2539,35 +2539,35 @@
         <v>0010</v>
       </c>
       <c r="AG14" t="str">
-        <f>INDEX(AQ:AQ,MATCH(X14,AP:AP,0))</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="AH14" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Y14,AP:AP,0))</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="AI14" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Z14,AP:AP,0))</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ14" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AA14,AP:AP,0))</f>
+        <f t="shared" si="12"/>
         <v>4</v>
       </c>
       <c r="AK14" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AB14,AP:AP,0))</f>
+        <f t="shared" si="13"/>
         <v>E</v>
       </c>
       <c r="AL14" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AC14,AP:AP,0))</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="AM14" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AD14,AP:AP,0))</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="AN14" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AE14,AP:AP,0))</f>
+        <f t="shared" si="16"/>
         <v>2</v>
       </c>
       <c r="AP14" s="1" t="s">
@@ -2630,11 +2630,11 @@
         <v>30</v>
       </c>
       <c r="R15" s="3" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="18"/>
         <v>11000000000000000011010000001010</v>
       </c>
       <c r="S15" s="4" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="19"/>
         <v>C000340A</v>
       </c>
       <c r="X15" t="str">
@@ -2670,35 +2670,35 @@
         <v>1010</v>
       </c>
       <c r="AG15" t="str">
-        <f>INDEX(AQ:AQ,MATCH(X15,AP:AP,0))</f>
+        <f t="shared" si="9"/>
         <v>C</v>
       </c>
       <c r="AH15" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Y15,AP:AP,0))</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AI15" t="str">
-        <f>INDEX(AQ:AQ,MATCH(Z15,AP:AP,0))</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AJ15" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AA15,AP:AP,0))</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="AK15" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AB15,AP:AP,0))</f>
+        <f t="shared" si="13"/>
         <v>3</v>
       </c>
       <c r="AL15" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AC15,AP:AP,0))</f>
+        <f t="shared" si="14"/>
         <v>4</v>
       </c>
       <c r="AM15" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AD15,AP:AP,0))</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="AN15" t="str">
-        <f>INDEX(AQ:AQ,MATCH(AE15,AP:AP,0))</f>
+        <f t="shared" si="16"/>
         <v>A</v>
       </c>
       <c r="AP15" s="1" t="s">
@@ -2763,35 +2763,35 @@
         <v/>
       </c>
       <c r="AG16" t="e">
-        <f>INDEX(AQ:AQ,MATCH(X16,AP:AP,0))</f>
+        <f t="shared" si="9"/>
         <v>#N/A</v>
       </c>
       <c r="AH16" t="e">
-        <f>INDEX(AQ:AQ,MATCH(Y16,AP:AP,0))</f>
+        <f t="shared" si="10"/>
         <v>#N/A</v>
       </c>
       <c r="AI16" t="e">
-        <f>INDEX(AQ:AQ,MATCH(Z16,AP:AP,0))</f>
+        <f t="shared" si="11"/>
         <v>#N/A</v>
       </c>
       <c r="AJ16" t="e">
-        <f>INDEX(AQ:AQ,MATCH(AA16,AP:AP,0))</f>
+        <f t="shared" si="12"/>
         <v>#N/A</v>
       </c>
       <c r="AK16" t="e">
-        <f>INDEX(AQ:AQ,MATCH(AB16,AP:AP,0))</f>
+        <f t="shared" si="13"/>
         <v>#N/A</v>
       </c>
       <c r="AL16" t="e">
-        <f>INDEX(AQ:AQ,MATCH(AC16,AP:AP,0))</f>
+        <f t="shared" si="14"/>
         <v>#N/A</v>
       </c>
       <c r="AM16" t="e">
-        <f>INDEX(AQ:AQ,MATCH(AD16,AP:AP,0))</f>
+        <f t="shared" si="15"/>
         <v>#N/A</v>
       </c>
       <c r="AN16" t="e">
-        <f>INDEX(AQ:AQ,MATCH(AE16,AP:AP,0))</f>
+        <f t="shared" si="16"/>
         <v>#N/A</v>
       </c>
       <c r="AP16" s="1" t="s">

</xml_diff>

<commit_message>
divide variable beta 5 close
</commit_message>
<xml_diff>
--- a/Instructions/Binary Instructions.xlsx
+++ b/Instructions/Binary Instructions.xlsx
@@ -728,7 +728,7 @@
   <dimension ref="A1:AQ19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="S2" sqref="S2:S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2210,10 +2210,10 @@
         <v>20</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="J12" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K12" s="24" t="s">
         <v>30</v>
@@ -2238,11 +2238,11 @@
       </c>
       <c r="R12" s="3" t="str">
         <f t="shared" si="18"/>
-        <v>01001000011100000011100000011010</v>
+        <v>01001000011100000000000000011010</v>
       </c>
       <c r="S12" s="4" t="str">
         <f t="shared" si="19"/>
-        <v>4870381A</v>
+        <v>4870001A</v>
       </c>
       <c r="X12" t="str">
         <f t="shared" si="1"/>
@@ -2262,11 +2262,11 @@
       </c>
       <c r="AB12" t="str">
         <f t="shared" si="5"/>
-        <v>0011</v>
+        <v>0000</v>
       </c>
       <c r="AC12" t="str">
         <f t="shared" si="6"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="AD12" t="str">
         <f t="shared" si="7"/>
@@ -2294,11 +2294,11 @@
       </c>
       <c r="AK12" t="str">
         <f t="shared" si="13"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AL12" t="str">
         <f t="shared" si="14"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AM12" t="str">
         <f t="shared" si="15"/>
@@ -2588,13 +2588,13 @@
         <v>20</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>20</v>
+        <v>87</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G15" s="19" t="s">
         <v>30</v>
@@ -2603,13 +2603,13 @@
         <v>20</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="J15" s="20" t="s">
         <v>30</v>
       </c>
       <c r="K15" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L15" s="20" t="s">
         <v>30</v>
@@ -2631,11 +2631,11 @@
       </c>
       <c r="R15" s="3" t="str">
         <f t="shared" si="18"/>
-        <v>11000000000000000011010000001010</v>
+        <v>11000000011010000000000000001010</v>
       </c>
       <c r="S15" s="4" t="str">
         <f t="shared" si="19"/>
-        <v>C000340A</v>
+        <v>C068000A</v>
       </c>
       <c r="X15" t="str">
         <f t="shared" si="1"/>
@@ -2647,19 +2647,19 @@
       </c>
       <c r="Z15" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>0110</v>
       </c>
       <c r="AA15" t="str">
         <f t="shared" si="4"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="AB15" t="str">
         <f t="shared" si="5"/>
-        <v>0011</v>
+        <v>0000</v>
       </c>
       <c r="AC15" t="str">
         <f t="shared" si="6"/>
-        <v>0100</v>
+        <v>0000</v>
       </c>
       <c r="AD15" t="str">
         <f t="shared" si="7"/>
@@ -2679,19 +2679,19 @@
       </c>
       <c r="AI15" t="str">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AJ15" t="str">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AK15" t="str">
         <f t="shared" si="13"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AL15" t="str">
         <f t="shared" si="14"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AM15" t="str">
         <f t="shared" si="15"/>

</xml_diff>

<commit_message>
divide variable beta 6 very close
</commit_message>
<xml_diff>
--- a/Instructions/Binary Instructions.xlsx
+++ b/Instructions/Binary Instructions.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="98">
   <si>
     <t>0001</t>
   </si>
@@ -319,9 +319,6 @@
   </si>
   <si>
     <t>10111</t>
-  </si>
-  <si>
-    <t>10001</t>
   </si>
   <si>
     <t>110</t>
@@ -1784,7 +1781,7 @@
         <v>43</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>97</v>
+        <v>58</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>20</v>
@@ -1833,11 +1830,11 @@
       </c>
       <c r="R9" s="3" t="str">
         <f t="shared" ref="R9:R15" si="18">B9&amp;C9&amp;D9&amp;E9&amp;F9&amp;G9&amp;H9&amp;I9&amp;J9&amp;K9&amp;L9&amp;M9&amp;N9&amp;O9&amp;P9&amp;Q9</f>
-        <v>10001000001010000001010000001100</v>
+        <v>00001000001010000001010000001100</v>
       </c>
       <c r="S9" s="4" t="str">
         <f t="shared" ref="S9:S15" si="19">AG9&amp;AH9&amp;AI9&amp;AJ9&amp;AK9&amp;AL9&amp;AM9&amp;AN9</f>
-        <v>8828140C</v>
+        <v>0828140C</v>
       </c>
       <c r="U9" s="1" t="s">
         <v>66</v>
@@ -1847,7 +1844,7 @@
       </c>
       <c r="X9" t="str">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="Y9" t="str">
         <f t="shared" si="2"/>
@@ -1879,7 +1876,7 @@
       </c>
       <c r="AG9" t="str">
         <f t="shared" si="9"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AH9" t="str">
         <f t="shared" si="10"/>
@@ -2472,7 +2469,7 @@
         <v>18</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="J14" s="24" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
test3 seems to fix the bugs
</commit_message>
<xml_diff>
--- a/Instructions/Binary Instructions.xlsx
+++ b/Instructions/Binary Instructions.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="532" uniqueCount="112">
   <si>
     <t>0001</t>
   </si>
@@ -325,6 +325,45 @@
   </si>
   <si>
     <t>010000</t>
+  </si>
+  <si>
+    <t>010001</t>
+  </si>
+  <si>
+    <t>010010</t>
+  </si>
+  <si>
+    <t>010011</t>
+  </si>
+  <si>
+    <t>010100</t>
+  </si>
+  <si>
+    <t>010101</t>
+  </si>
+  <si>
+    <t>010110</t>
+  </si>
+  <si>
+    <t>010111</t>
+  </si>
+  <si>
+    <t>011000</t>
+  </si>
+  <si>
+    <t>011001</t>
+  </si>
+  <si>
+    <t>011010</t>
+  </si>
+  <si>
+    <t>011011</t>
+  </si>
+  <si>
+    <t>011100</t>
+  </si>
+  <si>
+    <t>011101</t>
   </si>
 </sst>
 </file>
@@ -725,10 +764,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ21"/>
+  <dimension ref="A1:AQ30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:S17"/>
+      <selection activeCell="S2" sqref="S2:S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2582,34 +2621,34 @@
         <v>94</v>
       </c>
       <c r="B15" s="22" t="s">
-        <v>89</v>
+        <v>66</v>
       </c>
       <c r="C15" s="23" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="E15" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="G15" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="I15" s="24" t="s">
-        <v>18</v>
-      </c>
       <c r="J15" s="24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K15" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L15" s="24" t="s">
         <v>30</v>
@@ -2618,7 +2657,7 @@
         <v>20</v>
       </c>
       <c r="N15" s="25" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="O15" s="25" t="s">
         <v>30</v>
@@ -2631,35 +2670,35 @@
       </c>
       <c r="R15" s="3" t="str">
         <f>B15&amp;C15&amp;D15&amp;E15&amp;F15&amp;G15&amp;H15&amp;I15&amp;J15&amp;K15&amp;L15&amp;M15&amp;N15&amp;O15&amp;P15&amp;Q15</f>
-        <v>11000000011010000001010000010010</v>
+        <v>01001000000000000011100000011010</v>
       </c>
       <c r="S15" s="4" t="str">
         <f t="shared" si="11"/>
-        <v>C0681412</v>
+        <v>4800381A</v>
       </c>
       <c r="X15" t="str">
         <f t="shared" si="1"/>
-        <v>1100</v>
+        <v>0100</v>
       </c>
       <c r="Y15" t="str">
         <f t="shared" si="2"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="Z15" t="str">
         <f t="shared" si="3"/>
-        <v>0110</v>
+        <v>0000</v>
       </c>
       <c r="AA15" t="str">
         <f t="shared" si="4"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="AB15" t="str">
         <f t="shared" si="5"/>
-        <v>0001</v>
+        <v>0011</v>
       </c>
       <c r="AC15" t="str">
         <f t="shared" si="6"/>
-        <v>0100</v>
+        <v>1000</v>
       </c>
       <c r="AD15" t="str">
         <f t="shared" si="7"/>
@@ -2667,31 +2706,31 @@
       </c>
       <c r="AE15" t="str">
         <f t="shared" si="8"/>
-        <v>0010</v>
+        <v>1010</v>
       </c>
       <c r="AG15" t="str">
         <f>INDEX(AQ:AQ,MATCH(X15,AP:AP,0))</f>
-        <v>C</v>
+        <v>4</v>
       </c>
       <c r="AH15" t="str">
         <f>INDEX(AQ:AQ,MATCH(Y15,AP:AP,0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AI15" t="str">
         <f>INDEX(AQ:AQ,MATCH(Z15,AP:AP,0))</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AJ15" t="str">
         <f>INDEX(AQ:AQ,MATCH(AA15,AP:AP,0))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AK15" t="str">
         <f>INDEX(AQ:AQ,MATCH(AB15,AP:AP,0))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AL15" t="str">
         <f>INDEX(AQ:AQ,MATCH(AC15,AP:AP,0))</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AM15" t="str">
         <f>INDEX(AQ:AQ,MATCH(AD15,AP:AP,0))</f>
@@ -2699,7 +2738,7 @@
       </c>
       <c r="AN15" t="str">
         <f>INDEX(AQ:AQ,MATCH(AE15,AP:AP,0))</f>
-        <v>2</v>
+        <v>A</v>
       </c>
       <c r="AP15" s="1" t="s">
         <v>73</v>
@@ -2713,84 +2752,84 @@
         <v>95</v>
       </c>
       <c r="B16" s="22" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C16" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="23" t="s">
+      <c r="E16" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I16" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="E16" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="23" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="H16" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="I16" s="24" t="s">
-        <v>20</v>
-      </c>
       <c r="J16" s="24" t="s">
         <v>30</v>
       </c>
       <c r="K16" s="24" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L16" s="24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M16" s="25" t="s">
         <v>20</v>
       </c>
       <c r="N16" s="25" t="s">
-        <v>39</v>
+        <v>87</v>
       </c>
       <c r="O16" s="25" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P16" s="25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q16" s="25" t="s">
         <v>30</v>
       </c>
       <c r="R16" s="3" t="str">
         <f>B16&amp;C16&amp;D16&amp;E16&amp;F16&amp;G16&amp;H16&amp;I16&amp;J16&amp;K16&amp;L16&amp;M16&amp;N16&amp;O16&amp;P16&amp;Q16</f>
-        <v>00110001011001010000001000010010</v>
+        <v>00001000001001000011010000011100</v>
       </c>
       <c r="S16" s="4" t="str">
         <f t="shared" si="11"/>
-        <v>31650212</v>
+        <v>0824341C</v>
       </c>
       <c r="X16" t="str">
         <f t="shared" si="1"/>
-        <v>0011</v>
+        <v>0000</v>
       </c>
       <c r="Y16" t="str">
         <f t="shared" si="2"/>
-        <v>0001</v>
+        <v>1000</v>
       </c>
       <c r="Z16" t="str">
         <f t="shared" si="3"/>
-        <v>0110</v>
+        <v>0010</v>
       </c>
       <c r="AA16" t="str">
         <f t="shared" si="4"/>
-        <v>0101</v>
+        <v>0100</v>
       </c>
       <c r="AB16" t="str">
         <f t="shared" si="5"/>
-        <v>0000</v>
+        <v>0011</v>
       </c>
       <c r="AC16" t="str">
         <f t="shared" si="6"/>
-        <v>0010</v>
+        <v>0100</v>
       </c>
       <c r="AD16" t="str">
         <f t="shared" si="7"/>
@@ -2798,31 +2837,31 @@
       </c>
       <c r="AE16" t="str">
         <f t="shared" si="8"/>
-        <v>0010</v>
+        <v>1100</v>
       </c>
       <c r="AG16" t="str">
         <f>INDEX(AQ:AQ,MATCH(X16,AP:AP,0))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AH16" t="str">
         <f>INDEX(AQ:AQ,MATCH(Y16,AP:AP,0))</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="AI16" t="str">
         <f>INDEX(AQ:AQ,MATCH(Z16,AP:AP,0))</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AJ16" t="str">
         <f>INDEX(AQ:AQ,MATCH(AA16,AP:AP,0))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AK16" t="str">
         <f>INDEX(AQ:AQ,MATCH(AB16,AP:AP,0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL16" t="str">
         <f>INDEX(AQ:AQ,MATCH(AC16,AP:AP,0))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AM16" t="str">
         <f>INDEX(AQ:AQ,MATCH(AD16,AP:AP,0))</f>
@@ -2830,7 +2869,7 @@
       </c>
       <c r="AN16" t="str">
         <f>INDEX(AQ:AQ,MATCH(AE16,AP:AP,0))</f>
-        <v>2</v>
+        <v>C</v>
       </c>
       <c r="AP16" s="1" t="s">
         <v>74</v>
@@ -2843,89 +2882,89 @@
       <c r="A17" s="7" t="s">
         <v>98</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="C17" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="19" t="s">
+      <c r="B17" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="E17" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="I17" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="J17" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="K17" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="L17" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="M17" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="N17" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="O17" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="P17" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q17" s="21" t="s">
+      <c r="J17" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="K17" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="L17" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="M17" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="N17" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="O17" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="P17" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q17" s="25" t="s">
         <v>30</v>
       </c>
       <c r="R17" s="3" t="str">
         <f>B17&amp;C17&amp;D17&amp;E17&amp;F17&amp;G17&amp;H17&amp;I17&amp;J17&amp;K17&amp;L17&amp;M17&amp;N17&amp;O17&amp;P17&amp;Q17</f>
-        <v>11000000011010000000000000001010</v>
+        <v>01001000000000000011100000011010</v>
       </c>
       <c r="S17" s="4" t="str">
         <f t="shared" si="11"/>
-        <v>C068000A</v>
+        <v>4800381A</v>
       </c>
       <c r="X17" t="str">
         <f t="shared" ref="X17:X21" si="12">LEFT(RIGHT(R17,32),4)</f>
-        <v>1100</v>
+        <v>0100</v>
       </c>
       <c r="Y17" t="str">
         <f t="shared" ref="Y17:Y21" si="13">LEFT(RIGHT(R17,28),4)</f>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="Z17" t="str">
         <f t="shared" ref="Z17:Z21" si="14">LEFT(RIGHT(R17,24),4)</f>
-        <v>0110</v>
+        <v>0000</v>
       </c>
       <c r="AA17" t="str">
         <f t="shared" ref="AA17:AA21" si="15">LEFT(RIGHT(R17,20),4)</f>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="AB17" t="str">
         <f t="shared" ref="AB17:AB21" si="16">LEFT(RIGHT(R17,16),4)</f>
-        <v>0000</v>
+        <v>0011</v>
       </c>
       <c r="AC17" t="str">
         <f t="shared" ref="AC17:AC21" si="17">LEFT(RIGHT(R17,12),4)</f>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="AD17" t="str">
         <f t="shared" ref="AD17:AD21" si="18">LEFT(RIGHT(R17,8),4)</f>
-        <v>0000</v>
+        <v>0001</v>
       </c>
       <c r="AE17" t="str">
         <f t="shared" ref="AE17:AE21" si="19">LEFT(RIGHT(R17,4),4)</f>
@@ -2933,31 +2972,31 @@
       </c>
       <c r="AG17" t="str">
         <f t="shared" ref="AG17:AG21" si="20">INDEX(AQ:AQ,MATCH(X17,AP:AP,0))</f>
-        <v>C</v>
+        <v>4</v>
       </c>
       <c r="AH17" t="str">
         <f t="shared" ref="AH17:AH21" si="21">INDEX(AQ:AQ,MATCH(Y17,AP:AP,0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AI17" t="str">
         <f t="shared" ref="AI17:AI21" si="22">INDEX(AQ:AQ,MATCH(Z17,AP:AP,0))</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AJ17" t="str">
         <f t="shared" ref="AJ17:AJ21" si="23">INDEX(AQ:AQ,MATCH(AA17,AP:AP,0))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AK17" t="str">
         <f t="shared" ref="AK17:AK21" si="24">INDEX(AQ:AQ,MATCH(AB17,AP:AP,0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL17" t="str">
         <f t="shared" ref="AL17:AL21" si="25">INDEX(AQ:AQ,MATCH(AC17,AP:AP,0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AM17" t="str">
         <f t="shared" ref="AM17:AM21" si="26">INDEX(AQ:AQ,MATCH(AD17,AP:AP,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN17" t="str">
         <f t="shared" ref="AN17:AN21" si="27">INDEX(AQ:AQ,MATCH(AE17,AP:AP,0))</f>
@@ -2971,206 +3010,409 @@
       </c>
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E18" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="K18" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="L18" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="M18" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="N18" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="O18" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="P18" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q18" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="R18" s="3" t="str">
+        <f t="shared" ref="R18:R30" si="28">B18&amp;C18&amp;D18&amp;E18&amp;F18&amp;G18&amp;H18&amp;I18&amp;J18&amp;K18&amp;L18&amp;M18&amp;N18&amp;O18&amp;P18&amp;Q18</f>
+        <v>11000000011010000001010000010010</v>
+      </c>
+      <c r="S18" s="4" t="str">
+        <f t="shared" ref="S18:S30" si="29">AG18&amp;AH18&amp;AI18&amp;AJ18&amp;AK18&amp;AL18&amp;AM18&amp;AN18</f>
+        <v>C0681412</v>
+      </c>
       <c r="V18" s="5"/>
       <c r="X18" t="str">
         <f t="shared" si="12"/>
-        <v/>
+        <v>1100</v>
       </c>
       <c r="Y18" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="Z18" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>0110</v>
       </c>
       <c r="AA18" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>1000</v>
       </c>
       <c r="AB18" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>0001</v>
       </c>
       <c r="AC18" t="str">
         <f t="shared" si="17"/>
-        <v/>
+        <v>0100</v>
       </c>
       <c r="AD18" t="str">
         <f t="shared" si="18"/>
-        <v/>
+        <v>0001</v>
       </c>
       <c r="AE18" t="str">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="AG18" t="e">
+        <v>0010</v>
+      </c>
+      <c r="AG18" t="str">
         <f t="shared" si="20"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AH18" t="e">
+        <v>C</v>
+      </c>
+      <c r="AH18" t="str">
         <f t="shared" si="21"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AI18" t="e">
+        <v>0</v>
+      </c>
+      <c r="AI18" t="str">
         <f t="shared" si="22"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AJ18" t="e">
+        <v>6</v>
+      </c>
+      <c r="AJ18" t="str">
         <f t="shared" si="23"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AK18" t="e">
+        <v>8</v>
+      </c>
+      <c r="AK18" t="str">
         <f t="shared" si="24"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AL18" t="e">
+        <v>1</v>
+      </c>
+      <c r="AL18" t="str">
         <f t="shared" si="25"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AM18" t="e">
+        <v>4</v>
+      </c>
+      <c r="AM18" t="str">
         <f t="shared" si="26"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AN18" t="e">
+        <v>1</v>
+      </c>
+      <c r="AN18" t="str">
         <f t="shared" si="27"/>
-        <v>#N/A</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="R19" s="1"/>
+      <c r="A19" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B19" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="J19" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="K19" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="L19" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="M19" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="N19" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="O19" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="P19" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q19" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="R19" s="3" t="str">
+        <f t="shared" si="28"/>
+        <v>00110001011001010011001000010010</v>
+      </c>
+      <c r="S19" s="4" t="str">
+        <f t="shared" si="29"/>
+        <v>31653212</v>
+      </c>
       <c r="X19" t="str">
         <f t="shared" si="12"/>
-        <v/>
+        <v>0011</v>
       </c>
       <c r="Y19" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>0001</v>
       </c>
       <c r="Z19" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>0110</v>
       </c>
       <c r="AA19" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>0101</v>
       </c>
       <c r="AB19" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>0011</v>
       </c>
       <c r="AC19" t="str">
         <f t="shared" si="17"/>
-        <v/>
+        <v>0010</v>
       </c>
       <c r="AD19" t="str">
         <f t="shared" si="18"/>
-        <v/>
+        <v>0001</v>
       </c>
       <c r="AE19" t="str">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="AG19" t="e">
+        <v>0010</v>
+      </c>
+      <c r="AG19" t="str">
         <f t="shared" si="20"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AH19" t="e">
+        <v>3</v>
+      </c>
+      <c r="AH19" t="str">
         <f t="shared" si="21"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AI19" t="e">
+        <v>1</v>
+      </c>
+      <c r="AI19" t="str">
         <f t="shared" si="22"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AJ19" t="e">
+        <v>6</v>
+      </c>
+      <c r="AJ19" t="str">
         <f t="shared" si="23"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AK19" t="e">
+        <v>5</v>
+      </c>
+      <c r="AK19" t="str">
         <f t="shared" si="24"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AL19" t="e">
+        <v>3</v>
+      </c>
+      <c r="AL19" t="str">
         <f t="shared" si="25"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AM19" t="e">
+        <v>2</v>
+      </c>
+      <c r="AM19" t="str">
         <f t="shared" si="26"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AN19" t="e">
+        <v>1</v>
+      </c>
+      <c r="AN19" t="str">
         <f t="shared" si="27"/>
-        <v>#N/A</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="G20" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="K20" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="L20" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="M20" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="N20" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="O20" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="P20" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q20" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="R20" s="3" t="str">
+        <f t="shared" si="28"/>
+        <v>11000000011010000001010000011010</v>
+      </c>
+      <c r="S20" s="4" t="str">
+        <f t="shared" si="29"/>
+        <v>C068141A</v>
+      </c>
       <c r="X20" t="str">
         <f t="shared" si="12"/>
-        <v/>
+        <v>1100</v>
       </c>
       <c r="Y20" t="str">
         <f t="shared" si="13"/>
-        <v/>
+        <v>0000</v>
       </c>
       <c r="Z20" t="str">
         <f t="shared" si="14"/>
-        <v/>
+        <v>0110</v>
       </c>
       <c r="AA20" t="str">
         <f t="shared" si="15"/>
-        <v/>
+        <v>1000</v>
       </c>
       <c r="AB20" t="str">
         <f t="shared" si="16"/>
-        <v/>
+        <v>0001</v>
       </c>
       <c r="AC20" t="str">
         <f t="shared" si="17"/>
-        <v/>
+        <v>0100</v>
       </c>
       <c r="AD20" t="str">
         <f t="shared" si="18"/>
-        <v/>
+        <v>0001</v>
       </c>
       <c r="AE20" t="str">
         <f t="shared" si="19"/>
-        <v/>
-      </c>
-      <c r="AG20" t="e">
+        <v>1010</v>
+      </c>
+      <c r="AG20" t="str">
         <f t="shared" si="20"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AH20" t="e">
+        <v>C</v>
+      </c>
+      <c r="AH20" t="str">
         <f t="shared" si="21"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AI20" t="e">
+        <v>0</v>
+      </c>
+      <c r="AI20" t="str">
         <f t="shared" si="22"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AJ20" t="e">
+        <v>6</v>
+      </c>
+      <c r="AJ20" t="str">
         <f t="shared" si="23"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AK20" t="e">
+        <v>8</v>
+      </c>
+      <c r="AK20" t="str">
         <f t="shared" si="24"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AL20" t="e">
+        <v>1</v>
+      </c>
+      <c r="AL20" t="str">
         <f t="shared" si="25"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AM20" t="e">
+        <v>4</v>
+      </c>
+      <c r="AM20" t="str">
         <f t="shared" si="26"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AN20" t="e">
+        <v>1</v>
+      </c>
+      <c r="AN20" t="str">
         <f t="shared" si="27"/>
-        <v>#N/A</v>
+        <v>A</v>
       </c>
     </row>
     <row r="21" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B21" s="18"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="3" t="str">
+        <f t="shared" si="28"/>
+        <v/>
+      </c>
+      <c r="S21" s="4" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
       <c r="X21" t="str">
         <f t="shared" si="12"/>
         <v/>
@@ -3233,21 +3475,858 @@
       </c>
       <c r="AN21" t="e">
         <f t="shared" si="27"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="19"/>
+      <c r="E22" s="19"/>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="20"/>
+      <c r="J22" s="20"/>
+      <c r="K22" s="20"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="21"/>
+      <c r="Q22" s="21"/>
+      <c r="R22" s="3" t="str">
+        <f t="shared" si="28"/>
+        <v/>
+      </c>
+      <c r="S22" s="4" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X22" t="str">
+        <f t="shared" ref="X22:X30" si="30">LEFT(RIGHT(R22,32),4)</f>
+        <v/>
+      </c>
+      <c r="Y22" t="str">
+        <f t="shared" ref="Y22:Y30" si="31">LEFT(RIGHT(R22,28),4)</f>
+        <v/>
+      </c>
+      <c r="Z22" t="str">
+        <f t="shared" ref="Z22:Z30" si="32">LEFT(RIGHT(R22,24),4)</f>
+        <v/>
+      </c>
+      <c r="AA22" t="str">
+        <f t="shared" ref="AA22:AA30" si="33">LEFT(RIGHT(R22,20),4)</f>
+        <v/>
+      </c>
+      <c r="AB22" t="str">
+        <f t="shared" ref="AB22:AB30" si="34">LEFT(RIGHT(R22,16),4)</f>
+        <v/>
+      </c>
+      <c r="AC22" t="str">
+        <f t="shared" ref="AC22:AC30" si="35">LEFT(RIGHT(R22,12),4)</f>
+        <v/>
+      </c>
+      <c r="AD22" t="str">
+        <f t="shared" ref="AD22:AD30" si="36">LEFT(RIGHT(R22,8),4)</f>
+        <v/>
+      </c>
+      <c r="AE22" t="str">
+        <f t="shared" ref="AE22:AE30" si="37">LEFT(RIGHT(R22,4),4)</f>
+        <v/>
+      </c>
+      <c r="AG22" t="e">
+        <f t="shared" ref="AG22:AG30" si="38">INDEX(AQ:AQ,MATCH(X22,AP:AP,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AH22" t="e">
+        <f t="shared" ref="AH22:AH30" si="39">INDEX(AQ:AQ,MATCH(Y22,AP:AP,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AI22" t="e">
+        <f t="shared" ref="AI22:AI30" si="40">INDEX(AQ:AQ,MATCH(Z22,AP:AP,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AJ22" t="e">
+        <f t="shared" ref="AJ22:AJ30" si="41">INDEX(AQ:AQ,MATCH(AA22,AP:AP,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AK22" t="e">
+        <f t="shared" ref="AK22:AK30" si="42">INDEX(AQ:AQ,MATCH(AB22,AP:AP,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AL22" t="e">
+        <f t="shared" ref="AL22:AL30" si="43">INDEX(AQ:AQ,MATCH(AC22,AP:AP,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AM22" t="e">
+        <f t="shared" ref="AM22:AM30" si="44">INDEX(AQ:AQ,MATCH(AD22,AP:AP,0))</f>
+        <v>#N/A</v>
+      </c>
+      <c r="AN22" t="e">
+        <f t="shared" ref="AN22:AN30" si="45">INDEX(AQ:AQ,MATCH(AE22,AP:AP,0))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B23" s="18"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="20"/>
+      <c r="J23" s="20"/>
+      <c r="K23" s="20"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="21"/>
+      <c r="P23" s="21"/>
+      <c r="Q23" s="21"/>
+      <c r="R23" s="3" t="str">
+        <f t="shared" si="28"/>
+        <v/>
+      </c>
+      <c r="S23" s="4" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X23" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
+      <c r="Y23" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="Z23" t="str">
+        <f t="shared" si="32"/>
+        <v/>
+      </c>
+      <c r="AA23" t="str">
+        <f t="shared" si="33"/>
+        <v/>
+      </c>
+      <c r="AB23" t="str">
+        <f t="shared" si="34"/>
+        <v/>
+      </c>
+      <c r="AC23" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="AD23" t="str">
+        <f t="shared" si="36"/>
+        <v/>
+      </c>
+      <c r="AE23" t="str">
+        <f t="shared" si="37"/>
+        <v/>
+      </c>
+      <c r="AG23" t="e">
+        <f t="shared" si="38"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AH23" t="e">
+        <f t="shared" si="39"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AI23" t="e">
+        <f t="shared" si="40"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AJ23" t="e">
+        <f t="shared" si="41"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AK23" t="e">
+        <f t="shared" si="42"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AL23" t="e">
+        <f t="shared" si="43"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AM23" t="e">
+        <f t="shared" si="44"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AN23" t="e">
+        <f t="shared" si="45"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B24" s="18"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="20"/>
+      <c r="I24" s="20"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="21"/>
+      <c r="Q24" s="21"/>
+      <c r="R24" s="3" t="str">
+        <f t="shared" si="28"/>
+        <v/>
+      </c>
+      <c r="S24" s="4" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X24" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
+      <c r="Y24" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="Z24" t="str">
+        <f t="shared" si="32"/>
+        <v/>
+      </c>
+      <c r="AA24" t="str">
+        <f t="shared" si="33"/>
+        <v/>
+      </c>
+      <c r="AB24" t="str">
+        <f t="shared" si="34"/>
+        <v/>
+      </c>
+      <c r="AC24" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="AD24" t="str">
+        <f t="shared" si="36"/>
+        <v/>
+      </c>
+      <c r="AE24" t="str">
+        <f t="shared" si="37"/>
+        <v/>
+      </c>
+      <c r="AG24" t="e">
+        <f t="shared" si="38"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AH24" t="e">
+        <f t="shared" si="39"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AI24" t="e">
+        <f t="shared" si="40"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AJ24" t="e">
+        <f t="shared" si="41"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AK24" t="e">
+        <f t="shared" si="42"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AL24" t="e">
+        <f t="shared" si="43"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AM24" t="e">
+        <f t="shared" si="44"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AN24" t="e">
+        <f t="shared" si="45"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A25" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B25" s="18"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="3" t="str">
+        <f t="shared" si="28"/>
+        <v/>
+      </c>
+      <c r="S25" s="4" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X25" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
+      <c r="Y25" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="Z25" t="str">
+        <f t="shared" si="32"/>
+        <v/>
+      </c>
+      <c r="AA25" t="str">
+        <f t="shared" si="33"/>
+        <v/>
+      </c>
+      <c r="AB25" t="str">
+        <f t="shared" si="34"/>
+        <v/>
+      </c>
+      <c r="AC25" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="AD25" t="str">
+        <f t="shared" si="36"/>
+        <v/>
+      </c>
+      <c r="AE25" t="str">
+        <f t="shared" si="37"/>
+        <v/>
+      </c>
+      <c r="AG25" t="e">
+        <f t="shared" si="38"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AH25" t="e">
+        <f t="shared" si="39"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AI25" t="e">
+        <f t="shared" si="40"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AJ25" t="e">
+        <f t="shared" si="41"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AK25" t="e">
+        <f t="shared" si="42"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AL25" t="e">
+        <f t="shared" si="43"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AM25" t="e">
+        <f t="shared" si="44"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AN25" t="e">
+        <f t="shared" si="45"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="26" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B26" s="18"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="20"/>
+      <c r="I26" s="20"/>
+      <c r="J26" s="20"/>
+      <c r="K26" s="20"/>
+      <c r="L26" s="20"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="21"/>
+      <c r="R26" s="3" t="str">
+        <f t="shared" si="28"/>
+        <v/>
+      </c>
+      <c r="S26" s="4" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X26" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
+      <c r="Y26" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="Z26" t="str">
+        <f t="shared" si="32"/>
+        <v/>
+      </c>
+      <c r="AA26" t="str">
+        <f t="shared" si="33"/>
+        <v/>
+      </c>
+      <c r="AB26" t="str">
+        <f t="shared" si="34"/>
+        <v/>
+      </c>
+      <c r="AC26" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="AD26" t="str">
+        <f t="shared" si="36"/>
+        <v/>
+      </c>
+      <c r="AE26" t="str">
+        <f t="shared" si="37"/>
+        <v/>
+      </c>
+      <c r="AG26" t="e">
+        <f t="shared" si="38"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AH26" t="e">
+        <f t="shared" si="39"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AI26" t="e">
+        <f t="shared" si="40"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AJ26" t="e">
+        <f t="shared" si="41"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AK26" t="e">
+        <f t="shared" si="42"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AL26" t="e">
+        <f t="shared" si="43"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AM26" t="e">
+        <f t="shared" si="44"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AN26" t="e">
+        <f t="shared" si="45"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A27" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B27" s="18"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="20"/>
+      <c r="I27" s="20"/>
+      <c r="J27" s="20"/>
+      <c r="K27" s="20"/>
+      <c r="L27" s="20"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="21"/>
+      <c r="R27" s="3" t="str">
+        <f t="shared" si="28"/>
+        <v/>
+      </c>
+      <c r="S27" s="4" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X27" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
+      <c r="Y27" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="Z27" t="str">
+        <f t="shared" si="32"/>
+        <v/>
+      </c>
+      <c r="AA27" t="str">
+        <f t="shared" si="33"/>
+        <v/>
+      </c>
+      <c r="AB27" t="str">
+        <f t="shared" si="34"/>
+        <v/>
+      </c>
+      <c r="AC27" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="AD27" t="str">
+        <f t="shared" si="36"/>
+        <v/>
+      </c>
+      <c r="AE27" t="str">
+        <f t="shared" si="37"/>
+        <v/>
+      </c>
+      <c r="AG27" t="e">
+        <f t="shared" si="38"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AH27" t="e">
+        <f t="shared" si="39"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AI27" t="e">
+        <f t="shared" si="40"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AJ27" t="e">
+        <f t="shared" si="41"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AK27" t="e">
+        <f t="shared" si="42"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AL27" t="e">
+        <f t="shared" si="43"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AM27" t="e">
+        <f t="shared" si="44"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AN27" t="e">
+        <f t="shared" si="45"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A28" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="B28" s="18"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="21"/>
+      <c r="Q28" s="21"/>
+      <c r="R28" s="3" t="str">
+        <f t="shared" si="28"/>
+        <v/>
+      </c>
+      <c r="S28" s="4" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X28" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
+      <c r="Y28" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="Z28" t="str">
+        <f t="shared" si="32"/>
+        <v/>
+      </c>
+      <c r="AA28" t="str">
+        <f t="shared" si="33"/>
+        <v/>
+      </c>
+      <c r="AB28" t="str">
+        <f t="shared" si="34"/>
+        <v/>
+      </c>
+      <c r="AC28" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="AD28" t="str">
+        <f t="shared" si="36"/>
+        <v/>
+      </c>
+      <c r="AE28" t="str">
+        <f t="shared" si="37"/>
+        <v/>
+      </c>
+      <c r="AG28" t="e">
+        <f t="shared" si="38"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AH28" t="e">
+        <f t="shared" si="39"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AI28" t="e">
+        <f t="shared" si="40"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AJ28" t="e">
+        <f t="shared" si="41"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AK28" t="e">
+        <f t="shared" si="42"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AL28" t="e">
+        <f t="shared" si="43"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AM28" t="e">
+        <f t="shared" si="44"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AN28" t="e">
+        <f t="shared" si="45"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A29" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B29" s="18"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="19"/>
+      <c r="F29" s="19"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="20"/>
+      <c r="I29" s="20"/>
+      <c r="J29" s="20"/>
+      <c r="K29" s="20"/>
+      <c r="L29" s="20"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="21"/>
+      <c r="R29" s="3" t="str">
+        <f t="shared" si="28"/>
+        <v/>
+      </c>
+      <c r="S29" s="4" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X29" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
+      <c r="Y29" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="Z29" t="str">
+        <f t="shared" si="32"/>
+        <v/>
+      </c>
+      <c r="AA29" t="str">
+        <f t="shared" si="33"/>
+        <v/>
+      </c>
+      <c r="AB29" t="str">
+        <f t="shared" si="34"/>
+        <v/>
+      </c>
+      <c r="AC29" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="AD29" t="str">
+        <f t="shared" si="36"/>
+        <v/>
+      </c>
+      <c r="AE29" t="str">
+        <f t="shared" si="37"/>
+        <v/>
+      </c>
+      <c r="AG29" t="e">
+        <f t="shared" si="38"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AH29" t="e">
+        <f t="shared" si="39"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AI29" t="e">
+        <f t="shared" si="40"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AJ29" t="e">
+        <f t="shared" si="41"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AK29" t="e">
+        <f t="shared" si="42"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AL29" t="e">
+        <f t="shared" si="43"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AM29" t="e">
+        <f t="shared" si="44"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AN29" t="e">
+        <f t="shared" si="45"/>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
+      <c r="A30" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B30" s="18"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="20"/>
+      <c r="I30" s="20"/>
+      <c r="J30" s="20"/>
+      <c r="K30" s="20"/>
+      <c r="L30" s="20"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="21"/>
+      <c r="Q30" s="21"/>
+      <c r="R30" s="3" t="str">
+        <f t="shared" si="28"/>
+        <v/>
+      </c>
+      <c r="S30" s="4" t="e">
+        <f t="shared" si="29"/>
+        <v>#N/A</v>
+      </c>
+      <c r="X30" t="str">
+        <f t="shared" si="30"/>
+        <v/>
+      </c>
+      <c r="Y30" t="str">
+        <f t="shared" si="31"/>
+        <v/>
+      </c>
+      <c r="Z30" t="str">
+        <f t="shared" si="32"/>
+        <v/>
+      </c>
+      <c r="AA30" t="str">
+        <f t="shared" si="33"/>
+        <v/>
+      </c>
+      <c r="AB30" t="str">
+        <f t="shared" si="34"/>
+        <v/>
+      </c>
+      <c r="AC30" t="str">
+        <f t="shared" si="35"/>
+        <v/>
+      </c>
+      <c r="AD30" t="str">
+        <f t="shared" si="36"/>
+        <v/>
+      </c>
+      <c r="AE30" t="str">
+        <f t="shared" si="37"/>
+        <v/>
+      </c>
+      <c r="AG30" t="e">
+        <f t="shared" si="38"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AH30" t="e">
+        <f t="shared" si="39"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AI30" t="e">
+        <f t="shared" si="40"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AJ30" t="e">
+        <f t="shared" si="41"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AK30" t="e">
+        <f t="shared" si="42"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AL30" t="e">
+        <f t="shared" si="43"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AM30" t="e">
+        <f t="shared" si="44"/>
+        <v>#N/A</v>
+      </c>
+      <c r="AN30" t="e">
+        <f t="shared" si="45"/>
         <v>#N/A</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B17">
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B30">
       <formula1>5</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D17 M2:N17 H2:I17">
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:D30 H2:I30 M2:N30">
       <formula1>3</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:G17 O2:Q17 J2:L17">
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:G30 J2:L30 O2:Q30">
       <formula1>1</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A17">
+    <dataValidation type="textLength" operator="equal" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:A30">
       <formula1>6</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
divide finalised and working as expected
</commit_message>
<xml_diff>
--- a/Instructions/Binary Instructions.xlsx
+++ b/Instructions/Binary Instructions.xlsx
@@ -766,8 +766,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3146,13 +3146,13 @@
         <v>20</v>
       </c>
       <c r="D19" s="19" t="s">
-        <v>87</v>
+        <v>20</v>
       </c>
       <c r="E19" s="19" t="s">
         <v>30</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G19" s="19" t="s">
         <v>30</v>
@@ -3189,11 +3189,11 @@
       </c>
       <c r="R19" s="3" t="str">
         <f t="shared" si="36"/>
-        <v>11000000011010000001010000011010</v>
+        <v>11000000000000000001010000011010</v>
       </c>
       <c r="S19" s="4" t="str">
         <f t="shared" si="37"/>
-        <v>C068141A</v>
+        <v>C000141A</v>
       </c>
       <c r="X19" t="str">
         <f t="shared" si="20"/>
@@ -3205,11 +3205,11 @@
       </c>
       <c r="Z19" t="str">
         <f t="shared" si="22"/>
-        <v>0110</v>
+        <v>0000</v>
       </c>
       <c r="AA19" t="str">
         <f t="shared" si="23"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="AB19" t="str">
         <f t="shared" si="24"/>
@@ -3237,11 +3237,11 @@
       </c>
       <c r="AI19" t="str">
         <f t="shared" si="30"/>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AJ19" t="str">
         <f t="shared" si="31"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AK19" t="str">
         <f t="shared" si="32"/>

</xml_diff>

<commit_message>
added alt program counter
</commit_message>
<xml_diff>
--- a/Instructions/Binary Instructions.xlsx
+++ b/Instructions/Binary Instructions.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="161">
   <si>
     <t>0001</t>
   </si>
@@ -946,7 +946,7 @@
   <dimension ref="A1:AN33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="I2" sqref="I2:I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1385,129 +1385,129 @@
         <v>34</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>107</v>
+        <v>9</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>32</v>
+        <v>158</v>
       </c>
       <c r="D5" s="28" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F5" s="30" t="s">
+        <v>113</v>
+      </c>
+      <c r="G5" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="H5" s="41" t="s">
         <v>114</v>
-      </c>
-      <c r="G5" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="H5" s="41" t="s">
-        <v>113</v>
       </c>
       <c r="I5" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>60442424</v>
+        <v>4800381A</v>
       </c>
       <c r="L5" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B5,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01100</v>
+        <v>01001</v>
       </c>
       <c r="M5" t="str">
         <f>IF(ISNUMBER(MATCH(C5,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C5,'HEX GEN BACKEND'!G:G,0)),C5)</f>
-        <v>000010</v>
+        <v>000000</v>
       </c>
       <c r="N5" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D5,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>001</v>
+        <v>000</v>
       </c>
       <c r="O5" t="str">
         <f>IF(ISNUMBER(MATCH(E5,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E5,'HEX GEN BACKEND'!H:H,0)),E5)</f>
-        <v>000010</v>
+        <v>000011</v>
       </c>
       <c r="P5" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F5,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
+        <v>100</v>
       </c>
       <c r="Q5" t="str">
         <f>IF(ISNUMBER(MATCH(G5,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G5,'HEX GEN BACKEND'!I:I,0)),G5)</f>
-        <v>000100</v>
+        <v>000011</v>
       </c>
       <c r="R5" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H5,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
+        <v>010</v>
       </c>
       <c r="T5" t="str">
         <f t="shared" si="1"/>
-        <v>01100000010001000010010000100100</v>
+        <v>01001000000000000011100000011010</v>
       </c>
       <c r="V5" t="str">
         <f t="shared" si="2"/>
-        <v>0110</v>
+        <v>0100</v>
       </c>
       <c r="W5" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="X5" t="str">
         <f t="shared" si="4"/>
-        <v>0100</v>
+        <v>0000</v>
       </c>
       <c r="Y5" t="str">
         <f t="shared" si="5"/>
-        <v>0100</v>
+        <v>0000</v>
       </c>
       <c r="Z5" t="str">
         <f t="shared" si="6"/>
-        <v>0010</v>
+        <v>0011</v>
       </c>
       <c r="AA5" t="str">
         <f t="shared" si="7"/>
-        <v>0100</v>
+        <v>1000</v>
       </c>
       <c r="AB5" t="str">
         <f t="shared" si="8"/>
-        <v>0010</v>
+        <v>0001</v>
       </c>
       <c r="AC5" t="str">
         <f t="shared" si="9"/>
-        <v>0100</v>
+        <v>1010</v>
       </c>
       <c r="AE5" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V5,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AF5" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W5,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AG5" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X5,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AH5" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y5,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AI5" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z5,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AJ5" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA5,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AK5" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB5,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL5" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC5,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>A</v>
       </c>
       <c r="AN5" t="str">
         <f t="shared" si="10"/>
-        <v>60442424</v>
+        <v>4800381A</v>
       </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.25">
@@ -1515,37 +1515,37 @@
         <v>33</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D6" s="28" t="s">
         <v>115</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F6" s="30" t="s">
         <v>114</v>
       </c>
       <c r="G6" s="32" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H6" s="41" t="s">
         <v>113</v>
       </c>
       <c r="I6" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>6084242C</v>
+        <v>2824341C</v>
       </c>
       <c r="L6" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B6,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01100</v>
+        <v>00101</v>
       </c>
       <c r="M6" t="str">
         <f>IF(ISNUMBER(MATCH(C6,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C6,'HEX GEN BACKEND'!G:G,0)),C6)</f>
-        <v>000100</v>
+        <v>000001</v>
       </c>
       <c r="N6" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D6,'HEX GEN BACKEND'!D:D,0))</f>
@@ -1553,7 +1553,7 @@
       </c>
       <c r="O6" t="str">
         <f>IF(ISNUMBER(MATCH(E6,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E6,'HEX GEN BACKEND'!H:H,0)),E6)</f>
-        <v>000010</v>
+        <v>000011</v>
       </c>
       <c r="P6" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F6,'HEX GEN BACKEND'!D:D,0))</f>
@@ -1561,7 +1561,7 @@
       </c>
       <c r="Q6" t="str">
         <f>IF(ISNUMBER(MATCH(G6,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G6,'HEX GEN BACKEND'!I:I,0)),G6)</f>
-        <v>000101</v>
+        <v>000011</v>
       </c>
       <c r="R6" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H6,'HEX GEN BACKEND'!D:D,0))</f>
@@ -1569,19 +1569,19 @@
       </c>
       <c r="T6" t="str">
         <f t="shared" si="1"/>
-        <v>01100000100001000010010000101100</v>
+        <v>00101000001001000011010000011100</v>
       </c>
       <c r="V6" t="str">
         <f t="shared" si="2"/>
-        <v>0110</v>
+        <v>0010</v>
       </c>
       <c r="W6" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="X6" t="str">
         <f t="shared" si="4"/>
-        <v>1000</v>
+        <v>0010</v>
       </c>
       <c r="Y6" t="str">
         <f t="shared" si="5"/>
@@ -1589,7 +1589,7 @@
       </c>
       <c r="Z6" t="str">
         <f t="shared" si="6"/>
-        <v>0010</v>
+        <v>0011</v>
       </c>
       <c r="AA6" t="str">
         <f t="shared" si="7"/>
@@ -1597,7 +1597,7 @@
       </c>
       <c r="AB6" t="str">
         <f t="shared" si="8"/>
-        <v>0010</v>
+        <v>0001</v>
       </c>
       <c r="AC6" t="str">
         <f t="shared" si="9"/>
@@ -1605,15 +1605,15 @@
       </c>
       <c r="AE6" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V6,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AF6" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W6,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AG6" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X6,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AH6" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y6,'HEX GEN BACKEND'!L:L,0))</f>
@@ -1621,7 +1621,7 @@
       </c>
       <c r="AI6" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z6,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AJ6" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA6,'HEX GEN BACKEND'!L:L,0))</f>
@@ -1629,7 +1629,7 @@
       </c>
       <c r="AK6" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB6,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL6" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC6,'HEX GEN BACKEND'!L:L,0))</f>
@@ -1637,7 +1637,7 @@
       </c>
       <c r="AN6" t="str">
         <f t="shared" si="10"/>
-        <v>6084242C</v>
+        <v>2824341C</v>
       </c>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.25">
@@ -1645,37 +1645,37 @@
         <v>35</v>
       </c>
       <c r="B7" s="25" t="s">
-        <v>107</v>
+        <v>7</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D7" s="28" t="s">
         <v>115</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>137</v>
+        <v>36</v>
       </c>
       <c r="F7" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="G7" s="32" t="s">
+        <v>145</v>
+      </c>
+      <c r="H7" s="41" t="s">
         <v>114</v>
-      </c>
-      <c r="G7" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="H7" s="41" t="s">
-        <v>113</v>
       </c>
       <c r="I7" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>61042434</v>
+        <v>30E4621A</v>
       </c>
       <c r="L7" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B7,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01100</v>
+        <v>00110</v>
       </c>
       <c r="M7" t="str">
         <f>IF(ISNUMBER(MATCH(C7,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C7,'HEX GEN BACKEND'!G:G,0)),C7)</f>
-        <v>001000</v>
+        <v>000111</v>
       </c>
       <c r="N7" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D7,'HEX GEN BACKEND'!D:D,0))</f>
@@ -1683,35 +1683,35 @@
       </c>
       <c r="O7" t="str">
         <f>IF(ISNUMBER(MATCH(E7,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E7,'HEX GEN BACKEND'!H:H,0)),E7)</f>
-        <v>000010</v>
+        <v>000110</v>
       </c>
       <c r="P7" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F7,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
+        <v>001</v>
       </c>
       <c r="Q7" t="str">
         <f>IF(ISNUMBER(MATCH(G7,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G7,'HEX GEN BACKEND'!I:I,0)),G7)</f>
-        <v>000110</v>
+        <v>000011</v>
       </c>
       <c r="R7" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H7,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
+        <v>010</v>
       </c>
       <c r="T7" t="str">
         <f t="shared" si="1"/>
-        <v>01100001000001000010010000110100</v>
+        <v>00110000111001000110001000011010</v>
       </c>
       <c r="V7" t="str">
         <f t="shared" si="2"/>
-        <v>0110</v>
+        <v>0011</v>
       </c>
       <c r="W7" t="str">
         <f t="shared" si="3"/>
-        <v>0001</v>
+        <v>0000</v>
       </c>
       <c r="X7" t="str">
         <f t="shared" si="4"/>
-        <v>0000</v>
+        <v>1110</v>
       </c>
       <c r="Y7" t="str">
         <f t="shared" si="5"/>
@@ -1719,31 +1719,31 @@
       </c>
       <c r="Z7" t="str">
         <f t="shared" si="6"/>
-        <v>0010</v>
+        <v>0110</v>
       </c>
       <c r="AA7" t="str">
         <f t="shared" si="7"/>
-        <v>0100</v>
+        <v>0010</v>
       </c>
       <c r="AB7" t="str">
         <f t="shared" si="8"/>
-        <v>0011</v>
+        <v>0001</v>
       </c>
       <c r="AC7" t="str">
         <f t="shared" si="9"/>
-        <v>0100</v>
+        <v>1010</v>
       </c>
       <c r="AE7" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V7,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AF7" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W7,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG7" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X7,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>E</v>
       </c>
       <c r="AH7" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y7,'HEX GEN BACKEND'!L:L,0))</f>
@@ -1751,23 +1751,23 @@
       </c>
       <c r="AI7" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z7,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="AJ7" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA7,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AK7" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB7,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AL7" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC7,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>A</v>
       </c>
       <c r="AN7" t="str">
         <f t="shared" si="10"/>
-        <v>61042434</v>
+        <v>30E4621A</v>
       </c>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.25">
@@ -1775,65 +1775,65 @@
         <v>36</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C8" s="42" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="D8" s="28" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="F8" s="30" t="s">
+        <v>115</v>
+      </c>
+      <c r="G8" s="32" t="s">
+        <v>149</v>
+      </c>
+      <c r="H8" s="41" t="s">
         <v>113</v>
-      </c>
-      <c r="G8" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="H8" s="41" t="s">
-        <v>114</v>
       </c>
       <c r="I8" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>4800381A</v>
+        <v>0848023C</v>
       </c>
       <c r="L8" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B8,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01001</v>
+        <v>00001</v>
       </c>
       <c r="M8" t="str">
         <f>IF(ISNUMBER(MATCH(C8,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C8,'HEX GEN BACKEND'!G:G,0)),C8)</f>
-        <v>000000</v>
+        <v>000010</v>
       </c>
       <c r="N8" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D8,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
+        <v>010</v>
       </c>
       <c r="O8" t="str">
         <f>IF(ISNUMBER(MATCH(E8,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E8,'HEX GEN BACKEND'!H:H,0)),E8)</f>
-        <v>000011</v>
+        <v>000000</v>
       </c>
       <c r="P8" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F8,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
+        <v>001</v>
       </c>
       <c r="Q8" t="str">
         <f>IF(ISNUMBER(MATCH(G8,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G8,'HEX GEN BACKEND'!I:I,0)),G8)</f>
-        <v>000011</v>
+        <v>000111</v>
       </c>
       <c r="R8" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H8,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
+        <v>100</v>
       </c>
       <c r="T8" t="str">
         <f t="shared" si="1"/>
-        <v>01001000000000000011100000011010</v>
+        <v>00001000010010000000001000111100</v>
       </c>
       <c r="V8" t="str">
         <f t="shared" si="2"/>
-        <v>0100</v>
+        <v>0000</v>
       </c>
       <c r="W8" t="str">
         <f t="shared" si="3"/>
@@ -1841,31 +1841,31 @@
       </c>
       <c r="X8" t="str">
         <f t="shared" si="4"/>
-        <v>0000</v>
+        <v>0100</v>
       </c>
       <c r="Y8" t="str">
         <f t="shared" si="5"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="Z8" t="str">
         <f t="shared" si="6"/>
-        <v>0011</v>
+        <v>0000</v>
       </c>
       <c r="AA8" t="str">
         <f t="shared" si="7"/>
-        <v>1000</v>
+        <v>0010</v>
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="8"/>
-        <v>0001</v>
+        <v>0011</v>
       </c>
       <c r="AC8" t="str">
         <f t="shared" si="9"/>
-        <v>1010</v>
+        <v>1100</v>
       </c>
       <c r="AE8" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V8,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AF8" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W8,'HEX GEN BACKEND'!L:L,0))</f>
@@ -1873,31 +1873,31 @@
       </c>
       <c r="AG8" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X8,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AH8" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y8,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AI8" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z8,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AJ8" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA8,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AK8" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB8,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AL8" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC8,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>A</v>
+        <v>C</v>
       </c>
       <c r="AN8" t="str">
         <f t="shared" si="10"/>
-        <v>4800381A</v>
+        <v>0848023C</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.25">
@@ -1905,7 +1905,7 @@
         <v>37</v>
       </c>
       <c r="B9" s="25" t="s">
-        <v>9</v>
+        <v>156</v>
       </c>
       <c r="C9" s="42" t="s">
         <v>158</v>
@@ -1914,24 +1914,24 @@
         <v>117</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="F9" s="30" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="G9" s="32" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="H9" s="41" t="s">
         <v>114</v>
       </c>
       <c r="I9" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>48004822</v>
+        <v>C000003A</v>
       </c>
       <c r="L9" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B9,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01001</v>
+        <v>11000</v>
       </c>
       <c r="M9" t="str">
         <f>IF(ISNUMBER(MATCH(C9,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C9,'HEX GEN BACKEND'!G:G,0)),C9)</f>
@@ -1943,15 +1943,15 @@
       </c>
       <c r="O9" t="str">
         <f>IF(ISNUMBER(MATCH(E9,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E9,'HEX GEN BACKEND'!H:H,0)),E9)</f>
-        <v>000100</v>
+        <v>000000</v>
       </c>
       <c r="P9" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F9,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
+        <v>000</v>
       </c>
       <c r="Q9" t="str">
         <f>IF(ISNUMBER(MATCH(G9,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G9,'HEX GEN BACKEND'!I:I,0)),G9)</f>
-        <v>000100</v>
+        <v>000111</v>
       </c>
       <c r="R9" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H9,'HEX GEN BACKEND'!D:D,0))</f>
@@ -1959,15 +1959,15 @@
       </c>
       <c r="T9" t="str">
         <f t="shared" si="1"/>
-        <v>01001000000000000100100000100010</v>
+        <v>11000000000000000000000000111010</v>
       </c>
       <c r="V9" t="str">
         <f t="shared" si="2"/>
-        <v>0100</v>
+        <v>1100</v>
       </c>
       <c r="W9" t="str">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="X9" t="str">
         <f t="shared" si="4"/>
@@ -1979,27 +1979,27 @@
       </c>
       <c r="Z9" t="str">
         <f t="shared" si="6"/>
-        <v>0100</v>
+        <v>0000</v>
       </c>
       <c r="AA9" t="str">
         <f t="shared" si="7"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="AB9" t="str">
         <f t="shared" si="8"/>
-        <v>0010</v>
+        <v>0011</v>
       </c>
       <c r="AC9" t="str">
         <f t="shared" si="9"/>
-        <v>0010</v>
+        <v>1010</v>
       </c>
       <c r="AE9" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V9,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>C</v>
       </c>
       <c r="AF9" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W9,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AG9" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X9,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2011,2363 +2011,2111 @@
       </c>
       <c r="AI9" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z9,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AJ9" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA9,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AK9" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB9,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL9" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC9,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>A</v>
       </c>
       <c r="AN9" t="str">
         <f t="shared" si="10"/>
-        <v>48004822</v>
+        <v>C000003A</v>
       </c>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="42" t="s">
-        <v>158</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="F10" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="G10" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="H10" s="41" t="s">
-        <v>114</v>
-      </c>
-      <c r="I10" s="25" t="str">
+      <c r="B10" s="25"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="25" t="e">
         <f t="shared" si="0"/>
-        <v>4800582A</v>
-      </c>
-      <c r="L10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L10" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B10,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01001</v>
-      </c>
-      <c r="M10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M10">
         <f>IF(ISNUMBER(MATCH(C10,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C10,'HEX GEN BACKEND'!G:G,0)),C10)</f>
-        <v>000000</v>
-      </c>
-      <c r="N10" t="str">
+        <v>0</v>
+      </c>
+      <c r="N10" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D10,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
-      </c>
-      <c r="O10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O10">
         <f>IF(ISNUMBER(MATCH(E10,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E10,'HEX GEN BACKEND'!H:H,0)),E10)</f>
-        <v>000101</v>
-      </c>
-      <c r="P10" t="str">
+        <v>0</v>
+      </c>
+      <c r="P10" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F10,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
-      </c>
-      <c r="Q10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Q10">
         <f>IF(ISNUMBER(MATCH(G10,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G10,'HEX GEN BACKEND'!I:I,0)),G10)</f>
-        <v>000101</v>
-      </c>
-      <c r="R10" t="str">
+        <v>0</v>
+      </c>
+      <c r="R10" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H10,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="T10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="T10" t="e">
         <f t="shared" si="1"/>
-        <v>01001000000000000101100000101010</v>
-      </c>
-      <c r="V10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="V10" t="e">
         <f t="shared" si="2"/>
-        <v>0100</v>
-      </c>
-      <c r="W10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W10" t="e">
         <f t="shared" si="3"/>
-        <v>1000</v>
-      </c>
-      <c r="X10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X10" t="e">
         <f t="shared" si="4"/>
-        <v>0000</v>
-      </c>
-      <c r="Y10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y10" t="e">
         <f t="shared" si="5"/>
-        <v>0000</v>
-      </c>
-      <c r="Z10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z10" t="e">
         <f t="shared" si="6"/>
-        <v>0101</v>
-      </c>
-      <c r="AA10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA10" t="e">
         <f t="shared" si="7"/>
-        <v>1000</v>
-      </c>
-      <c r="AB10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB10" t="e">
         <f t="shared" si="8"/>
-        <v>0010</v>
-      </c>
-      <c r="AC10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC10" t="e">
         <f t="shared" si="9"/>
-        <v>1010</v>
-      </c>
-      <c r="AE10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AE10" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V10,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AF10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF10" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W10,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AG10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG10" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X10,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AH10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH10" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y10,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AI10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI10" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z10,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>5</v>
-      </c>
-      <c r="AJ10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ10" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA10,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AK10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK10" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB10,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
-      </c>
-      <c r="AL10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL10" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC10,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>A</v>
-      </c>
-      <c r="AN10" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AN10" t="e">
         <f t="shared" si="10"/>
-        <v>4800582A</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="42" t="s">
-        <v>158</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="G11" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="H11" s="41" t="s">
-        <v>114</v>
-      </c>
-      <c r="I11" s="25" t="str">
+      <c r="B11" s="25"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="25" t="e">
         <f t="shared" si="0"/>
-        <v>48006832</v>
-      </c>
-      <c r="L11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L11" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B11,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01001</v>
-      </c>
-      <c r="M11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M11">
         <f>IF(ISNUMBER(MATCH(C11,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C11,'HEX GEN BACKEND'!G:G,0)),C11)</f>
-        <v>000000</v>
-      </c>
-      <c r="N11" t="str">
+        <v>0</v>
+      </c>
+      <c r="N11" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D11,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
-      </c>
-      <c r="O11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O11">
         <f>IF(ISNUMBER(MATCH(E11,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E11,'HEX GEN BACKEND'!H:H,0)),E11)</f>
-        <v>000110</v>
-      </c>
-      <c r="P11" t="str">
+        <v>0</v>
+      </c>
+      <c r="P11" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F11,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
-      </c>
-      <c r="Q11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Q11">
         <f>IF(ISNUMBER(MATCH(G11,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G11,'HEX GEN BACKEND'!I:I,0)),G11)</f>
-        <v>000110</v>
-      </c>
-      <c r="R11" t="str">
+        <v>0</v>
+      </c>
+      <c r="R11" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H11,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="T11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="T11" t="e">
         <f t="shared" si="1"/>
-        <v>01001000000000000110100000110010</v>
-      </c>
-      <c r="V11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="V11" t="e">
         <f t="shared" si="2"/>
-        <v>0100</v>
-      </c>
-      <c r="W11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W11" t="e">
         <f t="shared" si="3"/>
-        <v>1000</v>
-      </c>
-      <c r="X11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X11" t="e">
         <f t="shared" si="4"/>
-        <v>0000</v>
-      </c>
-      <c r="Y11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y11" t="e">
         <f t="shared" si="5"/>
-        <v>0000</v>
-      </c>
-      <c r="Z11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z11" t="e">
         <f t="shared" si="6"/>
-        <v>0110</v>
-      </c>
-      <c r="AA11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA11" t="e">
         <f t="shared" si="7"/>
-        <v>1000</v>
-      </c>
-      <c r="AB11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB11" t="e">
         <f t="shared" si="8"/>
-        <v>0011</v>
-      </c>
-      <c r="AC11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC11" t="e">
         <f t="shared" si="9"/>
-        <v>0010</v>
-      </c>
-      <c r="AE11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AE11" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V11,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AF11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF11" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W11,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AG11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG11" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X11,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AH11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH11" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y11,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AI11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI11" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z11,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>6</v>
-      </c>
-      <c r="AJ11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ11" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA11,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AK11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK11" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB11,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
-      </c>
-      <c r="AL11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL11" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC11,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
-      </c>
-      <c r="AN11" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AN11" t="e">
         <f t="shared" si="10"/>
-        <v>48006832</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="C12" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="G12" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="H12" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="I12" s="25" t="str">
+      <c r="B12" s="25"/>
+      <c r="C12" s="42"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="25" t="e">
         <f t="shared" si="0"/>
-        <v>5048341C</v>
-      </c>
-      <c r="L12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L12" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B12,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01010</v>
-      </c>
-      <c r="M12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M12">
         <f>IF(ISNUMBER(MATCH(C12,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C12,'HEX GEN BACKEND'!G:G,0)),C12)</f>
-        <v>000010</v>
-      </c>
-      <c r="N12" t="str">
+        <v>0</v>
+      </c>
+      <c r="N12" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D12,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="O12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O12">
         <f>IF(ISNUMBER(MATCH(E12,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E12,'HEX GEN BACKEND'!H:H,0)),E12)</f>
-        <v>000011</v>
-      </c>
-      <c r="P12" t="str">
+        <v>0</v>
+      </c>
+      <c r="P12" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F12,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="Q12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Q12">
         <f>IF(ISNUMBER(MATCH(G12,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G12,'HEX GEN BACKEND'!I:I,0)),G12)</f>
-        <v>000011</v>
-      </c>
-      <c r="R12" t="str">
+        <v>0</v>
+      </c>
+      <c r="R12" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H12,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
-      </c>
-      <c r="T12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="T12" t="e">
         <f t="shared" si="1"/>
-        <v>01010000010010000011010000011100</v>
-      </c>
-      <c r="V12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="V12" t="e">
         <f t="shared" si="2"/>
-        <v>0101</v>
-      </c>
-      <c r="W12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W12" t="e">
         <f t="shared" si="3"/>
-        <v>0000</v>
-      </c>
-      <c r="X12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X12" t="e">
         <f t="shared" si="4"/>
-        <v>0100</v>
-      </c>
-      <c r="Y12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y12" t="e">
         <f t="shared" si="5"/>
-        <v>1000</v>
-      </c>
-      <c r="Z12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z12" t="e">
         <f t="shared" si="6"/>
-        <v>0011</v>
-      </c>
-      <c r="AA12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA12" t="e">
         <f t="shared" si="7"/>
-        <v>0100</v>
-      </c>
-      <c r="AB12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB12" t="e">
         <f t="shared" si="8"/>
-        <v>0001</v>
-      </c>
-      <c r="AC12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC12" t="e">
         <f t="shared" si="9"/>
-        <v>1100</v>
-      </c>
-      <c r="AE12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AE12" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V12,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>5</v>
-      </c>
-      <c r="AF12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF12" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W12,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AG12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG12" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X12,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AH12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH12" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y12,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AI12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI12" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z12,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
-      </c>
-      <c r="AJ12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ12" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA12,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AK12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK12" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB12,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
-      </c>
-      <c r="AL12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL12" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC12,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>C</v>
-      </c>
-      <c r="AN12" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AN12" t="e">
         <f t="shared" si="10"/>
-        <v>5048341C</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="C13" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="F13" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="G13" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="H13" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="I13" s="25" t="str">
+      <c r="B13" s="25"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="32"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="25" t="e">
         <f t="shared" si="0"/>
-        <v>50484424</v>
-      </c>
-      <c r="L13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L13" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B13,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01010</v>
-      </c>
-      <c r="M13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M13">
         <f>IF(ISNUMBER(MATCH(C13,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C13,'HEX GEN BACKEND'!G:G,0)),C13)</f>
-        <v>000010</v>
-      </c>
-      <c r="N13" t="str">
+        <v>0</v>
+      </c>
+      <c r="N13" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D13,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="O13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O13">
         <f>IF(ISNUMBER(MATCH(E13,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E13,'HEX GEN BACKEND'!H:H,0)),E13)</f>
-        <v>000100</v>
-      </c>
-      <c r="P13" t="str">
+        <v>0</v>
+      </c>
+      <c r="P13" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F13,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="Q13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Q13">
         <f>IF(ISNUMBER(MATCH(G13,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G13,'HEX GEN BACKEND'!I:I,0)),G13)</f>
-        <v>000100</v>
-      </c>
-      <c r="R13" t="str">
+        <v>0</v>
+      </c>
+      <c r="R13" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H13,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
-      </c>
-      <c r="T13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="T13" t="e">
         <f t="shared" si="1"/>
-        <v>01010000010010000100010000100100</v>
-      </c>
-      <c r="V13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="V13" t="e">
         <f t="shared" si="2"/>
-        <v>0101</v>
-      </c>
-      <c r="W13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W13" t="e">
         <f t="shared" si="3"/>
-        <v>0000</v>
-      </c>
-      <c r="X13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X13" t="e">
         <f t="shared" si="4"/>
-        <v>0100</v>
-      </c>
-      <c r="Y13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y13" t="e">
         <f t="shared" si="5"/>
-        <v>1000</v>
-      </c>
-      <c r="Z13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z13" t="e">
         <f t="shared" si="6"/>
-        <v>0100</v>
-      </c>
-      <c r="AA13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA13" t="e">
         <f t="shared" si="7"/>
-        <v>0100</v>
-      </c>
-      <c r="AB13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB13" t="e">
         <f t="shared" si="8"/>
-        <v>0010</v>
-      </c>
-      <c r="AC13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC13" t="e">
         <f t="shared" si="9"/>
-        <v>0100</v>
-      </c>
-      <c r="AE13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AE13" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V13,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>5</v>
-      </c>
-      <c r="AF13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF13" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W13,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AG13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG13" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X13,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AH13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH13" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y13,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AI13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI13" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z13,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AJ13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ13" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA13,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AK13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK13" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB13,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
-      </c>
-      <c r="AL13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL13" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC13,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AN13" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AN13" t="e">
         <f t="shared" si="10"/>
-        <v>50484424</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="C14" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="F14" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="G14" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="H14" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="I14" s="25" t="str">
+      <c r="B14" s="25"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="28"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="32"/>
+      <c r="H14" s="41"/>
+      <c r="I14" s="25" t="e">
         <f t="shared" si="0"/>
-        <v>5048542C</v>
-      </c>
-      <c r="L14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L14" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B14,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01010</v>
-      </c>
-      <c r="M14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M14">
         <f>IF(ISNUMBER(MATCH(C14,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C14,'HEX GEN BACKEND'!G:G,0)),C14)</f>
-        <v>000010</v>
-      </c>
-      <c r="N14" t="str">
+        <v>0</v>
+      </c>
+      <c r="N14" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D14,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="O14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O14">
         <f>IF(ISNUMBER(MATCH(E14,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E14,'HEX GEN BACKEND'!H:H,0)),E14)</f>
-        <v>000101</v>
-      </c>
-      <c r="P14" t="str">
+        <v>0</v>
+      </c>
+      <c r="P14" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F14,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="Q14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Q14">
         <f>IF(ISNUMBER(MATCH(G14,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G14,'HEX GEN BACKEND'!I:I,0)),G14)</f>
-        <v>000101</v>
-      </c>
-      <c r="R14" t="str">
+        <v>0</v>
+      </c>
+      <c r="R14" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H14,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
-      </c>
-      <c r="T14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="T14" t="e">
         <f t="shared" si="1"/>
-        <v>01010000010010000101010000101100</v>
-      </c>
-      <c r="V14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="V14" t="e">
         <f t="shared" si="2"/>
-        <v>0101</v>
-      </c>
-      <c r="W14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W14" t="e">
         <f t="shared" si="3"/>
-        <v>0000</v>
-      </c>
-      <c r="X14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X14" t="e">
         <f t="shared" si="4"/>
-        <v>0100</v>
-      </c>
-      <c r="Y14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y14" t="e">
         <f t="shared" si="5"/>
-        <v>1000</v>
-      </c>
-      <c r="Z14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z14" t="e">
         <f t="shared" si="6"/>
-        <v>0101</v>
-      </c>
-      <c r="AA14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA14" t="e">
         <f t="shared" si="7"/>
-        <v>0100</v>
-      </c>
-      <c r="AB14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB14" t="e">
         <f t="shared" si="8"/>
-        <v>0010</v>
-      </c>
-      <c r="AC14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC14" t="e">
         <f t="shared" si="9"/>
-        <v>1100</v>
-      </c>
-      <c r="AE14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AE14" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V14,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>5</v>
-      </c>
-      <c r="AF14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF14" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W14,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AG14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG14" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X14,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AH14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH14" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y14,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AI14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI14" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z14,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>5</v>
-      </c>
-      <c r="AJ14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ14" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA14,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AK14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK14" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB14,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
-      </c>
-      <c r="AL14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL14" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC14,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>C</v>
-      </c>
-      <c r="AN14" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AN14" t="e">
         <f t="shared" si="10"/>
-        <v>5048542C</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="C15" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="D15" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="F15" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="G15" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="H15" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="I15" s="25" t="str">
+      <c r="B15" s="25"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="10"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="32"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="25" t="e">
         <f t="shared" si="0"/>
-        <v>50486434</v>
-      </c>
-      <c r="L15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L15" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B15,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01010</v>
-      </c>
-      <c r="M15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M15">
         <f>IF(ISNUMBER(MATCH(C15,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C15,'HEX GEN BACKEND'!G:G,0)),C15)</f>
-        <v>000010</v>
-      </c>
-      <c r="N15" t="str">
+        <v>0</v>
+      </c>
+      <c r="N15" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D15,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="O15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O15">
         <f>IF(ISNUMBER(MATCH(E15,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E15,'HEX GEN BACKEND'!H:H,0)),E15)</f>
-        <v>000110</v>
-      </c>
-      <c r="P15" t="str">
+        <v>0</v>
+      </c>
+      <c r="P15" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F15,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="Q15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Q15">
         <f>IF(ISNUMBER(MATCH(G15,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G15,'HEX GEN BACKEND'!I:I,0)),G15)</f>
-        <v>000110</v>
-      </c>
-      <c r="R15" t="str">
+        <v>0</v>
+      </c>
+      <c r="R15" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H15,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
-      </c>
-      <c r="T15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="T15" t="e">
         <f t="shared" si="1"/>
-        <v>01010000010010000110010000110100</v>
-      </c>
-      <c r="V15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="V15" t="e">
         <f t="shared" si="2"/>
-        <v>0101</v>
-      </c>
-      <c r="W15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W15" t="e">
         <f t="shared" si="3"/>
-        <v>0000</v>
-      </c>
-      <c r="X15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X15" t="e">
         <f t="shared" si="4"/>
-        <v>0100</v>
-      </c>
-      <c r="Y15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y15" t="e">
         <f t="shared" si="5"/>
-        <v>1000</v>
-      </c>
-      <c r="Z15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z15" t="e">
         <f t="shared" si="6"/>
-        <v>0110</v>
-      </c>
-      <c r="AA15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA15" t="e">
         <f t="shared" si="7"/>
-        <v>0100</v>
-      </c>
-      <c r="AB15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB15" t="e">
         <f t="shared" si="8"/>
-        <v>0011</v>
-      </c>
-      <c r="AC15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC15" t="e">
         <f t="shared" si="9"/>
-        <v>0100</v>
-      </c>
-      <c r="AE15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AE15" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V15,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>5</v>
-      </c>
-      <c r="AF15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF15" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W15,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AG15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG15" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X15,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AH15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH15" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y15,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AI15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI15" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z15,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>6</v>
-      </c>
-      <c r="AJ15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ15" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA15,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AK15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK15" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB15,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
-      </c>
-      <c r="AL15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL15" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC15,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AN15" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AN15" t="e">
         <f t="shared" si="10"/>
-        <v>50486434</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="42" t="s">
-        <v>158</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F16" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="G16" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="H16" s="41" t="s">
-        <v>114</v>
-      </c>
-      <c r="I16" s="25" t="str">
+      <c r="B16" s="25"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="28"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="32"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="25" t="e">
         <f t="shared" si="0"/>
-        <v>4800381A</v>
-      </c>
-      <c r="L16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L16" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B16,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01001</v>
-      </c>
-      <c r="M16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M16">
         <f>IF(ISNUMBER(MATCH(C16,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C16,'HEX GEN BACKEND'!G:G,0)),C16)</f>
-        <v>000000</v>
-      </c>
-      <c r="N16" t="str">
+        <v>0</v>
+      </c>
+      <c r="N16" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D16,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
-      </c>
-      <c r="O16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O16">
         <f>IF(ISNUMBER(MATCH(E16,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E16,'HEX GEN BACKEND'!H:H,0)),E16)</f>
-        <v>000011</v>
-      </c>
-      <c r="P16" t="str">
+        <v>0</v>
+      </c>
+      <c r="P16" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F16,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
-      </c>
-      <c r="Q16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Q16">
         <f>IF(ISNUMBER(MATCH(G16,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G16,'HEX GEN BACKEND'!I:I,0)),G16)</f>
-        <v>000011</v>
-      </c>
-      <c r="R16" t="str">
+        <v>0</v>
+      </c>
+      <c r="R16" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H16,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="T16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="T16" t="e">
         <f t="shared" si="1"/>
-        <v>01001000000000000011100000011010</v>
-      </c>
-      <c r="V16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="V16" t="e">
         <f t="shared" si="2"/>
-        <v>0100</v>
-      </c>
-      <c r="W16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W16" t="e">
         <f t="shared" si="3"/>
-        <v>1000</v>
-      </c>
-      <c r="X16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X16" t="e">
         <f t="shared" si="4"/>
-        <v>0000</v>
-      </c>
-      <c r="Y16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y16" t="e">
         <f t="shared" si="5"/>
-        <v>0000</v>
-      </c>
-      <c r="Z16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z16" t="e">
         <f t="shared" si="6"/>
-        <v>0011</v>
-      </c>
-      <c r="AA16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA16" t="e">
         <f t="shared" si="7"/>
-        <v>1000</v>
-      </c>
-      <c r="AB16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB16" t="e">
         <f t="shared" si="8"/>
-        <v>0001</v>
-      </c>
-      <c r="AC16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC16" t="e">
         <f t="shared" si="9"/>
-        <v>1010</v>
-      </c>
-      <c r="AE16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AE16" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V16,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AF16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF16" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W16,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AG16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG16" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X16,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AH16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH16" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y16,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AI16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI16" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z16,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
-      </c>
-      <c r="AJ16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ16" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA16,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AK16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK16" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB16,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
-      </c>
-      <c r="AL16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL16" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC16,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>A</v>
-      </c>
-      <c r="AN16" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AN16" t="e">
         <f t="shared" si="10"/>
-        <v>4800381A</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="42" t="s">
-        <v>158</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="F17" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="G17" s="32" t="s">
-        <v>146</v>
-      </c>
-      <c r="H17" s="41" t="s">
-        <v>114</v>
-      </c>
-      <c r="I17" s="25" t="str">
+      <c r="B17" s="25"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="32"/>
+      <c r="H17" s="41"/>
+      <c r="I17" s="25" t="e">
         <f t="shared" si="0"/>
-        <v>48004822</v>
-      </c>
-      <c r="L17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L17" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B17,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01001</v>
-      </c>
-      <c r="M17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M17">
         <f>IF(ISNUMBER(MATCH(C17,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C17,'HEX GEN BACKEND'!G:G,0)),C17)</f>
-        <v>000000</v>
-      </c>
-      <c r="N17" t="str">
+        <v>0</v>
+      </c>
+      <c r="N17" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D17,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
-      </c>
-      <c r="O17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O17">
         <f>IF(ISNUMBER(MATCH(E17,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E17,'HEX GEN BACKEND'!H:H,0)),E17)</f>
-        <v>000100</v>
-      </c>
-      <c r="P17" t="str">
+        <v>0</v>
+      </c>
+      <c r="P17" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F17,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
-      </c>
-      <c r="Q17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Q17">
         <f>IF(ISNUMBER(MATCH(G17,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G17,'HEX GEN BACKEND'!I:I,0)),G17)</f>
-        <v>000100</v>
-      </c>
-      <c r="R17" t="str">
+        <v>0</v>
+      </c>
+      <c r="R17" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H17,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="T17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="T17" t="e">
         <f t="shared" si="1"/>
-        <v>01001000000000000100100000100010</v>
-      </c>
-      <c r="V17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="V17" t="e">
         <f t="shared" si="2"/>
-        <v>0100</v>
-      </c>
-      <c r="W17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W17" t="e">
         <f t="shared" si="3"/>
-        <v>1000</v>
-      </c>
-      <c r="X17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X17" t="e">
         <f t="shared" si="4"/>
-        <v>0000</v>
-      </c>
-      <c r="Y17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y17" t="e">
         <f t="shared" si="5"/>
-        <v>0000</v>
-      </c>
-      <c r="Z17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z17" t="e">
         <f t="shared" si="6"/>
-        <v>0100</v>
-      </c>
-      <c r="AA17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA17" t="e">
         <f t="shared" si="7"/>
-        <v>1000</v>
-      </c>
-      <c r="AB17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB17" t="e">
         <f t="shared" si="8"/>
-        <v>0010</v>
-      </c>
-      <c r="AC17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC17" t="e">
         <f t="shared" si="9"/>
-        <v>0010</v>
-      </c>
-      <c r="AE17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AE17" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AF17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF17" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AG17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG17" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AH17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH17" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AI17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI17" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AJ17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ17" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AK17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK17" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
-      </c>
-      <c r="AL17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL17" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
-      </c>
-      <c r="AN17" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AN17" t="e">
         <f t="shared" si="10"/>
-        <v>48004822</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="42" t="s">
-        <v>158</v>
-      </c>
-      <c r="D18" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="F18" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="G18" s="32" t="s">
-        <v>147</v>
-      </c>
-      <c r="H18" s="41" t="s">
-        <v>114</v>
-      </c>
-      <c r="I18" s="25" t="str">
+      <c r="B18" s="25"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="32"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="25" t="e">
         <f t="shared" si="0"/>
-        <v>4800582A</v>
-      </c>
-      <c r="L18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L18" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B18,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01001</v>
-      </c>
-      <c r="M18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M18">
         <f>IF(ISNUMBER(MATCH(C18,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C18,'HEX GEN BACKEND'!G:G,0)),C18)</f>
-        <v>000000</v>
-      </c>
-      <c r="N18" t="str">
+        <v>0</v>
+      </c>
+      <c r="N18" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D18,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
-      </c>
-      <c r="O18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O18">
         <f>IF(ISNUMBER(MATCH(E18,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E18,'HEX GEN BACKEND'!H:H,0)),E18)</f>
-        <v>000101</v>
-      </c>
-      <c r="P18" t="str">
+        <v>0</v>
+      </c>
+      <c r="P18" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F18,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
-      </c>
-      <c r="Q18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Q18">
         <f>IF(ISNUMBER(MATCH(G18,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G18,'HEX GEN BACKEND'!I:I,0)),G18)</f>
-        <v>000101</v>
-      </c>
-      <c r="R18" t="str">
+        <v>0</v>
+      </c>
+      <c r="R18" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H18,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="T18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="T18" t="e">
         <f t="shared" si="1"/>
-        <v>01001000000000000101100000101010</v>
-      </c>
-      <c r="V18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="V18" t="e">
         <f t="shared" si="2"/>
-        <v>0100</v>
-      </c>
-      <c r="W18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W18" t="e">
         <f t="shared" si="3"/>
-        <v>1000</v>
-      </c>
-      <c r="X18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X18" t="e">
         <f t="shared" si="4"/>
-        <v>0000</v>
-      </c>
-      <c r="Y18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y18" t="e">
         <f t="shared" si="5"/>
-        <v>0000</v>
-      </c>
-      <c r="Z18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z18" t="e">
         <f t="shared" si="6"/>
-        <v>0101</v>
-      </c>
-      <c r="AA18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA18" t="e">
         <f t="shared" si="7"/>
-        <v>1000</v>
-      </c>
-      <c r="AB18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB18" t="e">
         <f t="shared" si="8"/>
-        <v>0010</v>
-      </c>
-      <c r="AC18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC18" t="e">
         <f t="shared" si="9"/>
-        <v>1010</v>
-      </c>
-      <c r="AE18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AE18" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V18,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AF18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF18" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W18,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AG18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG18" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X18,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AH18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH18" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y18,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AI18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI18" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z18,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>5</v>
-      </c>
-      <c r="AJ18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ18" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA18,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AK18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK18" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB18,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
-      </c>
-      <c r="AL18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL18" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC18,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>A</v>
-      </c>
-      <c r="AN18" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AN18" t="e">
         <f t="shared" si="10"/>
-        <v>4800582A</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="42" t="s">
-        <v>158</v>
-      </c>
-      <c r="D19" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="F19" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="G19" s="32" t="s">
-        <v>148</v>
-      </c>
-      <c r="H19" s="41" t="s">
-        <v>114</v>
-      </c>
-      <c r="I19" s="25" t="str">
+      <c r="B19" s="25"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="25" t="e">
         <f t="shared" si="0"/>
-        <v>48006832</v>
-      </c>
-      <c r="L19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L19" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B19,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01001</v>
-      </c>
-      <c r="M19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M19">
         <f>IF(ISNUMBER(MATCH(C19,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C19,'HEX GEN BACKEND'!G:G,0)),C19)</f>
-        <v>000000</v>
-      </c>
-      <c r="N19" t="str">
+        <v>0</v>
+      </c>
+      <c r="N19" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D19,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
-      </c>
-      <c r="O19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O19">
         <f>IF(ISNUMBER(MATCH(E19,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E19,'HEX GEN BACKEND'!H:H,0)),E19)</f>
-        <v>000110</v>
-      </c>
-      <c r="P19" t="str">
+        <v>0</v>
+      </c>
+      <c r="P19" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F19,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
-      </c>
-      <c r="Q19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Q19">
         <f>IF(ISNUMBER(MATCH(G19,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G19,'HEX GEN BACKEND'!I:I,0)),G19)</f>
-        <v>000110</v>
-      </c>
-      <c r="R19" t="str">
+        <v>0</v>
+      </c>
+      <c r="R19" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H19,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="T19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="T19" t="e">
         <f t="shared" si="1"/>
-        <v>01001000000000000110100000110010</v>
-      </c>
-      <c r="V19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="V19" t="e">
         <f t="shared" si="2"/>
-        <v>0100</v>
-      </c>
-      <c r="W19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W19" t="e">
         <f t="shared" si="3"/>
-        <v>1000</v>
-      </c>
-      <c r="X19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X19" t="e">
         <f t="shared" si="4"/>
-        <v>0000</v>
-      </c>
-      <c r="Y19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y19" t="e">
         <f t="shared" si="5"/>
-        <v>0000</v>
-      </c>
-      <c r="Z19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z19" t="e">
         <f t="shared" si="6"/>
-        <v>0110</v>
-      </c>
-      <c r="AA19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA19" t="e">
         <f t="shared" si="7"/>
-        <v>1000</v>
-      </c>
-      <c r="AB19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB19" t="e">
         <f t="shared" si="8"/>
-        <v>0011</v>
-      </c>
-      <c r="AC19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC19" t="e">
         <f t="shared" si="9"/>
-        <v>0010</v>
-      </c>
-      <c r="AE19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AE19" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V19,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AF19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF19" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W19,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AG19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG19" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X19,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AH19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH19" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y19,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AI19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI19" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z19,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>6</v>
-      </c>
-      <c r="AJ19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ19" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA19,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AK19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK19" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB19,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
-      </c>
-      <c r="AL19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL19" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC19,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
-      </c>
-      <c r="AN19" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AN19" t="e">
         <f t="shared" si="10"/>
-        <v>48006832</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="42" t="s">
-        <v>151</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>115</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F20" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="G20" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="H20" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="I20" s="25" t="str">
+      <c r="B20" s="25"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="10"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="32"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="25" t="e">
         <f t="shared" si="0"/>
-        <v>0804341C</v>
-      </c>
-      <c r="L20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L20" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B20,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>00001</v>
-      </c>
-      <c r="M20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M20">
         <f>IF(ISNUMBER(MATCH(C20,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C20,'HEX GEN BACKEND'!G:G,0)),C20)</f>
-        <v>000000</v>
-      </c>
-      <c r="N20" t="str">
+        <v>0</v>
+      </c>
+      <c r="N20" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D20,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>001</v>
-      </c>
-      <c r="O20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O20">
         <f>IF(ISNUMBER(MATCH(E20,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E20,'HEX GEN BACKEND'!H:H,0)),E20)</f>
-        <v>000011</v>
-      </c>
-      <c r="P20" t="str">
+        <v>0</v>
+      </c>
+      <c r="P20" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F20,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="Q20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Q20">
         <f>IF(ISNUMBER(MATCH(G20,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G20,'HEX GEN BACKEND'!I:I,0)),G20)</f>
-        <v>000011</v>
-      </c>
-      <c r="R20" t="str">
+        <v>0</v>
+      </c>
+      <c r="R20" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H20,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
-      </c>
-      <c r="T20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="T20" t="e">
         <f t="shared" si="1"/>
-        <v>00001000000001000011010000011100</v>
-      </c>
-      <c r="V20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="V20" t="e">
         <f t="shared" si="2"/>
-        <v>0000</v>
-      </c>
-      <c r="W20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W20" t="e">
         <f t="shared" si="3"/>
-        <v>1000</v>
-      </c>
-      <c r="X20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X20" t="e">
         <f t="shared" si="4"/>
-        <v>0000</v>
-      </c>
-      <c r="Y20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y20" t="e">
         <f t="shared" si="5"/>
-        <v>0100</v>
-      </c>
-      <c r="Z20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z20" t="e">
         <f t="shared" si="6"/>
-        <v>0011</v>
-      </c>
-      <c r="AA20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA20" t="e">
         <f t="shared" si="7"/>
-        <v>0100</v>
-      </c>
-      <c r="AB20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB20" t="e">
         <f t="shared" si="8"/>
-        <v>0001</v>
-      </c>
-      <c r="AC20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC20" t="e">
         <f t="shared" si="9"/>
-        <v>1100</v>
-      </c>
-      <c r="AE20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AE20" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AF20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF20" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AG20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG20" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AH20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH20" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AI20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI20" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
-      </c>
-      <c r="AJ20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ20" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AK20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK20" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
-      </c>
-      <c r="AL20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL20" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>C</v>
-      </c>
-      <c r="AN20" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AN20" t="e">
         <f t="shared" si="10"/>
-        <v>0804341C</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="D21" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="F21" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="G21" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="H21" s="41" t="s">
-        <v>114</v>
-      </c>
-      <c r="I21" s="25" t="str">
+      <c r="B21" s="25"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="32"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="25" t="e">
         <f t="shared" si="0"/>
-        <v>4850001A</v>
-      </c>
-      <c r="L21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L21" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B21,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01001</v>
-      </c>
-      <c r="M21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M21">
         <f>IF(ISNUMBER(MATCH(C21,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C21,'HEX GEN BACKEND'!G:G,0)),C21)</f>
-        <v>000010</v>
-      </c>
-      <c r="N21" t="str">
+        <v>0</v>
+      </c>
+      <c r="N21" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D21,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
-      </c>
-      <c r="O21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O21">
         <f>IF(ISNUMBER(MATCH(E21,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E21,'HEX GEN BACKEND'!H:H,0)),E21)</f>
-        <v>000000</v>
-      </c>
-      <c r="P21" t="str">
+        <v>0</v>
+      </c>
+      <c r="P21" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F21,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
-      </c>
-      <c r="Q21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Q21">
         <f>IF(ISNUMBER(MATCH(G21,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G21,'HEX GEN BACKEND'!I:I,0)),G21)</f>
-        <v>000011</v>
-      </c>
-      <c r="R21" t="str">
+        <v>0</v>
+      </c>
+      <c r="R21" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H21,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="T21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="T21" t="e">
         <f t="shared" si="1"/>
-        <v>01001000010100000000000000011010</v>
-      </c>
-      <c r="V21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="V21" t="e">
         <f t="shared" si="2"/>
-        <v>0100</v>
-      </c>
-      <c r="W21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W21" t="e">
         <f t="shared" si="3"/>
-        <v>1000</v>
-      </c>
-      <c r="X21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X21" t="e">
         <f t="shared" si="4"/>
-        <v>0101</v>
-      </c>
-      <c r="Y21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y21" t="e">
         <f t="shared" si="5"/>
-        <v>0000</v>
-      </c>
-      <c r="Z21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z21" t="e">
         <f t="shared" si="6"/>
-        <v>0000</v>
-      </c>
-      <c r="AA21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA21" t="e">
         <f t="shared" si="7"/>
-        <v>0000</v>
-      </c>
-      <c r="AB21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB21" t="e">
         <f t="shared" si="8"/>
-        <v>0001</v>
-      </c>
-      <c r="AC21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC21" t="e">
         <f t="shared" si="9"/>
-        <v>1010</v>
-      </c>
-      <c r="AE21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AE21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AF21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AG21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>5</v>
-      </c>
-      <c r="AH21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AI21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AJ21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AK21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
-      </c>
-      <c r="AL21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL21" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>A</v>
-      </c>
-      <c r="AN21" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AN21" t="e">
         <f t="shared" si="10"/>
-        <v>4850001A</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A22" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="D22" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="F22" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="G22" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="H22" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="I22" s="25" t="str">
+      <c r="B22" s="25"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="30"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="25" t="e">
         <f t="shared" si="0"/>
-        <v>0848441C</v>
-      </c>
-      <c r="L22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L22" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B22,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>00001</v>
-      </c>
-      <c r="M22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M22">
         <f>IF(ISNUMBER(MATCH(C22,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C22,'HEX GEN BACKEND'!G:G,0)),C22)</f>
-        <v>000010</v>
-      </c>
-      <c r="N22" t="str">
+        <v>0</v>
+      </c>
+      <c r="N22" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D22,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="O22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O22">
         <f>IF(ISNUMBER(MATCH(E22,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E22,'HEX GEN BACKEND'!H:H,0)),E22)</f>
-        <v>000100</v>
-      </c>
-      <c r="P22" t="str">
+        <v>0</v>
+      </c>
+      <c r="P22" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F22,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="Q22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Q22">
         <f>IF(ISNUMBER(MATCH(G22,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G22,'HEX GEN BACKEND'!I:I,0)),G22)</f>
-        <v>000011</v>
-      </c>
-      <c r="R22" t="str">
+        <v>0</v>
+      </c>
+      <c r="R22" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H22,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
-      </c>
-      <c r="T22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="T22" t="e">
         <f t="shared" si="1"/>
-        <v>00001000010010000100010000011100</v>
-      </c>
-      <c r="V22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="V22" t="e">
         <f t="shared" si="2"/>
-        <v>0000</v>
-      </c>
-      <c r="W22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W22" t="e">
         <f t="shared" si="3"/>
-        <v>1000</v>
-      </c>
-      <c r="X22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X22" t="e">
         <f t="shared" si="4"/>
-        <v>0100</v>
-      </c>
-      <c r="Y22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y22" t="e">
         <f t="shared" si="5"/>
-        <v>1000</v>
-      </c>
-      <c r="Z22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z22" t="e">
         <f t="shared" si="6"/>
-        <v>0100</v>
-      </c>
-      <c r="AA22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA22" t="e">
         <f t="shared" si="7"/>
-        <v>0100</v>
-      </c>
-      <c r="AB22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB22" t="e">
         <f t="shared" si="8"/>
-        <v>0001</v>
-      </c>
-      <c r="AC22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC22" t="e">
         <f t="shared" si="9"/>
-        <v>1100</v>
-      </c>
-      <c r="AE22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AE22" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AF22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF22" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AG22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG22" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AH22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH22" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AI22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI22" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AJ22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ22" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AK22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK22" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
-      </c>
-      <c r="AL22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL22" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>C</v>
-      </c>
-      <c r="AN22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AN22" t="e">
         <f t="shared" si="10"/>
-        <v>0848441C</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A23" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="B23" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="D23" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="F23" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="G23" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="H23" s="41" t="s">
-        <v>114</v>
-      </c>
-      <c r="I23" s="25" t="str">
+      <c r="B23" s="25"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="30"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="25" t="e">
         <f t="shared" si="0"/>
-        <v>4850001A</v>
-      </c>
-      <c r="L23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L23" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B23,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01001</v>
-      </c>
-      <c r="M23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M23">
         <f>IF(ISNUMBER(MATCH(C23,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C23,'HEX GEN BACKEND'!G:G,0)),C23)</f>
-        <v>000010</v>
-      </c>
-      <c r="N23" t="str">
+        <v>0</v>
+      </c>
+      <c r="N23" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D23,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
-      </c>
-      <c r="O23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O23">
         <f>IF(ISNUMBER(MATCH(E23,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E23,'HEX GEN BACKEND'!H:H,0)),E23)</f>
-        <v>000000</v>
-      </c>
-      <c r="P23" t="str">
+        <v>0</v>
+      </c>
+      <c r="P23" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F23,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
-      </c>
-      <c r="Q23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Q23">
         <f>IF(ISNUMBER(MATCH(G23,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G23,'HEX GEN BACKEND'!I:I,0)),G23)</f>
-        <v>000011</v>
-      </c>
-      <c r="R23" t="str">
+        <v>0</v>
+      </c>
+      <c r="R23" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H23,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="T23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="T23" t="e">
         <f t="shared" si="1"/>
-        <v>01001000010100000000000000011010</v>
-      </c>
-      <c r="V23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="V23" t="e">
         <f t="shared" si="2"/>
-        <v>0100</v>
-      </c>
-      <c r="W23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W23" t="e">
         <f t="shared" si="3"/>
-        <v>1000</v>
-      </c>
-      <c r="X23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X23" t="e">
         <f t="shared" si="4"/>
-        <v>0101</v>
-      </c>
-      <c r="Y23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y23" t="e">
         <f t="shared" si="5"/>
-        <v>0000</v>
-      </c>
-      <c r="Z23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z23" t="e">
         <f t="shared" si="6"/>
-        <v>0000</v>
-      </c>
-      <c r="AA23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA23" t="e">
         <f t="shared" si="7"/>
-        <v>0000</v>
-      </c>
-      <c r="AB23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB23" t="e">
         <f t="shared" si="8"/>
-        <v>0001</v>
-      </c>
-      <c r="AC23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC23" t="e">
         <f t="shared" si="9"/>
-        <v>1010</v>
-      </c>
-      <c r="AE23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AE23" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AF23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF23" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AG23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG23" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>5</v>
-      </c>
-      <c r="AH23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH23" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AI23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI23" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AJ23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ23" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AK23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK23" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
-      </c>
-      <c r="AL23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL23" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>A</v>
-      </c>
-      <c r="AN23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AN23" t="e">
         <f t="shared" si="10"/>
-        <v>4850001A</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A24" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="B24" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C24" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="D24" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="F24" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="G24" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="H24" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="I24" s="25" t="str">
+      <c r="B24" s="25"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="30"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="41"/>
+      <c r="I24" s="25" t="e">
         <f t="shared" si="0"/>
-        <v>0848541C</v>
-      </c>
-      <c r="L24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L24" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B24,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>00001</v>
-      </c>
-      <c r="M24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M24">
         <f>IF(ISNUMBER(MATCH(C24,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C24,'HEX GEN BACKEND'!G:G,0)),C24)</f>
-        <v>000010</v>
-      </c>
-      <c r="N24" t="str">
+        <v>0</v>
+      </c>
+      <c r="N24" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D24,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="O24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O24">
         <f>IF(ISNUMBER(MATCH(E24,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E24,'HEX GEN BACKEND'!H:H,0)),E24)</f>
-        <v>000101</v>
-      </c>
-      <c r="P24" t="str">
+        <v>0</v>
+      </c>
+      <c r="P24" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F24,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="Q24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Q24">
         <f>IF(ISNUMBER(MATCH(G24,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G24,'HEX GEN BACKEND'!I:I,0)),G24)</f>
-        <v>000011</v>
-      </c>
-      <c r="R24" t="str">
+        <v>0</v>
+      </c>
+      <c r="R24" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H24,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
-      </c>
-      <c r="T24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="T24" t="e">
         <f t="shared" si="1"/>
-        <v>00001000010010000101010000011100</v>
-      </c>
-      <c r="V24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="V24" t="e">
         <f t="shared" si="2"/>
-        <v>0000</v>
-      </c>
-      <c r="W24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W24" t="e">
         <f t="shared" si="3"/>
-        <v>1000</v>
-      </c>
-      <c r="X24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X24" t="e">
         <f t="shared" si="4"/>
-        <v>0100</v>
-      </c>
-      <c r="Y24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y24" t="e">
         <f t="shared" si="5"/>
-        <v>1000</v>
-      </c>
-      <c r="Z24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z24" t="e">
         <f t="shared" si="6"/>
-        <v>0101</v>
-      </c>
-      <c r="AA24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA24" t="e">
         <f t="shared" si="7"/>
-        <v>0100</v>
-      </c>
-      <c r="AB24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB24" t="e">
         <f t="shared" si="8"/>
-        <v>0001</v>
-      </c>
-      <c r="AC24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC24" t="e">
         <f t="shared" si="9"/>
-        <v>1100</v>
-      </c>
-      <c r="AE24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AE24" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V24,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AF24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF24" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W24,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AG24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG24" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X24,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AH24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH24" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y24,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AI24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI24" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z24,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>5</v>
-      </c>
-      <c r="AJ24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ24" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA24,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AK24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK24" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB24,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
-      </c>
-      <c r="AL24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL24" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC24,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>C</v>
-      </c>
-      <c r="AN24" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AN24" t="e">
         <f t="shared" si="10"/>
-        <v>0848541C</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A25" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="B25" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="D25" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="F25" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="G25" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="H25" s="41" t="s">
-        <v>114</v>
-      </c>
-      <c r="I25" s="25" t="str">
+      <c r="B25" s="25"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="30"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="41"/>
+      <c r="I25" s="25" t="e">
         <f t="shared" si="0"/>
-        <v>4850001A</v>
-      </c>
-      <c r="L25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L25" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B25,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01001</v>
-      </c>
-      <c r="M25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M25">
         <f>IF(ISNUMBER(MATCH(C25,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C25,'HEX GEN BACKEND'!G:G,0)),C25)</f>
-        <v>000010</v>
-      </c>
-      <c r="N25" t="str">
+        <v>0</v>
+      </c>
+      <c r="N25" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D25,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
-      </c>
-      <c r="O25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O25">
         <f>IF(ISNUMBER(MATCH(E25,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E25,'HEX GEN BACKEND'!H:H,0)),E25)</f>
-        <v>000000</v>
-      </c>
-      <c r="P25" t="str">
+        <v>0</v>
+      </c>
+      <c r="P25" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F25,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
-      </c>
-      <c r="Q25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Q25">
         <f>IF(ISNUMBER(MATCH(G25,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G25,'HEX GEN BACKEND'!I:I,0)),G25)</f>
-        <v>000011</v>
-      </c>
-      <c r="R25" t="str">
+        <v>0</v>
+      </c>
+      <c r="R25" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H25,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="T25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="T25" t="e">
         <f t="shared" si="1"/>
-        <v>01001000010100000000000000011010</v>
-      </c>
-      <c r="V25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="V25" t="e">
         <f t="shared" si="2"/>
-        <v>0100</v>
-      </c>
-      <c r="W25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W25" t="e">
         <f t="shared" si="3"/>
-        <v>1000</v>
-      </c>
-      <c r="X25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X25" t="e">
         <f t="shared" si="4"/>
-        <v>0101</v>
-      </c>
-      <c r="Y25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y25" t="e">
         <f t="shared" si="5"/>
-        <v>0000</v>
-      </c>
-      <c r="Z25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z25" t="e">
         <f t="shared" si="6"/>
-        <v>0000</v>
-      </c>
-      <c r="AA25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA25" t="e">
         <f t="shared" si="7"/>
-        <v>0000</v>
-      </c>
-      <c r="AB25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB25" t="e">
         <f t="shared" si="8"/>
-        <v>0001</v>
-      </c>
-      <c r="AC25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC25" t="e">
         <f t="shared" si="9"/>
-        <v>1010</v>
-      </c>
-      <c r="AE25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AE25" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V25,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AF25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF25" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W25,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AG25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG25" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X25,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>5</v>
-      </c>
-      <c r="AH25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH25" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y25,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AI25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI25" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z25,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AJ25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ25" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA25,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AK25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK25" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB25,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
-      </c>
-      <c r="AL25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL25" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC25,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>A</v>
-      </c>
-      <c r="AN25" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AN25" t="e">
         <f t="shared" si="10"/>
-        <v>4850001A</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A26" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="B26" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26" s="42" t="s">
-        <v>130</v>
-      </c>
-      <c r="D26" s="28" t="s">
-        <v>114</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="F26" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="G26" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="H26" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="I26" s="25" t="str">
+      <c r="B26" s="25"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="10"/>
+      <c r="F26" s="30"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="41"/>
+      <c r="I26" s="25" t="e">
         <f t="shared" si="0"/>
-        <v>0848641C</v>
-      </c>
-      <c r="L26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L26" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B26,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>00001</v>
-      </c>
-      <c r="M26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M26">
         <f>IF(ISNUMBER(MATCH(C26,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C26,'HEX GEN BACKEND'!G:G,0)),C26)</f>
-        <v>000010</v>
-      </c>
-      <c r="N26" t="str">
+        <v>0</v>
+      </c>
+      <c r="N26" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D26,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="O26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O26">
         <f>IF(ISNUMBER(MATCH(E26,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E26,'HEX GEN BACKEND'!H:H,0)),E26)</f>
-        <v>000110</v>
-      </c>
-      <c r="P26" t="str">
+        <v>0</v>
+      </c>
+      <c r="P26" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F26,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="Q26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Q26">
         <f>IF(ISNUMBER(MATCH(G26,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G26,'HEX GEN BACKEND'!I:I,0)),G26)</f>
-        <v>000011</v>
-      </c>
-      <c r="R26" t="str">
+        <v>0</v>
+      </c>
+      <c r="R26" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H26,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
-      </c>
-      <c r="T26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="T26" t="e">
         <f t="shared" si="1"/>
-        <v>00001000010010000110010000011100</v>
-      </c>
-      <c r="V26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="V26" t="e">
         <f t="shared" si="2"/>
-        <v>0000</v>
-      </c>
-      <c r="W26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W26" t="e">
         <f t="shared" si="3"/>
-        <v>1000</v>
-      </c>
-      <c r="X26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X26" t="e">
         <f t="shared" si="4"/>
-        <v>0100</v>
-      </c>
-      <c r="Y26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y26" t="e">
         <f t="shared" si="5"/>
-        <v>1000</v>
-      </c>
-      <c r="Z26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z26" t="e">
         <f t="shared" si="6"/>
-        <v>0110</v>
-      </c>
-      <c r="AA26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA26" t="e">
         <f t="shared" si="7"/>
-        <v>0100</v>
-      </c>
-      <c r="AB26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB26" t="e">
         <f t="shared" si="8"/>
-        <v>0001</v>
-      </c>
-      <c r="AC26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC26" t="e">
         <f t="shared" si="9"/>
-        <v>1100</v>
-      </c>
-      <c r="AE26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AE26" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V26,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AF26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF26" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W26,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AG26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG26" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X26,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AH26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH26" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y26,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
-      </c>
-      <c r="AI26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI26" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z26,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>6</v>
-      </c>
-      <c r="AJ26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ26" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA26,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
-      </c>
-      <c r="AK26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK26" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB26,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
-      </c>
-      <c r="AL26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL26" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC26,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>C</v>
-      </c>
-      <c r="AN26" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AN26" t="e">
         <f t="shared" si="10"/>
-        <v>0848641C</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A27" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="B27" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="C27" s="42" t="s">
-        <v>158</v>
-      </c>
-      <c r="D27" s="28" t="s">
-        <v>117</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="F27" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="G27" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="H27" s="41" t="s">
-        <v>114</v>
-      </c>
-      <c r="I27" s="25" t="str">
+      <c r="B27" s="25"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="10"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="41"/>
+      <c r="I27" s="25" t="e">
         <f t="shared" si="0"/>
-        <v>C000001A</v>
-      </c>
-      <c r="L27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L27" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B27,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>11000</v>
-      </c>
-      <c r="M27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M27">
         <f>IF(ISNUMBER(MATCH(C27,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C27,'HEX GEN BACKEND'!G:G,0)),C27)</f>
-        <v>000000</v>
-      </c>
-      <c r="N27" t="str">
+        <v>0</v>
+      </c>
+      <c r="N27" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D27,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
-      </c>
-      <c r="O27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O27">
         <f>IF(ISNUMBER(MATCH(E27,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E27,'HEX GEN BACKEND'!H:H,0)),E27)</f>
-        <v>000000</v>
-      </c>
-      <c r="P27" t="str">
+        <v>0</v>
+      </c>
+      <c r="P27" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F27,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
-      </c>
-      <c r="Q27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Q27">
         <f>IF(ISNUMBER(MATCH(G27,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G27,'HEX GEN BACKEND'!I:I,0)),G27)</f>
-        <v>000011</v>
-      </c>
-      <c r="R27" t="str">
+        <v>0</v>
+      </c>
+      <c r="R27" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H27,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="T27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="T27" t="e">
         <f t="shared" si="1"/>
-        <v>11000000000000000000000000011010</v>
-      </c>
-      <c r="V27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="V27" t="e">
         <f t="shared" si="2"/>
-        <v>1100</v>
-      </c>
-      <c r="W27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W27" t="e">
         <f t="shared" si="3"/>
-        <v>0000</v>
-      </c>
-      <c r="X27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X27" t="e">
         <f t="shared" si="4"/>
-        <v>0000</v>
-      </c>
-      <c r="Y27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y27" t="e">
         <f t="shared" si="5"/>
-        <v>0000</v>
-      </c>
-      <c r="Z27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z27" t="e">
         <f t="shared" si="6"/>
-        <v>0000</v>
-      </c>
-      <c r="AA27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA27" t="e">
         <f t="shared" si="7"/>
-        <v>0000</v>
-      </c>
-      <c r="AB27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB27" t="e">
         <f t="shared" si="8"/>
-        <v>0001</v>
-      </c>
-      <c r="AC27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC27" t="e">
         <f t="shared" si="9"/>
-        <v>1010</v>
-      </c>
-      <c r="AE27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AE27" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V27,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>C</v>
-      </c>
-      <c r="AF27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF27" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W27,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AG27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG27" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X27,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AH27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH27" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y27,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AI27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI27" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z27,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AJ27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ27" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA27,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AK27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK27" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB27,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
-      </c>
-      <c r="AL27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL27" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC27,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>A</v>
-      </c>
-      <c r="AN27" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AN27" t="e">
         <f t="shared" si="10"/>
-        <v>C000001A</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.25">
@@ -4969,7 +4717,7 @@
           <x14:formula1>
             <xm:f>'HEX GEN BACKEND'!$D$1:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H32 F2:F32 D2:D32</xm:sqref>
+          <xm:sqref>D2:D32 F2:F32 H2:H32</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
multiply using loop made smaller
</commit_message>
<xml_diff>
--- a/Instructions/Binary Instructions.xlsx
+++ b/Instructions/Binary Instructions.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="194">
   <si>
     <t>0001</t>
   </si>
@@ -615,7 +615,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -634,13 +634,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -776,13 +769,13 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1066,7 +1059,7 @@
   <dimension ref="A1:AN101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I23"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1379,13 +1372,13 @@
         <v>32</v>
       </c>
       <c r="B4" s="52" t="s">
-        <v>107</v>
+        <v>9</v>
       </c>
       <c r="C4" s="53" t="s">
-        <v>31</v>
+        <v>158</v>
       </c>
       <c r="D4" s="54" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="E4" s="55" t="s">
         <v>137</v>
@@ -1401,19 +1394,19 @@
       </c>
       <c r="I4" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>6024241C</v>
+        <v>4800241C</v>
       </c>
       <c r="L4" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B4,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01100</v>
+        <v>01001</v>
       </c>
       <c r="M4" t="str">
         <f>IF(ISNUMBER(MATCH(C4,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C4,'HEX GEN BACKEND'!G:G,0)),C4)</f>
-        <v>000001</v>
+        <v>000000</v>
       </c>
       <c r="N4" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D4,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>001</v>
+        <v>000</v>
       </c>
       <c r="O4" t="str">
         <f>IF(ISNUMBER(MATCH(E4,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E4,'HEX GEN BACKEND'!H:H,0)),E4)</f>
@@ -1433,23 +1426,23 @@
       </c>
       <c r="T4" t="str">
         <f t="shared" si="1"/>
-        <v>01100000001001000010010000011100</v>
+        <v>01001000000000000010010000011100</v>
       </c>
       <c r="V4" t="str">
         <f t="shared" si="2"/>
-        <v>0110</v>
+        <v>0100</v>
       </c>
       <c r="W4" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="X4" t="str">
         <f t="shared" si="4"/>
-        <v>0010</v>
+        <v>0000</v>
       </c>
       <c r="Y4" t="str">
         <f t="shared" si="5"/>
-        <v>0100</v>
+        <v>0000</v>
       </c>
       <c r="Z4" t="str">
         <f t="shared" si="6"/>
@@ -1469,19 +1462,19 @@
       </c>
       <c r="AE4" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V4,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AF4" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W4,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AG4" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X4,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH4" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y4,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AI4" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z4,'HEX GEN BACKEND'!L:L,0))</f>
@@ -1501,7 +1494,7 @@
       </c>
       <c r="AN4" t="str">
         <f t="shared" si="10"/>
-        <v>6024241C</v>
+        <v>4800241C</v>
       </c>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
@@ -1509,19 +1502,19 @@
         <v>34</v>
       </c>
       <c r="B5" s="52" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" s="53" t="s">
-        <v>158</v>
+        <v>35</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E5" s="55" t="s">
-        <v>138</v>
+        <v>33</v>
       </c>
       <c r="F5" s="56" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="G5" s="57" t="s">
         <v>145</v>
@@ -1531,27 +1524,27 @@
       </c>
       <c r="I5" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>4800381A</v>
+        <v>30A4421A</v>
       </c>
       <c r="L5" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B5,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01001</v>
+        <v>00110</v>
       </c>
       <c r="M5" t="str">
         <f>IF(ISNUMBER(MATCH(C5,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C5,'HEX GEN BACKEND'!G:G,0)),C5)</f>
-        <v>000000</v>
+        <v>000101</v>
       </c>
       <c r="N5" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D5,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
+        <v>001</v>
       </c>
       <c r="O5" t="str">
         <f>IF(ISNUMBER(MATCH(E5,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E5,'HEX GEN BACKEND'!H:H,0)),E5)</f>
-        <v>000011</v>
+        <v>000100</v>
       </c>
       <c r="P5" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F5,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
+        <v>001</v>
       </c>
       <c r="Q5" t="str">
         <f>IF(ISNUMBER(MATCH(G5,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G5,'HEX GEN BACKEND'!I:I,0)),G5)</f>
@@ -1563,31 +1556,31 @@
       </c>
       <c r="T5" t="str">
         <f t="shared" si="1"/>
-        <v>01001000000000000011100000011010</v>
+        <v>00110000101001000100001000011010</v>
       </c>
       <c r="V5" t="str">
         <f t="shared" si="2"/>
-        <v>0100</v>
+        <v>0011</v>
       </c>
       <c r="W5" t="str">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="X5" t="str">
         <f t="shared" si="4"/>
-        <v>0000</v>
+        <v>1010</v>
       </c>
       <c r="Y5" t="str">
         <f t="shared" si="5"/>
-        <v>0000</v>
+        <v>0100</v>
       </c>
       <c r="Z5" t="str">
         <f t="shared" si="6"/>
-        <v>0011</v>
+        <v>0100</v>
       </c>
       <c r="AA5" t="str">
         <f t="shared" si="7"/>
-        <v>1000</v>
+        <v>0010</v>
       </c>
       <c r="AB5" t="str">
         <f t="shared" si="8"/>
@@ -1599,27 +1592,27 @@
       </c>
       <c r="AE5" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V5,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AF5" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W5,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AG5" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X5,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>A</v>
       </c>
       <c r="AH5" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y5,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AI5" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z5,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AJ5" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA5,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AK5" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB5,'HEX GEN BACKEND'!L:L,0))</f>
@@ -1631,7 +1624,7 @@
       </c>
       <c r="AN5" t="str">
         <f t="shared" si="10"/>
-        <v>4800381A</v>
+        <v>30A4421A</v>
       </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.25">
@@ -1639,53 +1632,53 @@
         <v>33</v>
       </c>
       <c r="B6" s="52" t="s">
-        <v>124</v>
+        <v>9</v>
       </c>
       <c r="C6" s="53" t="s">
-        <v>31</v>
+        <v>130</v>
       </c>
       <c r="D6" s="54" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E6" s="55" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="F6" s="56" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="G6" s="57" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="H6" s="58" t="s">
         <v>113</v>
       </c>
       <c r="I6" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>2824341C</v>
+        <v>4848003C</v>
       </c>
       <c r="L6" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B6,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>00101</v>
+        <v>01001</v>
       </c>
       <c r="M6" t="str">
         <f>IF(ISNUMBER(MATCH(C6,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C6,'HEX GEN BACKEND'!G:G,0)),C6)</f>
-        <v>000001</v>
+        <v>000010</v>
       </c>
       <c r="N6" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D6,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>001</v>
+        <v>010</v>
       </c>
       <c r="O6" t="str">
         <f>IF(ISNUMBER(MATCH(E6,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E6,'HEX GEN BACKEND'!H:H,0)),E6)</f>
-        <v>000011</v>
+        <v>000000</v>
       </c>
       <c r="P6" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F6,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
+        <v>000</v>
       </c>
       <c r="Q6" t="str">
         <f>IF(ISNUMBER(MATCH(G6,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G6,'HEX GEN BACKEND'!I:I,0)),G6)</f>
-        <v>000011</v>
+        <v>000111</v>
       </c>
       <c r="R6" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H6,'HEX GEN BACKEND'!D:D,0))</f>
@@ -1693,11 +1686,11 @@
       </c>
       <c r="T6" t="str">
         <f t="shared" si="1"/>
-        <v>00101000001001000011010000011100</v>
+        <v>01001000010010000000000000111100</v>
       </c>
       <c r="V6" t="str">
         <f t="shared" si="2"/>
-        <v>0010</v>
+        <v>0100</v>
       </c>
       <c r="W6" t="str">
         <f t="shared" si="3"/>
@@ -1705,23 +1698,23 @@
       </c>
       <c r="X6" t="str">
         <f t="shared" si="4"/>
-        <v>0010</v>
+        <v>0100</v>
       </c>
       <c r="Y6" t="str">
         <f t="shared" si="5"/>
-        <v>0100</v>
+        <v>1000</v>
       </c>
       <c r="Z6" t="str">
         <f t="shared" si="6"/>
-        <v>0011</v>
+        <v>0000</v>
       </c>
       <c r="AA6" t="str">
         <f t="shared" si="7"/>
-        <v>0100</v>
+        <v>0000</v>
       </c>
       <c r="AB6" t="str">
         <f t="shared" si="8"/>
-        <v>0001</v>
+        <v>0011</v>
       </c>
       <c r="AC6" t="str">
         <f t="shared" si="9"/>
@@ -1729,7 +1722,7 @@
       </c>
       <c r="AE6" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V6,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AF6" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W6,'HEX GEN BACKEND'!L:L,0))</f>
@@ -1737,23 +1730,23 @@
       </c>
       <c r="AG6" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X6,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AH6" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y6,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AI6" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z6,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AJ6" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA6,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AK6" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB6,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AL6" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC6,'HEX GEN BACKEND'!L:L,0))</f>
@@ -1761,7 +1754,7 @@
       </c>
       <c r="AN6" t="str">
         <f t="shared" si="10"/>
-        <v>2824341C</v>
+        <v>4848003C</v>
       </c>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.25">
@@ -1769,129 +1762,129 @@
         <v>35</v>
       </c>
       <c r="B7" s="52" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C7" s="53" t="s">
-        <v>37</v>
+        <v>158</v>
       </c>
       <c r="D7" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="55" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="G7" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="58" t="s">
         <v>115</v>
-      </c>
-      <c r="E7" s="55" t="s">
-        <v>36</v>
-      </c>
-      <c r="F7" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="G7" s="57" t="s">
-        <v>145</v>
-      </c>
-      <c r="H7" s="58" t="s">
-        <v>114</v>
       </c>
       <c r="I7" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>30E4621A</v>
+        <v>48004809</v>
       </c>
       <c r="L7" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B7,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>00110</v>
+        <v>01001</v>
       </c>
       <c r="M7" t="str">
         <f>IF(ISNUMBER(MATCH(C7,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C7,'HEX GEN BACKEND'!G:G,0)),C7)</f>
-        <v>000111</v>
+        <v>000000</v>
       </c>
       <c r="N7" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D7,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>001</v>
+        <v>000</v>
       </c>
       <c r="O7" t="str">
         <f>IF(ISNUMBER(MATCH(E7,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E7,'HEX GEN BACKEND'!H:H,0)),E7)</f>
-        <v>000110</v>
+        <v>000100</v>
       </c>
       <c r="P7" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F7,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>001</v>
+        <v>100</v>
       </c>
       <c r="Q7" t="str">
         <f>IF(ISNUMBER(MATCH(G7,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G7,'HEX GEN BACKEND'!I:I,0)),G7)</f>
-        <v>000011</v>
+        <v>000001</v>
       </c>
       <c r="R7" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H7,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
+        <v>001</v>
       </c>
       <c r="T7" t="str">
         <f t="shared" si="1"/>
-        <v>00110000111001000110001000011010</v>
+        <v>01001000000000000100100000001001</v>
       </c>
       <c r="V7" t="str">
         <f t="shared" si="2"/>
-        <v>0011</v>
+        <v>0100</v>
       </c>
       <c r="W7" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="X7" t="str">
         <f t="shared" si="4"/>
-        <v>1110</v>
+        <v>0000</v>
       </c>
       <c r="Y7" t="str">
         <f t="shared" si="5"/>
-        <v>0100</v>
+        <v>0000</v>
       </c>
       <c r="Z7" t="str">
         <f t="shared" si="6"/>
-        <v>0110</v>
+        <v>0100</v>
       </c>
       <c r="AA7" t="str">
         <f t="shared" si="7"/>
-        <v>0010</v>
+        <v>1000</v>
       </c>
       <c r="AB7" t="str">
         <f t="shared" si="8"/>
-        <v>0001</v>
+        <v>0000</v>
       </c>
       <c r="AC7" t="str">
         <f t="shared" si="9"/>
-        <v>1010</v>
+        <v>1001</v>
       </c>
       <c r="AE7" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V7,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AF7" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W7,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AG7" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X7,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>E</v>
+        <v>0</v>
       </c>
       <c r="AH7" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y7,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AI7" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z7,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AJ7" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA7,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AK7" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB7,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL7" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC7,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>A</v>
+        <v>9</v>
       </c>
       <c r="AN7" t="str">
         <f t="shared" si="10"/>
-        <v>30E4621A</v>
+        <v>48004809</v>
       </c>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.25">
@@ -1899,53 +1892,53 @@
         <v>36</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>2</v>
+        <v>105</v>
       </c>
       <c r="C8" s="53" t="s">
-        <v>130</v>
+        <v>31</v>
       </c>
       <c r="D8" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" s="55" t="s">
+        <v>139</v>
+      </c>
+      <c r="F8" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="E8" s="55" t="s">
-        <v>151</v>
-      </c>
-      <c r="F8" s="56" t="s">
-        <v>115</v>
-      </c>
       <c r="G8" s="57" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="H8" s="58" t="s">
         <v>113</v>
       </c>
       <c r="I8" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>0848023C</v>
+        <v>50244424</v>
       </c>
       <c r="L8" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B8,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>00001</v>
+        <v>01010</v>
       </c>
       <c r="M8" t="str">
         <f>IF(ISNUMBER(MATCH(C8,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C8,'HEX GEN BACKEND'!G:G,0)),C8)</f>
-        <v>000010</v>
+        <v>000001</v>
       </c>
       <c r="N8" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D8,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
+        <v>001</v>
       </c>
       <c r="O8" t="str">
         <f>IF(ISNUMBER(MATCH(E8,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E8,'HEX GEN BACKEND'!H:H,0)),E8)</f>
-        <v>000000</v>
+        <v>000100</v>
       </c>
       <c r="P8" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F8,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>001</v>
+        <v>010</v>
       </c>
       <c r="Q8" t="str">
         <f>IF(ISNUMBER(MATCH(G8,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G8,'HEX GEN BACKEND'!I:I,0)),G8)</f>
-        <v>000111</v>
+        <v>000100</v>
       </c>
       <c r="R8" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H8,'HEX GEN BACKEND'!D:D,0))</f>
@@ -1953,75 +1946,75 @@
       </c>
       <c r="T8" t="str">
         <f t="shared" si="1"/>
-        <v>00001000010010000000001000111100</v>
+        <v>01010000001001000100010000100100</v>
       </c>
       <c r="V8" t="str">
         <f t="shared" si="2"/>
-        <v>0000</v>
+        <v>0101</v>
       </c>
       <c r="W8" t="str">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="X8" t="str">
         <f t="shared" si="4"/>
-        <v>0100</v>
+        <v>0010</v>
       </c>
       <c r="Y8" t="str">
         <f t="shared" si="5"/>
-        <v>1000</v>
+        <v>0100</v>
       </c>
       <c r="Z8" t="str">
         <f t="shared" si="6"/>
-        <v>0000</v>
+        <v>0100</v>
       </c>
       <c r="AA8" t="str">
         <f t="shared" si="7"/>
-        <v>0010</v>
+        <v>0100</v>
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="8"/>
-        <v>0011</v>
+        <v>0010</v>
       </c>
       <c r="AC8" t="str">
         <f t="shared" si="9"/>
-        <v>1100</v>
+        <v>0100</v>
       </c>
       <c r="AE8" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V8,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AF8" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W8,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AG8" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X8,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AH8" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y8,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="AI8" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z8,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AJ8" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA8,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AK8" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB8,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AL8" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC8,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>C</v>
+        <v>4</v>
       </c>
       <c r="AN8" t="str">
         <f t="shared" si="10"/>
-        <v>0848023C</v>
+        <v>50244424</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.25">
@@ -2032,10 +2025,10 @@
         <v>9</v>
       </c>
       <c r="C9" s="53" t="s">
-        <v>158</v>
+        <v>132</v>
       </c>
       <c r="D9" s="54" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E9" s="55" t="s">
         <v>139</v>
@@ -2044,14 +2037,14 @@
         <v>113</v>
       </c>
       <c r="G9" s="57" t="s">
-        <v>31</v>
+        <v>146</v>
       </c>
       <c r="H9" s="58" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I9" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>48004809</v>
+        <v>48904822</v>
       </c>
       <c r="L9" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B9,'HEX GEN BACKEND'!A:A,0))</f>
@@ -2059,11 +2052,11 @@
       </c>
       <c r="M9" t="str">
         <f>IF(ISNUMBER(MATCH(C9,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C9,'HEX GEN BACKEND'!G:G,0)),C9)</f>
-        <v>000000</v>
+        <v>000100</v>
       </c>
       <c r="N9" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D9,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
+        <v>100</v>
       </c>
       <c r="O9" t="str">
         <f>IF(ISNUMBER(MATCH(E9,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E9,'HEX GEN BACKEND'!H:H,0)),E9)</f>
@@ -2075,15 +2068,15 @@
       </c>
       <c r="Q9" t="str">
         <f>IF(ISNUMBER(MATCH(G9,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G9,'HEX GEN BACKEND'!I:I,0)),G9)</f>
-        <v>000001</v>
+        <v>000100</v>
       </c>
       <c r="R9" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H9,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>001</v>
+        <v>010</v>
       </c>
       <c r="T9" t="str">
         <f t="shared" si="1"/>
-        <v>01001000000000000100100000001001</v>
+        <v>01001000100100000100100000100010</v>
       </c>
       <c r="V9" t="str">
         <f t="shared" si="2"/>
@@ -2095,7 +2088,7 @@
       </c>
       <c r="X9" t="str">
         <f t="shared" si="4"/>
-        <v>0000</v>
+        <v>1001</v>
       </c>
       <c r="Y9" t="str">
         <f t="shared" si="5"/>
@@ -2111,11 +2104,11 @@
       </c>
       <c r="AB9" t="str">
         <f t="shared" si="8"/>
-        <v>0000</v>
+        <v>0010</v>
       </c>
       <c r="AC9" t="str">
         <f t="shared" si="9"/>
-        <v>1001</v>
+        <v>0010</v>
       </c>
       <c r="AE9" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V9,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2127,7 +2120,7 @@
       </c>
       <c r="AG9" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X9,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="AH9" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y9,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2143,61 +2136,61 @@
       </c>
       <c r="AK9" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB9,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL9" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC9,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="AN9" t="str">
         <f t="shared" si="10"/>
-        <v>48004809</v>
+        <v>48904822</v>
       </c>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="F10" s="29" t="s">
+      <c r="B10" s="52" t="s">
+        <v>107</v>
+      </c>
+      <c r="C10" s="53" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="54" t="s">
         <v>114</v>
       </c>
-      <c r="G10" s="31" t="s">
-        <v>146</v>
-      </c>
-      <c r="H10" s="40" t="s">
+      <c r="E10" s="55" t="s">
+        <v>137</v>
+      </c>
+      <c r="F10" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="G10" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="H10" s="58" t="s">
         <v>113</v>
       </c>
       <c r="I10" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>50244424</v>
+        <v>6088241C</v>
       </c>
       <c r="L10" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B10,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01010</v>
+        <v>01100</v>
       </c>
       <c r="M10" t="str">
         <f>IF(ISNUMBER(MATCH(C10,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C10,'HEX GEN BACKEND'!G:G,0)),C10)</f>
-        <v>000001</v>
+        <v>000100</v>
       </c>
       <c r="N10" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D10,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>001</v>
+        <v>010</v>
       </c>
       <c r="O10" t="str">
         <f>IF(ISNUMBER(MATCH(E10,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E10,'HEX GEN BACKEND'!H:H,0)),E10)</f>
-        <v>000100</v>
+        <v>000010</v>
       </c>
       <c r="P10" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F10,'HEX GEN BACKEND'!D:D,0))</f>
@@ -2205,7 +2198,7 @@
       </c>
       <c r="Q10" t="str">
         <f>IF(ISNUMBER(MATCH(G10,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G10,'HEX GEN BACKEND'!I:I,0)),G10)</f>
-        <v>000100</v>
+        <v>000011</v>
       </c>
       <c r="R10" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H10,'HEX GEN BACKEND'!D:D,0))</f>
@@ -2213,11 +2206,11 @@
       </c>
       <c r="T10" t="str">
         <f t="shared" si="1"/>
-        <v>01010000001001000100010000100100</v>
+        <v>01100000100010000010010000011100</v>
       </c>
       <c r="V10" t="str">
         <f t="shared" si="2"/>
-        <v>0101</v>
+        <v>0110</v>
       </c>
       <c r="W10" t="str">
         <f t="shared" si="3"/>
@@ -2225,15 +2218,15 @@
       </c>
       <c r="X10" t="str">
         <f t="shared" si="4"/>
-        <v>0010</v>
+        <v>1000</v>
       </c>
       <c r="Y10" t="str">
         <f t="shared" si="5"/>
-        <v>0100</v>
+        <v>1000</v>
       </c>
       <c r="Z10" t="str">
         <f t="shared" si="6"/>
-        <v>0100</v>
+        <v>0010</v>
       </c>
       <c r="AA10" t="str">
         <f t="shared" si="7"/>
@@ -2241,15 +2234,15 @@
       </c>
       <c r="AB10" t="str">
         <f t="shared" si="8"/>
-        <v>0010</v>
+        <v>0001</v>
       </c>
       <c r="AC10" t="str">
         <f t="shared" si="9"/>
-        <v>0100</v>
+        <v>1100</v>
       </c>
       <c r="AE10" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V10,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AF10" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W10,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2257,15 +2250,15 @@
       </c>
       <c r="AG10" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X10,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AH10" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y10,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AI10" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z10,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AJ10" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA10,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2273,45 +2266,45 @@
       </c>
       <c r="AK10" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB10,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL10" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC10,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>C</v>
       </c>
       <c r="AN10" t="str">
         <f t="shared" si="10"/>
-        <v>50244424</v>
+        <v>6088241C</v>
       </c>
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="D11" s="27" t="s">
+      <c r="C11" s="53" t="s">
+        <v>158</v>
+      </c>
+      <c r="D11" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" s="55" t="s">
+        <v>138</v>
+      </c>
+      <c r="F11" s="56" t="s">
         <v>113</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="F11" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="G11" s="31" t="s">
-        <v>146</v>
-      </c>
-      <c r="H11" s="40" t="s">
+      <c r="G11" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="H11" s="58" t="s">
         <v>114</v>
       </c>
       <c r="I11" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>48904822</v>
+        <v>4800381A</v>
       </c>
       <c r="L11" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B11,'HEX GEN BACKEND'!A:A,0))</f>
@@ -2319,15 +2312,15 @@
       </c>
       <c r="M11" t="str">
         <f>IF(ISNUMBER(MATCH(C11,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C11,'HEX GEN BACKEND'!G:G,0)),C11)</f>
-        <v>000100</v>
+        <v>000000</v>
       </c>
       <c r="N11" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D11,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
+        <v>000</v>
       </c>
       <c r="O11" t="str">
         <f>IF(ISNUMBER(MATCH(E11,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E11,'HEX GEN BACKEND'!H:H,0)),E11)</f>
-        <v>000100</v>
+        <v>000011</v>
       </c>
       <c r="P11" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F11,'HEX GEN BACKEND'!D:D,0))</f>
@@ -2335,7 +2328,7 @@
       </c>
       <c r="Q11" t="str">
         <f>IF(ISNUMBER(MATCH(G11,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G11,'HEX GEN BACKEND'!I:I,0)),G11)</f>
-        <v>000100</v>
+        <v>000011</v>
       </c>
       <c r="R11" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H11,'HEX GEN BACKEND'!D:D,0))</f>
@@ -2343,7 +2336,7 @@
       </c>
       <c r="T11" t="str">
         <f t="shared" si="1"/>
-        <v>01001000100100000100100000100010</v>
+        <v>01001000000000000011100000011010</v>
       </c>
       <c r="V11" t="str">
         <f t="shared" si="2"/>
@@ -2355,7 +2348,7 @@
       </c>
       <c r="X11" t="str">
         <f t="shared" si="4"/>
-        <v>1001</v>
+        <v>0000</v>
       </c>
       <c r="Y11" t="str">
         <f t="shared" si="5"/>
@@ -2363,7 +2356,7 @@
       </c>
       <c r="Z11" t="str">
         <f t="shared" si="6"/>
-        <v>0100</v>
+        <v>0011</v>
       </c>
       <c r="AA11" t="str">
         <f t="shared" si="7"/>
@@ -2371,11 +2364,11 @@
       </c>
       <c r="AB11" t="str">
         <f t="shared" si="8"/>
-        <v>0010</v>
+        <v>0001</v>
       </c>
       <c r="AC11" t="str">
         <f t="shared" si="9"/>
-        <v>0010</v>
+        <v>1010</v>
       </c>
       <c r="AE11" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V11,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2387,7 +2380,7 @@
       </c>
       <c r="AG11" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X11,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AH11" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y11,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2395,7 +2388,7 @@
       </c>
       <c r="AI11" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z11,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AJ11" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA11,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2403,49 +2396,49 @@
       </c>
       <c r="AK11" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB11,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AL11" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC11,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>A</v>
       </c>
       <c r="AN11" t="str">
         <f t="shared" si="10"/>
-        <v>48904822</v>
+        <v>4800381A</v>
       </c>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="C12" s="41" t="s">
+      <c r="B12" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="C12" s="53" t="s">
         <v>132</v>
       </c>
-      <c r="D12" s="27" t="s">
+      <c r="D12" s="54" t="s">
         <v>114</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="F12" s="29" t="s">
+      <c r="E12" s="55" t="s">
+        <v>138</v>
+      </c>
+      <c r="F12" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="G12" s="57" t="s">
         <v>145</v>
       </c>
-      <c r="H12" s="40" t="s">
+      <c r="H12" s="58" t="s">
         <v>113</v>
       </c>
       <c r="I12" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>6088241C</v>
+        <v>2888341C</v>
       </c>
       <c r="L12" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B12,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01100</v>
+        <v>00101</v>
       </c>
       <c r="M12" t="str">
         <f>IF(ISNUMBER(MATCH(C12,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C12,'HEX GEN BACKEND'!G:G,0)),C12)</f>
@@ -2457,7 +2450,7 @@
       </c>
       <c r="O12" t="str">
         <f>IF(ISNUMBER(MATCH(E12,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E12,'HEX GEN BACKEND'!H:H,0)),E12)</f>
-        <v>000010</v>
+        <v>000011</v>
       </c>
       <c r="P12" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F12,'HEX GEN BACKEND'!D:D,0))</f>
@@ -2473,15 +2466,15 @@
       </c>
       <c r="T12" t="str">
         <f t="shared" si="1"/>
-        <v>01100000100010000010010000011100</v>
+        <v>00101000100010000011010000011100</v>
       </c>
       <c r="V12" t="str">
         <f t="shared" si="2"/>
-        <v>0110</v>
+        <v>0010</v>
       </c>
       <c r="W12" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="X12" t="str">
         <f t="shared" si="4"/>
@@ -2493,7 +2486,7 @@
       </c>
       <c r="Z12" t="str">
         <f t="shared" si="6"/>
-        <v>0010</v>
+        <v>0011</v>
       </c>
       <c r="AA12" t="str">
         <f t="shared" si="7"/>
@@ -2509,11 +2502,11 @@
       </c>
       <c r="AE12" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V12,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AF12" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W12,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AG12" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X12,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2525,7 +2518,7 @@
       </c>
       <c r="AI12" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z12,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AJ12" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA12,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2541,37 +2534,37 @@
       </c>
       <c r="AN12" t="str">
         <f t="shared" si="10"/>
-        <v>6088241C</v>
+        <v>2888341C</v>
       </c>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="53" t="s">
+        <v>130</v>
+      </c>
+      <c r="D13" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="E13" s="55" t="s">
+        <v>142</v>
+      </c>
+      <c r="F13" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="G13" s="57" t="s">
         <v>158</v>
       </c>
-      <c r="D13" s="27" t="s">
+      <c r="H13" s="58" t="s">
         <v>117</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F13" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="G13" s="31" t="s">
-        <v>145</v>
-      </c>
-      <c r="H13" s="40" t="s">
-        <v>114</v>
       </c>
       <c r="I13" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>4800381A</v>
+        <v>48487800</v>
       </c>
       <c r="L13" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B13,'HEX GEN BACKEND'!A:A,0))</f>
@@ -2579,15 +2572,15 @@
       </c>
       <c r="M13" t="str">
         <f>IF(ISNUMBER(MATCH(C13,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C13,'HEX GEN BACKEND'!G:G,0)),C13)</f>
-        <v>000000</v>
+        <v>000010</v>
       </c>
       <c r="N13" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D13,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
+        <v>010</v>
       </c>
       <c r="O13" t="str">
         <f>IF(ISNUMBER(MATCH(E13,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E13,'HEX GEN BACKEND'!H:H,0)),E13)</f>
-        <v>000011</v>
+        <v>000111</v>
       </c>
       <c r="P13" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F13,'HEX GEN BACKEND'!D:D,0))</f>
@@ -2595,15 +2588,15 @@
       </c>
       <c r="Q13" t="str">
         <f>IF(ISNUMBER(MATCH(G13,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G13,'HEX GEN BACKEND'!I:I,0)),G13)</f>
-        <v>000011</v>
+        <v>000000</v>
       </c>
       <c r="R13" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H13,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
+        <v>000</v>
       </c>
       <c r="T13" t="str">
         <f t="shared" si="1"/>
-        <v>01001000000000000011100000011010</v>
+        <v>01001000010010000111100000000000</v>
       </c>
       <c r="V13" t="str">
         <f t="shared" si="2"/>
@@ -2615,15 +2608,15 @@
       </c>
       <c r="X13" t="str">
         <f t="shared" si="4"/>
-        <v>0000</v>
+        <v>0100</v>
       </c>
       <c r="Y13" t="str">
         <f t="shared" si="5"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="Z13" t="str">
         <f t="shared" si="6"/>
-        <v>0011</v>
+        <v>0111</v>
       </c>
       <c r="AA13" t="str">
         <f t="shared" si="7"/>
@@ -2631,11 +2624,11 @@
       </c>
       <c r="AB13" t="str">
         <f t="shared" si="8"/>
-        <v>0001</v>
+        <v>0000</v>
       </c>
       <c r="AC13" t="str">
         <f t="shared" si="9"/>
-        <v>1010</v>
+        <v>0000</v>
       </c>
       <c r="AE13" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V13,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2647,15 +2640,15 @@
       </c>
       <c r="AG13" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X13,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AH13" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y13,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AI13" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z13,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AJ13" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA13,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2663,61 +2656,61 @@
       </c>
       <c r="AK13" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB13,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL13" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC13,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>A</v>
+        <v>0</v>
       </c>
       <c r="AN13" t="str">
         <f t="shared" si="10"/>
-        <v>4800381A</v>
+        <v>48487800</v>
       </c>
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="B14" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="C14" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="D14" s="27" t="s">
+      <c r="B14" s="52" t="s">
+        <v>105</v>
+      </c>
+      <c r="C14" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="E14" s="55" t="s">
+        <v>142</v>
+      </c>
+      <c r="F14" s="56" t="s">
         <v>114</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F14" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="G14" s="31" t="s">
-        <v>145</v>
-      </c>
-      <c r="H14" s="40" t="s">
+      <c r="G14" s="57" t="s">
+        <v>148</v>
+      </c>
+      <c r="H14" s="58" t="s">
         <v>113</v>
       </c>
       <c r="I14" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>2888341C</v>
+        <v>50247434</v>
       </c>
       <c r="L14" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B14,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>00101</v>
+        <v>01010</v>
       </c>
       <c r="M14" t="str">
         <f>IF(ISNUMBER(MATCH(C14,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C14,'HEX GEN BACKEND'!G:G,0)),C14)</f>
-        <v>000100</v>
+        <v>000001</v>
       </c>
       <c r="N14" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D14,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
+        <v>001</v>
       </c>
       <c r="O14" t="str">
         <f>IF(ISNUMBER(MATCH(E14,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E14,'HEX GEN BACKEND'!H:H,0)),E14)</f>
-        <v>000011</v>
+        <v>000111</v>
       </c>
       <c r="P14" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F14,'HEX GEN BACKEND'!D:D,0))</f>
@@ -2725,7 +2718,7 @@
       </c>
       <c r="Q14" t="str">
         <f>IF(ISNUMBER(MATCH(G14,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G14,'HEX GEN BACKEND'!I:I,0)),G14)</f>
-        <v>000011</v>
+        <v>000110</v>
       </c>
       <c r="R14" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H14,'HEX GEN BACKEND'!D:D,0))</f>
@@ -2733,27 +2726,27 @@
       </c>
       <c r="T14" t="str">
         <f t="shared" si="1"/>
-        <v>00101000100010000011010000011100</v>
+        <v>01010000001001000111010000110100</v>
       </c>
       <c r="V14" t="str">
         <f t="shared" si="2"/>
-        <v>0010</v>
+        <v>0101</v>
       </c>
       <c r="W14" t="str">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="X14" t="str">
         <f t="shared" si="4"/>
-        <v>1000</v>
+        <v>0010</v>
       </c>
       <c r="Y14" t="str">
         <f t="shared" si="5"/>
-        <v>1000</v>
+        <v>0100</v>
       </c>
       <c r="Z14" t="str">
         <f t="shared" si="6"/>
-        <v>0011</v>
+        <v>0111</v>
       </c>
       <c r="AA14" t="str">
         <f t="shared" si="7"/>
@@ -2761,31 +2754,31 @@
       </c>
       <c r="AB14" t="str">
         <f t="shared" si="8"/>
-        <v>0001</v>
+        <v>0011</v>
       </c>
       <c r="AC14" t="str">
         <f t="shared" si="9"/>
-        <v>1100</v>
+        <v>0100</v>
       </c>
       <c r="AE14" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V14,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AF14" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W14,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AG14" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X14,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AH14" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y14,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="AI14" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z14,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AJ14" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA14,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2793,45 +2786,45 @@
       </c>
       <c r="AK14" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB14,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AL14" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC14,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>C</v>
+        <v>4</v>
       </c>
       <c r="AN14" t="str">
         <f t="shared" si="10"/>
-        <v>2888341C</v>
+        <v>50247434</v>
       </c>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="53" t="s">
         <v>130</v>
       </c>
-      <c r="D15" s="27" t="s">
+      <c r="D15" s="54" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="55" t="s">
+        <v>158</v>
+      </c>
+      <c r="F15" s="56" t="s">
+        <v>117</v>
+      </c>
+      <c r="G15" s="57" t="s">
+        <v>148</v>
+      </c>
+      <c r="H15" s="58" t="s">
         <v>114</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="F15" s="29" t="s">
-        <v>113</v>
-      </c>
-      <c r="G15" s="31" t="s">
-        <v>158</v>
-      </c>
-      <c r="H15" s="40" t="s">
-        <v>117</v>
       </c>
       <c r="I15" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>48487800</v>
+        <v>48500032</v>
       </c>
       <c r="L15" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B15,'HEX GEN BACKEND'!A:A,0))</f>
@@ -2843,27 +2836,27 @@
       </c>
       <c r="N15" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D15,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
+        <v>100</v>
       </c>
       <c r="O15" t="str">
         <f>IF(ISNUMBER(MATCH(E15,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E15,'HEX GEN BACKEND'!H:H,0)),E15)</f>
-        <v>000111</v>
+        <v>000000</v>
       </c>
       <c r="P15" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F15,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
+        <v>000</v>
       </c>
       <c r="Q15" t="str">
         <f>IF(ISNUMBER(MATCH(G15,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G15,'HEX GEN BACKEND'!I:I,0)),G15)</f>
-        <v>000000</v>
+        <v>000110</v>
       </c>
       <c r="R15" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H15,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
+        <v>010</v>
       </c>
       <c r="T15" t="str">
         <f t="shared" si="1"/>
-        <v>01001000010010000111100000000000</v>
+        <v>01001000010100000000000000110010</v>
       </c>
       <c r="V15" t="str">
         <f t="shared" si="2"/>
@@ -2875,27 +2868,27 @@
       </c>
       <c r="X15" t="str">
         <f t="shared" si="4"/>
-        <v>0100</v>
+        <v>0101</v>
       </c>
       <c r="Y15" t="str">
         <f t="shared" si="5"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="Z15" t="str">
         <f t="shared" si="6"/>
-        <v>0111</v>
+        <v>0000</v>
       </c>
       <c r="AA15" t="str">
         <f t="shared" si="7"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="AB15" t="str">
         <f t="shared" si="8"/>
-        <v>0000</v>
+        <v>0011</v>
       </c>
       <c r="AC15" t="str">
         <f t="shared" si="9"/>
-        <v>0000</v>
+        <v>0010</v>
       </c>
       <c r="AE15" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V15,'HEX GEN BACKEND'!L:L,0))</f>
@@ -2907,73 +2900,73 @@
       </c>
       <c r="AG15" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X15,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH15" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y15,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AI15" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z15,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AJ15" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA15,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AK15" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB15,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL15" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC15,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN15" t="str">
         <f t="shared" si="10"/>
-        <v>48487800</v>
+        <v>48500032</v>
       </c>
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="25" t="s">
-        <v>105</v>
-      </c>
-      <c r="C16" s="41" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="E16" s="10" t="s">
+      <c r="B16" s="52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="53" t="s">
+        <v>158</v>
+      </c>
+      <c r="D16" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" s="55" t="s">
         <v>142</v>
       </c>
-      <c r="F16" s="29" t="s">
+      <c r="F16" s="56" t="s">
+        <v>113</v>
+      </c>
+      <c r="G16" s="57" t="s">
+        <v>149</v>
+      </c>
+      <c r="H16" s="58" t="s">
         <v>114</v>
-      </c>
-      <c r="G16" s="31" t="s">
-        <v>148</v>
-      </c>
-      <c r="H16" s="40" t="s">
-        <v>113</v>
       </c>
       <c r="I16" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>50247434</v>
+        <v>4800783A</v>
       </c>
       <c r="L16" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B16,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01010</v>
+        <v>01001</v>
       </c>
       <c r="M16" t="str">
         <f>IF(ISNUMBER(MATCH(C16,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C16,'HEX GEN BACKEND'!G:G,0)),C16)</f>
-        <v>000001</v>
+        <v>000000</v>
       </c>
       <c r="N16" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D16,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>001</v>
+        <v>000</v>
       </c>
       <c r="O16" t="str">
         <f>IF(ISNUMBER(MATCH(E16,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E16,'HEX GEN BACKEND'!H:H,0)),E16)</f>
@@ -2981,35 +2974,35 @@
       </c>
       <c r="P16" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F16,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
+        <v>100</v>
       </c>
       <c r="Q16" t="str">
         <f>IF(ISNUMBER(MATCH(G16,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G16,'HEX GEN BACKEND'!I:I,0)),G16)</f>
-        <v>000110</v>
+        <v>000111</v>
       </c>
       <c r="R16" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H16,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
+        <v>010</v>
       </c>
       <c r="T16" t="str">
         <f t="shared" si="1"/>
-        <v>01010000001001000111010000110100</v>
+        <v>01001000000000000111100000111010</v>
       </c>
       <c r="V16" t="str">
         <f t="shared" si="2"/>
-        <v>0101</v>
+        <v>0100</v>
       </c>
       <c r="W16" t="str">
         <f t="shared" si="3"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="X16" t="str">
         <f t="shared" si="4"/>
-        <v>0010</v>
+        <v>0000</v>
       </c>
       <c r="Y16" t="str">
         <f t="shared" si="5"/>
-        <v>0100</v>
+        <v>0000</v>
       </c>
       <c r="Z16" t="str">
         <f t="shared" si="6"/>
@@ -3017,7 +3010,7 @@
       </c>
       <c r="AA16" t="str">
         <f t="shared" si="7"/>
-        <v>0100</v>
+        <v>1000</v>
       </c>
       <c r="AB16" t="str">
         <f t="shared" si="8"/>
@@ -3025,23 +3018,23 @@
       </c>
       <c r="AC16" t="str">
         <f t="shared" si="9"/>
-        <v>0100</v>
+        <v>1010</v>
       </c>
       <c r="AE16" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V16,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AF16" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W16,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AG16" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X16,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AH16" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y16,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AI16" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z16,'HEX GEN BACKEND'!L:L,0))</f>
@@ -3049,7 +3042,7 @@
       </c>
       <c r="AJ16" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA16,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="AK16" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB16,'HEX GEN BACKEND'!L:L,0))</f>
@@ -3057,65 +3050,65 @@
       </c>
       <c r="AL16" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC16,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>A</v>
       </c>
       <c r="AN16" t="str">
         <f t="shared" si="10"/>
-        <v>50247434</v>
+        <v>4800783A</v>
       </c>
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A17" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="B17" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="F17" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="G17" s="31" t="s">
-        <v>148</v>
-      </c>
-      <c r="H17" s="40" t="s">
+      <c r="B17" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="55" t="s">
+        <v>75</v>
+      </c>
+      <c r="F17" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="G17" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="H17" s="58" t="s">
         <v>114</v>
       </c>
       <c r="I17" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>48500032</v>
+        <v>3225021A</v>
       </c>
       <c r="L17" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B17,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01001</v>
+        <v>00110</v>
       </c>
       <c r="M17" t="str">
         <f>IF(ISNUMBER(MATCH(C17,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C17,'HEX GEN BACKEND'!G:G,0)),C17)</f>
-        <v>000010</v>
+        <v>010001</v>
       </c>
       <c r="N17" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D17,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
+        <v>001</v>
       </c>
       <c r="O17" t="str">
         <f>IF(ISNUMBER(MATCH(E17,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E17,'HEX GEN BACKEND'!H:H,0)),E17)</f>
-        <v>000000</v>
+        <v>010000</v>
       </c>
       <c r="P17" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F17,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
+        <v>001</v>
       </c>
       <c r="Q17" t="str">
         <f>IF(ISNUMBER(MATCH(G17,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G17,'HEX GEN BACKEND'!I:I,0)),G17)</f>
-        <v>000110</v>
+        <v>000011</v>
       </c>
       <c r="R17" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H17,'HEX GEN BACKEND'!D:D,0))</f>
@@ -3123,23 +3116,23 @@
       </c>
       <c r="T17" t="str">
         <f t="shared" si="1"/>
-        <v>01001000010100000000000000110010</v>
+        <v>00110010001001010000001000011010</v>
       </c>
       <c r="V17" t="str">
         <f t="shared" si="2"/>
-        <v>0100</v>
+        <v>0011</v>
       </c>
       <c r="W17" t="str">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>0010</v>
       </c>
       <c r="X17" t="str">
         <f t="shared" si="4"/>
-        <v>0101</v>
+        <v>0010</v>
       </c>
       <c r="Y17" t="str">
         <f t="shared" si="5"/>
-        <v>0000</v>
+        <v>0101</v>
       </c>
       <c r="Z17" t="str">
         <f t="shared" si="6"/>
@@ -3147,31 +3140,31 @@
       </c>
       <c r="AA17" t="str">
         <f t="shared" si="7"/>
-        <v>0000</v>
+        <v>0010</v>
       </c>
       <c r="AB17" t="str">
         <f t="shared" si="8"/>
-        <v>0011</v>
+        <v>0001</v>
       </c>
       <c r="AC17" t="str">
         <f t="shared" si="9"/>
-        <v>0010</v>
+        <v>1010</v>
       </c>
       <c r="AE17" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AF17" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="AG17" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AH17" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI17" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z17,'HEX GEN BACKEND'!L:L,0))</f>
@@ -3179,61 +3172,61 @@
       </c>
       <c r="AJ17" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AK17" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AL17" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC17,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>A</v>
       </c>
       <c r="AN17" t="str">
         <f t="shared" si="10"/>
-        <v>48500032</v>
+        <v>3225021A</v>
       </c>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A18" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="41" t="s">
-        <v>158</v>
-      </c>
-      <c r="D18" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="E18" s="10" t="s">
+      <c r="B18" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="C18" s="53" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="E18" s="55" t="s">
         <v>142</v>
       </c>
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="56" t="s">
+        <v>114</v>
+      </c>
+      <c r="G18" s="57" t="s">
+        <v>149</v>
+      </c>
+      <c r="H18" s="58" t="s">
         <v>113</v>
-      </c>
-      <c r="G18" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="H18" s="40" t="s">
-        <v>114</v>
       </c>
       <c r="I18" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>4800783A</v>
+        <v>0848743C</v>
       </c>
       <c r="L18" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B18,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>01001</v>
+        <v>00001</v>
       </c>
       <c r="M18" t="str">
         <f>IF(ISNUMBER(MATCH(C18,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C18,'HEX GEN BACKEND'!G:G,0)),C18)</f>
-        <v>000000</v>
+        <v>000010</v>
       </c>
       <c r="N18" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D18,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
+        <v>010</v>
       </c>
       <c r="O18" t="str">
         <f>IF(ISNUMBER(MATCH(E18,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E18,'HEX GEN BACKEND'!H:H,0)),E18)</f>
@@ -3241,7 +3234,7 @@
       </c>
       <c r="P18" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F18,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
+        <v>010</v>
       </c>
       <c r="Q18" t="str">
         <f>IF(ISNUMBER(MATCH(G18,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G18,'HEX GEN BACKEND'!I:I,0)),G18)</f>
@@ -3249,15 +3242,15 @@
       </c>
       <c r="R18" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H18,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
+        <v>100</v>
       </c>
       <c r="T18" t="str">
         <f t="shared" si="1"/>
-        <v>01001000000000000111100000111010</v>
+        <v>00001000010010000111010000111100</v>
       </c>
       <c r="V18" t="str">
         <f t="shared" si="2"/>
-        <v>0100</v>
+        <v>0000</v>
       </c>
       <c r="W18" t="str">
         <f t="shared" si="3"/>
@@ -3265,11 +3258,11 @@
       </c>
       <c r="X18" t="str">
         <f t="shared" si="4"/>
-        <v>0000</v>
+        <v>0100</v>
       </c>
       <c r="Y18" t="str">
         <f t="shared" si="5"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="Z18" t="str">
         <f t="shared" si="6"/>
@@ -3277,7 +3270,7 @@
       </c>
       <c r="AA18" t="str">
         <f t="shared" si="7"/>
-        <v>1000</v>
+        <v>0100</v>
       </c>
       <c r="AB18" t="str">
         <f t="shared" si="8"/>
@@ -3285,11 +3278,11 @@
       </c>
       <c r="AC18" t="str">
         <f t="shared" si="9"/>
-        <v>1010</v>
+        <v>1100</v>
       </c>
       <c r="AE18" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V18,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AF18" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W18,'HEX GEN BACKEND'!L:L,0))</f>
@@ -3297,11 +3290,11 @@
       </c>
       <c r="AG18" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X18,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AH18" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y18,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AI18" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z18,'HEX GEN BACKEND'!L:L,0))</f>
@@ -3309,7 +3302,7 @@
       </c>
       <c r="AJ18" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA18,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="AK18" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB18,'HEX GEN BACKEND'!L:L,0))</f>
@@ -3317,57 +3310,57 @@
       </c>
       <c r="AL18" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC18,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>A</v>
+        <v>C</v>
       </c>
       <c r="AN18" t="str">
         <f t="shared" si="10"/>
-        <v>4800783A</v>
+        <v>0848743C</v>
       </c>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A19" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="B19" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19" s="41" t="s">
-        <v>78</v>
-      </c>
-      <c r="D19" s="27" t="s">
+      <c r="B19" s="52" t="s">
+        <v>124</v>
+      </c>
+      <c r="C19" s="53" t="s">
+        <v>132</v>
+      </c>
+      <c r="D19" s="54" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="55" t="s">
+        <v>162</v>
+      </c>
+      <c r="F19" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="F19" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="G19" s="31" t="s">
-        <v>145</v>
-      </c>
-      <c r="H19" s="40" t="s">
-        <v>114</v>
+      <c r="G19" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="H19" s="58" t="s">
+        <v>113</v>
       </c>
       <c r="I19" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>3265221A</v>
+        <v>288A022C</v>
       </c>
       <c r="L19" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B19,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>00110</v>
+        <v>00101</v>
       </c>
       <c r="M19" t="str">
         <f>IF(ISNUMBER(MATCH(C19,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C19,'HEX GEN BACKEND'!G:G,0)),C19)</f>
-        <v>010011</v>
+        <v>000100</v>
       </c>
       <c r="N19" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D19,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>001</v>
+        <v>010</v>
       </c>
       <c r="O19" t="str">
         <f>IF(ISNUMBER(MATCH(E19,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E19,'HEX GEN BACKEND'!H:H,0)),E19)</f>
-        <v>010010</v>
+        <v>100000</v>
       </c>
       <c r="P19" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F19,'HEX GEN BACKEND'!D:D,0))</f>
@@ -3375,35 +3368,35 @@
       </c>
       <c r="Q19" t="str">
         <f>IF(ISNUMBER(MATCH(G19,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G19,'HEX GEN BACKEND'!I:I,0)),G19)</f>
-        <v>000011</v>
+        <v>000101</v>
       </c>
       <c r="R19" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H19,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
+        <v>100</v>
       </c>
       <c r="T19" t="str">
         <f t="shared" si="1"/>
-        <v>00110010011001010010001000011010</v>
+        <v>00101000100010100000001000101100</v>
       </c>
       <c r="V19" t="str">
         <f t="shared" si="2"/>
-        <v>0011</v>
+        <v>0010</v>
       </c>
       <c r="W19" t="str">
         <f t="shared" si="3"/>
-        <v>0010</v>
+        <v>1000</v>
       </c>
       <c r="X19" t="str">
         <f t="shared" si="4"/>
-        <v>0110</v>
+        <v>1000</v>
       </c>
       <c r="Y19" t="str">
         <f t="shared" si="5"/>
-        <v>0101</v>
+        <v>1010</v>
       </c>
       <c r="Z19" t="str">
         <f t="shared" si="6"/>
-        <v>0010</v>
+        <v>0000</v>
       </c>
       <c r="AA19" t="str">
         <f t="shared" si="7"/>
@@ -3411,31 +3404,31 @@
       </c>
       <c r="AB19" t="str">
         <f t="shared" si="8"/>
-        <v>0001</v>
+        <v>0010</v>
       </c>
       <c r="AC19" t="str">
         <f t="shared" si="9"/>
-        <v>1010</v>
+        <v>1100</v>
       </c>
       <c r="AE19" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V19,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AF19" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W19,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AG19" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X19,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="AH19" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y19,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>5</v>
+        <v>A</v>
       </c>
       <c r="AI19" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z19,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AJ19" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA19,'HEX GEN BACKEND'!L:L,0))</f>
@@ -3443,223 +3436,223 @@
       </c>
       <c r="AK19" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB19,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL19" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC19,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>A</v>
+        <v>C</v>
       </c>
       <c r="AN19" t="str">
         <f t="shared" si="10"/>
-        <v>3265221A</v>
+        <v>288A022C</v>
       </c>
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A20" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="B20" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="41" t="s">
-        <v>130</v>
-      </c>
-      <c r="D20" s="27" t="s">
+      <c r="B20" s="52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="53" t="s">
+        <v>36</v>
+      </c>
+      <c r="D20" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="E20" s="55" t="s">
+        <v>78</v>
+      </c>
+      <c r="F20" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="G20" s="57" t="s">
+        <v>147</v>
+      </c>
+      <c r="H20" s="58" t="s">
         <v>114</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="F20" s="29" t="s">
-        <v>114</v>
-      </c>
-      <c r="G20" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="H20" s="40" t="s">
-        <v>113</v>
       </c>
       <c r="I20" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>0848743C</v>
+        <v>30C5322A</v>
       </c>
       <c r="L20" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B20,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>00001</v>
+        <v>00110</v>
       </c>
       <c r="M20" t="str">
         <f>IF(ISNUMBER(MATCH(C20,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C20,'HEX GEN BACKEND'!G:G,0)),C20)</f>
-        <v>000010</v>
+        <v>000110</v>
       </c>
       <c r="N20" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D20,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
+        <v>001</v>
       </c>
       <c r="O20" t="str">
         <f>IF(ISNUMBER(MATCH(E20,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E20,'HEX GEN BACKEND'!H:H,0)),E20)</f>
-        <v>000111</v>
+        <v>010011</v>
       </c>
       <c r="P20" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F20,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
+        <v>001</v>
       </c>
       <c r="Q20" t="str">
         <f>IF(ISNUMBER(MATCH(G20,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G20,'HEX GEN BACKEND'!I:I,0)),G20)</f>
-        <v>000111</v>
+        <v>000101</v>
       </c>
       <c r="R20" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H20,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
+        <v>010</v>
       </c>
       <c r="T20" t="str">
         <f t="shared" si="1"/>
-        <v>00001000010010000111010000111100</v>
+        <v>00110000110001010011001000101010</v>
       </c>
       <c r="V20" t="str">
         <f t="shared" si="2"/>
-        <v>0000</v>
+        <v>0011</v>
       </c>
       <c r="W20" t="str">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="X20" t="str">
         <f t="shared" si="4"/>
-        <v>0100</v>
+        <v>1100</v>
       </c>
       <c r="Y20" t="str">
         <f t="shared" si="5"/>
-        <v>1000</v>
+        <v>0101</v>
       </c>
       <c r="Z20" t="str">
         <f t="shared" si="6"/>
-        <v>0111</v>
+        <v>0011</v>
       </c>
       <c r="AA20" t="str">
         <f t="shared" si="7"/>
-        <v>0100</v>
+        <v>0010</v>
       </c>
       <c r="AB20" t="str">
         <f t="shared" si="8"/>
-        <v>0011</v>
+        <v>0010</v>
       </c>
       <c r="AC20" t="str">
         <f t="shared" si="9"/>
-        <v>1100</v>
+        <v>1010</v>
       </c>
       <c r="AE20" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AF20" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AG20" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>C</v>
       </c>
       <c r="AH20" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="AI20" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="AJ20" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AK20" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AL20" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC20,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="AN20" t="str">
         <f t="shared" si="10"/>
-        <v>0848743C</v>
+        <v>30C5322A</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="B21" s="25" t="s">
-        <v>124</v>
-      </c>
-      <c r="C21" s="41" t="s">
-        <v>132</v>
-      </c>
-      <c r="D21" s="27" t="s">
+      <c r="B21" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="C21" s="53" t="s">
+        <v>158</v>
+      </c>
+      <c r="D21" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="E21" s="55" t="s">
+        <v>158</v>
+      </c>
+      <c r="F21" s="56" t="s">
+        <v>117</v>
+      </c>
+      <c r="G21" s="57" t="s">
+        <v>149</v>
+      </c>
+      <c r="H21" s="58" t="s">
         <v>114</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="F21" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="G21" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="H21" s="40" t="s">
-        <v>113</v>
       </c>
       <c r="I21" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>288A022C</v>
+        <v>C000003A</v>
       </c>
       <c r="L21" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B21,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>00101</v>
+        <v>11000</v>
       </c>
       <c r="M21" t="str">
         <f>IF(ISNUMBER(MATCH(C21,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C21,'HEX GEN BACKEND'!G:G,0)),C21)</f>
-        <v>000100</v>
+        <v>000000</v>
       </c>
       <c r="N21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D21,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
+        <v>000</v>
       </c>
       <c r="O21" t="str">
         <f>IF(ISNUMBER(MATCH(E21,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E21,'HEX GEN BACKEND'!H:H,0)),E21)</f>
-        <v>100000</v>
+        <v>000000</v>
       </c>
       <c r="P21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F21,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>001</v>
+        <v>000</v>
       </c>
       <c r="Q21" t="str">
         <f>IF(ISNUMBER(MATCH(G21,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G21,'HEX GEN BACKEND'!I:I,0)),G21)</f>
-        <v>000101</v>
+        <v>000111</v>
       </c>
       <c r="R21" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H21,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
+        <v>010</v>
       </c>
       <c r="T21" t="str">
         <f t="shared" si="1"/>
-        <v>00101000100010100000001000101100</v>
+        <v>11000000000000000000000000111010</v>
       </c>
       <c r="V21" t="str">
         <f t="shared" si="2"/>
-        <v>0010</v>
+        <v>1100</v>
       </c>
       <c r="W21" t="str">
         <f t="shared" si="3"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="X21" t="str">
         <f t="shared" si="4"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="Y21" t="str">
         <f t="shared" si="5"/>
-        <v>1010</v>
+        <v>0000</v>
       </c>
       <c r="Z21" t="str">
         <f t="shared" si="6"/>
@@ -3667,31 +3660,31 @@
       </c>
       <c r="AA21" t="str">
         <f t="shared" si="7"/>
-        <v>0010</v>
+        <v>0000</v>
       </c>
       <c r="AB21" t="str">
         <f t="shared" si="8"/>
-        <v>0010</v>
+        <v>0011</v>
       </c>
       <c r="AC21" t="str">
         <f t="shared" si="9"/>
-        <v>1100</v>
+        <v>1010</v>
       </c>
       <c r="AE21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>C</v>
       </c>
       <c r="AF21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AG21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AH21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>A</v>
+        <v>0</v>
       </c>
       <c r="AI21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z21,'HEX GEN BACKEND'!L:L,0))</f>
@@ -3699,279 +3692,251 @@
       </c>
       <c r="AJ21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AK21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL21" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC21,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="AN21" t="str">
         <f t="shared" si="10"/>
-        <v>288A022C</v>
+        <v>C000003A</v>
       </c>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A22" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="25" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="41" t="s">
-        <v>38</v>
-      </c>
-      <c r="D22" s="27" t="s">
-        <v>115</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>80</v>
-      </c>
-      <c r="F22" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="G22" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="H22" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="I22" s="25" t="str">
+      <c r="B22" s="25"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="25" t="e">
         <f t="shared" si="0"/>
-        <v>3105522A</v>
-      </c>
-      <c r="L22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L22" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B22,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>00110</v>
-      </c>
-      <c r="M22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M22">
         <f>IF(ISNUMBER(MATCH(C22,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C22,'HEX GEN BACKEND'!G:G,0)),C22)</f>
-        <v>001000</v>
-      </c>
-      <c r="N22" t="str">
+        <v>0</v>
+      </c>
+      <c r="N22" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D22,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>001</v>
-      </c>
-      <c r="O22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O22">
         <f>IF(ISNUMBER(MATCH(E22,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E22,'HEX GEN BACKEND'!H:H,0)),E22)</f>
-        <v>010101</v>
-      </c>
-      <c r="P22" t="str">
+        <v>0</v>
+      </c>
+      <c r="P22" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F22,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>001</v>
-      </c>
-      <c r="Q22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Q22">
         <f>IF(ISNUMBER(MATCH(G22,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G22,'HEX GEN BACKEND'!I:I,0)),G22)</f>
-        <v>000101</v>
-      </c>
-      <c r="R22" t="str">
+        <v>0</v>
+      </c>
+      <c r="R22" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H22,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="T22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="T22" t="e">
         <f t="shared" si="1"/>
-        <v>00110001000001010101001000101010</v>
-      </c>
-      <c r="V22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="V22" t="e">
         <f t="shared" si="2"/>
-        <v>0011</v>
-      </c>
-      <c r="W22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W22" t="e">
         <f t="shared" si="3"/>
-        <v>0001</v>
-      </c>
-      <c r="X22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X22" t="e">
         <f t="shared" si="4"/>
-        <v>0000</v>
-      </c>
-      <c r="Y22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y22" t="e">
         <f t="shared" si="5"/>
-        <v>0101</v>
-      </c>
-      <c r="Z22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z22" t="e">
         <f t="shared" si="6"/>
-        <v>0101</v>
-      </c>
-      <c r="AA22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA22" t="e">
         <f t="shared" si="7"/>
-        <v>0010</v>
-      </c>
-      <c r="AB22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB22" t="e">
         <f t="shared" si="8"/>
-        <v>0010</v>
-      </c>
-      <c r="AC22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC22" t="e">
         <f t="shared" si="9"/>
-        <v>1010</v>
-      </c>
-      <c r="AE22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AE22" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
-      </c>
-      <c r="AF22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF22" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>1</v>
-      </c>
-      <c r="AG22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG22" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AH22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH22" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>5</v>
-      </c>
-      <c r="AI22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI22" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>5</v>
-      </c>
-      <c r="AJ22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ22" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
-      </c>
-      <c r="AK22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK22" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>2</v>
-      </c>
-      <c r="AL22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL22" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC22,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>A</v>
-      </c>
-      <c r="AN22" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AN22" t="e">
         <f t="shared" si="10"/>
-        <v>3105522A</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A23" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="B23" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="C23" s="41" t="s">
-        <v>158</v>
-      </c>
-      <c r="D23" s="27" t="s">
-        <v>117</v>
-      </c>
-      <c r="E23" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="F23" s="29" t="s">
-        <v>117</v>
-      </c>
-      <c r="G23" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="H23" s="40" t="s">
-        <v>114</v>
-      </c>
-      <c r="I23" s="25" t="str">
+      <c r="B23" s="25"/>
+      <c r="C23" s="41"/>
+      <c r="D23" s="27"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="25" t="e">
         <f t="shared" si="0"/>
-        <v>C000003A</v>
-      </c>
-      <c r="L23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="L23" t="e">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B23,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>11000</v>
-      </c>
-      <c r="M23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="M23">
         <f>IF(ISNUMBER(MATCH(C23,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C23,'HEX GEN BACKEND'!G:G,0)),C23)</f>
-        <v>000000</v>
-      </c>
-      <c r="N23" t="str">
+        <v>0</v>
+      </c>
+      <c r="N23" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D23,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
-      </c>
-      <c r="O23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="O23">
         <f>IF(ISNUMBER(MATCH(E23,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E23,'HEX GEN BACKEND'!H:H,0)),E23)</f>
-        <v>000000</v>
-      </c>
-      <c r="P23" t="str">
+        <v>0</v>
+      </c>
+      <c r="P23" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F23,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
-      </c>
-      <c r="Q23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Q23">
         <f>IF(ISNUMBER(MATCH(G23,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G23,'HEX GEN BACKEND'!I:I,0)),G23)</f>
-        <v>000111</v>
-      </c>
-      <c r="R23" t="str">
+        <v>0</v>
+      </c>
+      <c r="R23" t="e">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H23,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
-      </c>
-      <c r="T23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="T23" t="e">
         <f t="shared" si="1"/>
-        <v>11000000000000000000000000111010</v>
-      </c>
-      <c r="V23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="V23" t="e">
         <f t="shared" si="2"/>
-        <v>1100</v>
-      </c>
-      <c r="W23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="W23" t="e">
         <f t="shared" si="3"/>
-        <v>0000</v>
-      </c>
-      <c r="X23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="X23" t="e">
         <f t="shared" si="4"/>
-        <v>0000</v>
-      </c>
-      <c r="Y23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Y23" t="e">
         <f t="shared" si="5"/>
-        <v>0000</v>
-      </c>
-      <c r="Z23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="Z23" t="e">
         <f t="shared" si="6"/>
-        <v>0000</v>
-      </c>
-      <c r="AA23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AA23" t="e">
         <f t="shared" si="7"/>
-        <v>0000</v>
-      </c>
-      <c r="AB23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AB23" t="e">
         <f t="shared" si="8"/>
-        <v>0011</v>
-      </c>
-      <c r="AC23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AC23" t="e">
         <f t="shared" si="9"/>
-        <v>1010</v>
-      </c>
-      <c r="AE23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AE23" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>C</v>
-      </c>
-      <c r="AF23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AF23" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AG23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AG23" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AH23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AH23" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AI23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AI23" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AJ23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AJ23" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
-      </c>
-      <c r="AK23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AK23" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
-      </c>
-      <c r="AL23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AL23" t="e">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC23,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>A</v>
-      </c>
-      <c r="AN23" t="str">
+        <v>#N/A</v>
+      </c>
+      <c r="AN23" t="e">
         <f t="shared" si="10"/>
-        <v>C000003A</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.25">
@@ -12955,7 +12920,7 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="3">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'HEX GEN BACKEND'!$A:$A</xm:f>
@@ -12966,13 +12931,13 @@
           <x14:formula1>
             <xm:f>'HEX GEN BACKEND'!$D$1:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>D24:D53 F24:F53 D2:D20 H2:H20 F2:F20 F22 D22 H22 H24:H53</xm:sqref>
+          <xm:sqref>D24:D53 F24:F53 F2:F18 D2:D18 H24:H53 F22 D22 H22 H2:H18 F20 D20 H20</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>'HEX GEN BACKEND'!$D:$D</xm:f>
           </x14:formula1>
-          <xm:sqref>D54:D101 F54:F101 H54:H101 D21 F21 H21 D23 F23 H23</xm:sqref>
+          <xm:sqref>D54:D101 F54:F101 H54:H101 D23 F23 H23 D21 F21 H21 D19 F19 H19</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
added a square minus b square
</commit_message>
<xml_diff>
--- a/Instructions/Binary Instructions.xlsx
+++ b/Instructions/Binary Instructions.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="618" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="215">
   <si>
     <t>0001</t>
   </si>
@@ -1126,7 +1126,7 @@
   <dimension ref="A1:AN101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5605,16 +5605,16 @@
         <v>9</v>
       </c>
       <c r="C36" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="D36" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="E36" s="42" t="s">
         <v>158</v>
       </c>
-      <c r="D36" s="41" t="s">
+      <c r="F36" s="43" t="s">
         <v>117</v>
-      </c>
-      <c r="E36" s="42" t="s">
-        <v>138</v>
-      </c>
-      <c r="F36" s="43" t="s">
-        <v>113</v>
       </c>
       <c r="G36" s="44" t="s">
         <v>149</v>
@@ -5624,7 +5624,7 @@
       </c>
       <c r="I36" s="49" t="str">
         <f t="shared" si="20"/>
-        <v>4800383A</v>
+        <v>48B0003A</v>
       </c>
       <c r="L36" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B36,'HEX GEN BACKEND'!A:A,0))</f>
@@ -5632,19 +5632,19 @@
       </c>
       <c r="M36" s="47" t="str">
         <f>IF(ISNUMBER(MATCH(C36,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C36,'HEX GEN BACKEND'!G:G,0)),C36)</f>
-        <v>000000</v>
+        <v>000101</v>
       </c>
       <c r="N36" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D36,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
+        <v>100</v>
       </c>
       <c r="O36" s="47" t="str">
         <f>IF(ISNUMBER(MATCH(E36,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E36,'HEX GEN BACKEND'!H:H,0)),E36)</f>
-        <v>000011</v>
+        <v>000000</v>
       </c>
       <c r="P36" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F36,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>100</v>
+        <v>000</v>
       </c>
       <c r="Q36" s="47" t="str">
         <f>IF(ISNUMBER(MATCH(G36,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G36,'HEX GEN BACKEND'!I:I,0)),G36)</f>
@@ -5656,7 +5656,7 @@
       </c>
       <c r="T36" s="47" t="str">
         <f t="shared" si="11"/>
-        <v>01001000000000000011100000111010</v>
+        <v>01001000101100000000000000111010</v>
       </c>
       <c r="V36" s="47" t="str">
         <f t="shared" si="12"/>
@@ -5668,7 +5668,7 @@
       </c>
       <c r="X36" s="47" t="str">
         <f t="shared" si="14"/>
-        <v>0000</v>
+        <v>1011</v>
       </c>
       <c r="Y36" s="47" t="str">
         <f t="shared" si="15"/>
@@ -5676,11 +5676,11 @@
       </c>
       <c r="Z36" s="47" t="str">
         <f t="shared" si="16"/>
-        <v>0011</v>
+        <v>0000</v>
       </c>
       <c r="AA36" s="47" t="str">
         <f t="shared" si="17"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="AB36" s="47" t="str">
         <f t="shared" si="18"/>
@@ -5700,7 +5700,7 @@
       </c>
       <c r="AG36" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X36,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>B</v>
       </c>
       <c r="AH36" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y36,'HEX GEN BACKEND'!L:L,0))</f>
@@ -5708,11 +5708,11 @@
       </c>
       <c r="AI36" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z36,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AJ36" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA36,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AK36" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB36,'HEX GEN BACKEND'!L:L,0))</f>
@@ -5724,7 +5724,7 @@
       </c>
       <c r="AN36" s="47" t="str">
         <f t="shared" si="10"/>
-        <v>4800383A</v>
+        <v>48B0003A</v>
       </c>
     </row>
     <row r="37" spans="1:40" x14ac:dyDescent="0.25">
@@ -5732,19 +5732,19 @@
         <v>165</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C37" s="40" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="D37" s="41" t="s">
         <v>114</v>
       </c>
       <c r="E37" s="42" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="F37" s="43" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="G37" s="44" t="s">
         <v>149</v>
@@ -5754,15 +5754,15 @@
       </c>
       <c r="I37" s="49" t="str">
         <f t="shared" si="20"/>
-        <v>0868343C</v>
+        <v>10A8003C</v>
       </c>
       <c r="L37" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B37,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>00001</v>
+        <v>00010</v>
       </c>
       <c r="M37" s="47" t="str">
         <f>IF(ISNUMBER(MATCH(C37,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C37,'HEX GEN BACKEND'!G:G,0)),C37)</f>
-        <v>000011</v>
+        <v>000101</v>
       </c>
       <c r="N37" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D37,'HEX GEN BACKEND'!D:D,0))</f>
@@ -5770,11 +5770,11 @@
       </c>
       <c r="O37" s="47" t="str">
         <f>IF(ISNUMBER(MATCH(E37,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E37,'HEX GEN BACKEND'!H:H,0)),E37)</f>
-        <v>000011</v>
+        <v>000000</v>
       </c>
       <c r="P37" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F37,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>010</v>
+        <v>000</v>
       </c>
       <c r="Q37" s="47" t="str">
         <f>IF(ISNUMBER(MATCH(G37,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G37,'HEX GEN BACKEND'!I:I,0)),G37)</f>
@@ -5786,19 +5786,19 @@
       </c>
       <c r="T37" s="47" t="str">
         <f t="shared" si="11"/>
-        <v>00001000011010000011010000111100</v>
+        <v>00010000101010000000000000111100</v>
       </c>
       <c r="V37" s="47" t="str">
         <f t="shared" si="12"/>
-        <v>0000</v>
+        <v>0001</v>
       </c>
       <c r="W37" s="47" t="str">
         <f t="shared" si="13"/>
-        <v>1000</v>
+        <v>0000</v>
       </c>
       <c r="X37" s="47" t="str">
         <f t="shared" si="14"/>
-        <v>0110</v>
+        <v>1010</v>
       </c>
       <c r="Y37" s="47" t="str">
         <f t="shared" si="15"/>
@@ -5806,11 +5806,11 @@
       </c>
       <c r="Z37" s="47" t="str">
         <f t="shared" si="16"/>
-        <v>0011</v>
+        <v>0000</v>
       </c>
       <c r="AA37" s="47" t="str">
         <f t="shared" si="17"/>
-        <v>0100</v>
+        <v>0000</v>
       </c>
       <c r="AB37" s="47" t="str">
         <f t="shared" si="18"/>
@@ -5822,15 +5822,15 @@
       </c>
       <c r="AE37" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V37,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF37" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W37,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="AG37" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X37,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>6</v>
+        <v>A</v>
       </c>
       <c r="AH37" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y37,'HEX GEN BACKEND'!L:L,0))</f>
@@ -5838,11 +5838,11 @@
       </c>
       <c r="AI37" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z37,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AJ37" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA37,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="AK37" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB37,'HEX GEN BACKEND'!L:L,0))</f>
@@ -5854,7 +5854,7 @@
       </c>
       <c r="AN37" s="47" t="str">
         <f t="shared" si="10"/>
-        <v>0868343C</v>
+        <v>10A8003C</v>
       </c>
     </row>
     <row r="38" spans="1:40" x14ac:dyDescent="0.25">
@@ -5862,13 +5862,13 @@
         <v>166</v>
       </c>
       <c r="B38" s="39" t="s">
-        <v>156</v>
+        <v>9</v>
       </c>
       <c r="C38" s="40" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="D38" s="41" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E38" s="42" t="s">
         <v>158</v>
@@ -5884,19 +5884,19 @@
       </c>
       <c r="I38" s="49" t="str">
         <f t="shared" si="20"/>
-        <v>C000003A</v>
+        <v>48B0003A</v>
       </c>
       <c r="L38" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B38,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>11000</v>
+        <v>01001</v>
       </c>
       <c r="M38" s="47" t="str">
         <f>IF(ISNUMBER(MATCH(C38,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C38,'HEX GEN BACKEND'!G:G,0)),C38)</f>
-        <v>000000</v>
+        <v>000101</v>
       </c>
       <c r="N38" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D38,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>000</v>
+        <v>100</v>
       </c>
       <c r="O38" s="47" t="str">
         <f>IF(ISNUMBER(MATCH(E38,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E38,'HEX GEN BACKEND'!H:H,0)),E38)</f>
@@ -5916,19 +5916,19 @@
       </c>
       <c r="T38" s="47" t="str">
         <f t="shared" si="11"/>
-        <v>11000000000000000000000000111010</v>
+        <v>01001000101100000000000000111010</v>
       </c>
       <c r="V38" s="47" t="str">
         <f t="shared" si="12"/>
-        <v>1100</v>
+        <v>0100</v>
       </c>
       <c r="W38" s="47" t="str">
         <f t="shared" si="13"/>
-        <v>0000</v>
+        <v>1000</v>
       </c>
       <c r="X38" s="47" t="str">
         <f t="shared" si="14"/>
-        <v>0000</v>
+        <v>1011</v>
       </c>
       <c r="Y38" s="47" t="str">
         <f t="shared" si="15"/>
@@ -5952,15 +5952,15 @@
       </c>
       <c r="AE38" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V38,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>C</v>
+        <v>4</v>
       </c>
       <c r="AF38" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W38,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AG38" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X38,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>0</v>
+        <v>B</v>
       </c>
       <c r="AH38" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y38,'HEX GEN BACKEND'!L:L,0))</f>
@@ -5984,471 +5984,527 @@
       </c>
       <c r="AN38" s="47" t="str">
         <f t="shared" si="10"/>
-        <v>C000003A</v>
+        <v>48B0003A</v>
       </c>
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A39" s="46" t="s">
         <v>167</v>
       </c>
-      <c r="B39" s="39"/>
-      <c r="C39" s="40"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="42"/>
-      <c r="F39" s="43"/>
-      <c r="G39" s="44"/>
-      <c r="H39" s="45"/>
-      <c r="I39" s="49" t="e">
+      <c r="B39" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C39" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="D39" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="E39" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" s="43" t="s">
+        <v>115</v>
+      </c>
+      <c r="G39" s="44" t="s">
+        <v>149</v>
+      </c>
+      <c r="H39" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="I39" s="49" t="str">
         <f t="shared" si="20"/>
-        <v>#N/A</v>
-      </c>
-      <c r="L39" s="47" t="e">
+        <v>08A8123C</v>
+      </c>
+      <c r="L39" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B39,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M39" s="47">
+        <v>00001</v>
+      </c>
+      <c r="M39" s="47" t="str">
         <f>IF(ISNUMBER(MATCH(C39,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C39,'HEX GEN BACKEND'!G:G,0)),C39)</f>
-        <v>0</v>
-      </c>
-      <c r="N39" s="47" t="e">
+        <v>000101</v>
+      </c>
+      <c r="N39" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D39,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O39" s="47">
+        <v>010</v>
+      </c>
+      <c r="O39" s="47" t="str">
         <f>IF(ISNUMBER(MATCH(E39,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E39,'HEX GEN BACKEND'!H:H,0)),E39)</f>
-        <v>0</v>
-      </c>
-      <c r="P39" s="47" t="e">
+        <v>000001</v>
+      </c>
+      <c r="P39" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F39,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q39" s="47">
+        <v>001</v>
+      </c>
+      <c r="Q39" s="47" t="str">
         <f>IF(ISNUMBER(MATCH(G39,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G39,'HEX GEN BACKEND'!I:I,0)),G39)</f>
-        <v>0</v>
-      </c>
-      <c r="R39" s="47" t="e">
+        <v>000111</v>
+      </c>
+      <c r="R39" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H39,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T39" s="47" t="e">
+        <v>100</v>
+      </c>
+      <c r="T39" s="47" t="str">
         <f t="shared" si="11"/>
-        <v>#N/A</v>
-      </c>
-      <c r="V39" s="47" t="e">
+        <v>00001000101010000001001000111100</v>
+      </c>
+      <c r="V39" s="47" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="W39" s="47" t="e">
+        <v>0000</v>
+      </c>
+      <c r="W39" s="47" t="str">
         <f t="shared" si="13"/>
-        <v>#N/A</v>
-      </c>
-      <c r="X39" s="47" t="e">
+        <v>1000</v>
+      </c>
+      <c r="X39" s="47" t="str">
         <f t="shared" si="14"/>
-        <v>#N/A</v>
-      </c>
-      <c r="Y39" s="47" t="e">
+        <v>1010</v>
+      </c>
+      <c r="Y39" s="47" t="str">
         <f t="shared" si="15"/>
-        <v>#N/A</v>
-      </c>
-      <c r="Z39" s="47" t="e">
+        <v>1000</v>
+      </c>
+      <c r="Z39" s="47" t="str">
         <f t="shared" si="16"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AA39" s="47" t="e">
+        <v>0001</v>
+      </c>
+      <c r="AA39" s="47" t="str">
         <f t="shared" si="17"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AB39" s="47" t="e">
+        <v>0010</v>
+      </c>
+      <c r="AB39" s="47" t="str">
         <f t="shared" si="18"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AC39" s="47" t="e">
+        <v>0011</v>
+      </c>
+      <c r="AC39" s="47" t="str">
         <f t="shared" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AE39" s="47" t="e">
+        <v>1100</v>
+      </c>
+      <c r="AE39" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V39,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AF39" s="47" t="e">
+        <v>0</v>
+      </c>
+      <c r="AF39" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W39,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AG39" s="47" t="e">
+        <v>8</v>
+      </c>
+      <c r="AG39" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X39,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AH39" s="47" t="e">
+        <v>A</v>
+      </c>
+      <c r="AH39" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y39,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AI39" s="47" t="e">
+        <v>8</v>
+      </c>
+      <c r="AI39" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z39,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AJ39" s="47" t="e">
+        <v>1</v>
+      </c>
+      <c r="AJ39" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA39,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AK39" s="47" t="e">
+        <v>2</v>
+      </c>
+      <c r="AK39" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB39,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AL39" s="47" t="e">
+        <v>3</v>
+      </c>
+      <c r="AL39" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC39,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AN39" s="47" t="e">
+        <v>C</v>
+      </c>
+      <c r="AN39" s="47" t="str">
         <f t="shared" si="10"/>
-        <v>#N/A</v>
+        <v>08A8123C</v>
       </c>
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A40" s="46" t="s">
         <v>168</v>
       </c>
-      <c r="B40" s="39"/>
-      <c r="C40" s="40"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="42"/>
-      <c r="F40" s="43"/>
-      <c r="G40" s="44"/>
-      <c r="H40" s="45"/>
-      <c r="I40" s="49" t="e">
+      <c r="B40" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="D40" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="E40" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="F40" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="G40" s="44" t="s">
+        <v>149</v>
+      </c>
+      <c r="H40" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="I40" s="49" t="str">
         <f t="shared" si="20"/>
-        <v>#N/A</v>
-      </c>
-      <c r="L40" s="47" t="e">
+        <v>4800383A</v>
+      </c>
+      <c r="L40" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B40,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M40" s="47">
+        <v>01001</v>
+      </c>
+      <c r="M40" s="47" t="str">
         <f>IF(ISNUMBER(MATCH(C40,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C40,'HEX GEN BACKEND'!G:G,0)),C40)</f>
-        <v>0</v>
-      </c>
-      <c r="N40" s="47" t="e">
+        <v>000000</v>
+      </c>
+      <c r="N40" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D40,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O40" s="47">
+        <v>000</v>
+      </c>
+      <c r="O40" s="47" t="str">
         <f>IF(ISNUMBER(MATCH(E40,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E40,'HEX GEN BACKEND'!H:H,0)),E40)</f>
-        <v>0</v>
-      </c>
-      <c r="P40" s="47" t="e">
+        <v>000011</v>
+      </c>
+      <c r="P40" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F40,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q40" s="47">
+        <v>100</v>
+      </c>
+      <c r="Q40" s="47" t="str">
         <f>IF(ISNUMBER(MATCH(G40,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G40,'HEX GEN BACKEND'!I:I,0)),G40)</f>
-        <v>0</v>
-      </c>
-      <c r="R40" s="47" t="e">
+        <v>000111</v>
+      </c>
+      <c r="R40" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H40,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T40" s="47" t="e">
+        <v>010</v>
+      </c>
+      <c r="T40" s="47" t="str">
         <f t="shared" si="11"/>
-        <v>#N/A</v>
-      </c>
-      <c r="V40" s="47" t="e">
+        <v>01001000000000000011100000111010</v>
+      </c>
+      <c r="V40" s="47" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="W40" s="47" t="e">
+        <v>0100</v>
+      </c>
+      <c r="W40" s="47" t="str">
         <f t="shared" si="13"/>
-        <v>#N/A</v>
-      </c>
-      <c r="X40" s="47" t="e">
+        <v>1000</v>
+      </c>
+      <c r="X40" s="47" t="str">
         <f t="shared" si="14"/>
-        <v>#N/A</v>
-      </c>
-      <c r="Y40" s="47" t="e">
+        <v>0000</v>
+      </c>
+      <c r="Y40" s="47" t="str">
         <f t="shared" si="15"/>
-        <v>#N/A</v>
-      </c>
-      <c r="Z40" s="47" t="e">
+        <v>0000</v>
+      </c>
+      <c r="Z40" s="47" t="str">
         <f t="shared" si="16"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AA40" s="47" t="e">
+        <v>0011</v>
+      </c>
+      <c r="AA40" s="47" t="str">
         <f t="shared" si="17"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AB40" s="47" t="e">
+        <v>1000</v>
+      </c>
+      <c r="AB40" s="47" t="str">
         <f t="shared" si="18"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AC40" s="47" t="e">
+        <v>0011</v>
+      </c>
+      <c r="AC40" s="47" t="str">
         <f t="shared" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AE40" s="47" t="e">
+        <v>1010</v>
+      </c>
+      <c r="AE40" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V40,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AF40" s="47" t="e">
+        <v>4</v>
+      </c>
+      <c r="AF40" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W40,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AG40" s="47" t="e">
+        <v>8</v>
+      </c>
+      <c r="AG40" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X40,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AH40" s="47" t="e">
+        <v>0</v>
+      </c>
+      <c r="AH40" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y40,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AI40" s="47" t="e">
+        <v>0</v>
+      </c>
+      <c r="AI40" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z40,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AJ40" s="47" t="e">
+        <v>3</v>
+      </c>
+      <c r="AJ40" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA40,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AK40" s="47" t="e">
+        <v>8</v>
+      </c>
+      <c r="AK40" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB40,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AL40" s="47" t="e">
+        <v>3</v>
+      </c>
+      <c r="AL40" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC40,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AN40" s="47" t="e">
+        <v>A</v>
+      </c>
+      <c r="AN40" s="47" t="str">
         <f t="shared" si="10"/>
-        <v>#N/A</v>
+        <v>4800383A</v>
       </c>
     </row>
     <row r="41" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A41" s="46" t="s">
         <v>169</v>
       </c>
-      <c r="B41" s="39"/>
-      <c r="C41" s="40"/>
-      <c r="D41" s="41"/>
-      <c r="E41" s="42"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="44"/>
-      <c r="H41" s="45"/>
-      <c r="I41" s="49" t="e">
+      <c r="B41" s="39" t="s">
+        <v>2</v>
+      </c>
+      <c r="C41" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="D41" s="41" t="s">
+        <v>114</v>
+      </c>
+      <c r="E41" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="F41" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="G41" s="44" t="s">
+        <v>149</v>
+      </c>
+      <c r="H41" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="I41" s="49" t="str">
         <f t="shared" si="20"/>
-        <v>#N/A</v>
-      </c>
-      <c r="L41" s="47" t="e">
+        <v>0868343C</v>
+      </c>
+      <c r="L41" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B41,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M41" s="47">
+        <v>00001</v>
+      </c>
+      <c r="M41" s="47" t="str">
         <f>IF(ISNUMBER(MATCH(C41,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C41,'HEX GEN BACKEND'!G:G,0)),C41)</f>
-        <v>0</v>
-      </c>
-      <c r="N41" s="47" t="e">
+        <v>000011</v>
+      </c>
+      <c r="N41" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D41,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O41" s="47">
+        <v>010</v>
+      </c>
+      <c r="O41" s="47" t="str">
         <f>IF(ISNUMBER(MATCH(E41,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E41,'HEX GEN BACKEND'!H:H,0)),E41)</f>
-        <v>0</v>
-      </c>
-      <c r="P41" s="47" t="e">
+        <v>000011</v>
+      </c>
+      <c r="P41" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F41,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q41" s="47">
+        <v>010</v>
+      </c>
+      <c r="Q41" s="47" t="str">
         <f>IF(ISNUMBER(MATCH(G41,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G41,'HEX GEN BACKEND'!I:I,0)),G41)</f>
-        <v>0</v>
-      </c>
-      <c r="R41" s="47" t="e">
+        <v>000111</v>
+      </c>
+      <c r="R41" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H41,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T41" s="47" t="e">
+        <v>100</v>
+      </c>
+      <c r="T41" s="47" t="str">
         <f t="shared" si="11"/>
-        <v>#N/A</v>
-      </c>
-      <c r="V41" s="47" t="e">
+        <v>00001000011010000011010000111100</v>
+      </c>
+      <c r="V41" s="47" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="W41" s="47" t="e">
+        <v>0000</v>
+      </c>
+      <c r="W41" s="47" t="str">
         <f t="shared" si="13"/>
-        <v>#N/A</v>
-      </c>
-      <c r="X41" s="47" t="e">
+        <v>1000</v>
+      </c>
+      <c r="X41" s="47" t="str">
         <f t="shared" si="14"/>
-        <v>#N/A</v>
-      </c>
-      <c r="Y41" s="47" t="e">
+        <v>0110</v>
+      </c>
+      <c r="Y41" s="47" t="str">
         <f t="shared" si="15"/>
-        <v>#N/A</v>
-      </c>
-      <c r="Z41" s="47" t="e">
+        <v>1000</v>
+      </c>
+      <c r="Z41" s="47" t="str">
         <f t="shared" si="16"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AA41" s="47" t="e">
+        <v>0011</v>
+      </c>
+      <c r="AA41" s="47" t="str">
         <f t="shared" si="17"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AB41" s="47" t="e">
+        <v>0100</v>
+      </c>
+      <c r="AB41" s="47" t="str">
         <f t="shared" si="18"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AC41" s="47" t="e">
+        <v>0011</v>
+      </c>
+      <c r="AC41" s="47" t="str">
         <f t="shared" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AE41" s="47" t="e">
+        <v>1100</v>
+      </c>
+      <c r="AE41" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V41,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AF41" s="47" t="e">
+        <v>0</v>
+      </c>
+      <c r="AF41" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W41,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AG41" s="47" t="e">
+        <v>8</v>
+      </c>
+      <c r="AG41" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X41,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AH41" s="47" t="e">
+        <v>6</v>
+      </c>
+      <c r="AH41" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y41,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AI41" s="47" t="e">
+        <v>8</v>
+      </c>
+      <c r="AI41" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z41,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AJ41" s="47" t="e">
+        <v>3</v>
+      </c>
+      <c r="AJ41" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA41,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AK41" s="47" t="e">
+        <v>4</v>
+      </c>
+      <c r="AK41" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB41,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AL41" s="47" t="e">
+        <v>3</v>
+      </c>
+      <c r="AL41" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC41,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AN41" s="47" t="e">
+        <v>C</v>
+      </c>
+      <c r="AN41" s="47" t="str">
         <f t="shared" si="10"/>
-        <v>#N/A</v>
+        <v>0868343C</v>
       </c>
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A42" s="46" t="s">
         <v>170</v>
       </c>
-      <c r="B42" s="39"/>
-      <c r="C42" s="40"/>
-      <c r="D42" s="41"/>
-      <c r="E42" s="42"/>
-      <c r="F42" s="43"/>
-      <c r="G42" s="44"/>
-      <c r="H42" s="45"/>
-      <c r="I42" s="49" t="e">
+      <c r="B42" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="C42" s="40" t="s">
+        <v>158</v>
+      </c>
+      <c r="D42" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="E42" s="42" t="s">
+        <v>158</v>
+      </c>
+      <c r="F42" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="G42" s="44" t="s">
+        <v>149</v>
+      </c>
+      <c r="H42" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="I42" s="49" t="str">
         <f t="shared" si="20"/>
-        <v>#N/A</v>
-      </c>
-      <c r="L42" s="47" t="e">
+        <v>C000003A</v>
+      </c>
+      <c r="L42" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!B:B,MATCH(B42,'HEX GEN BACKEND'!A:A,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M42" s="47">
+        <v>11000</v>
+      </c>
+      <c r="M42" s="47" t="str">
         <f>IF(ISNUMBER(MATCH(C42,'HEX GEN BACKEND'!G:G,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(C42,'HEX GEN BACKEND'!G:G,0)),C42)</f>
-        <v>0</v>
-      </c>
-      <c r="N42" s="47" t="e">
+        <v>000000</v>
+      </c>
+      <c r="N42" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(D42,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O42" s="47">
+        <v>000</v>
+      </c>
+      <c r="O42" s="47" t="str">
         <f>IF(ISNUMBER(MATCH(E42,'HEX GEN BACKEND'!H:H,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(E42,'HEX GEN BACKEND'!H:H,0)),E42)</f>
-        <v>0</v>
-      </c>
-      <c r="P42" s="47" t="e">
+        <v>000000</v>
+      </c>
+      <c r="P42" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(F42,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="Q42" s="47">
+        <v>000</v>
+      </c>
+      <c r="Q42" s="47" t="str">
         <f>IF(ISNUMBER(MATCH(G42,'HEX GEN BACKEND'!I:I,0)),INDEX('HEX GEN BACKEND'!J:J,MATCH(G42,'HEX GEN BACKEND'!I:I,0)),G42)</f>
-        <v>0</v>
-      </c>
-      <c r="R42" s="47" t="e">
+        <v>000111</v>
+      </c>
+      <c r="R42" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!E:E,MATCH(H42,'HEX GEN BACKEND'!D:D,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T42" s="47" t="e">
+        <v>010</v>
+      </c>
+      <c r="T42" s="47" t="str">
         <f t="shared" si="11"/>
-        <v>#N/A</v>
-      </c>
-      <c r="V42" s="47" t="e">
+        <v>11000000000000000000000000111010</v>
+      </c>
+      <c r="V42" s="47" t="str">
         <f t="shared" si="12"/>
-        <v>#N/A</v>
-      </c>
-      <c r="W42" s="47" t="e">
+        <v>1100</v>
+      </c>
+      <c r="W42" s="47" t="str">
         <f t="shared" si="13"/>
-        <v>#N/A</v>
-      </c>
-      <c r="X42" s="47" t="e">
+        <v>0000</v>
+      </c>
+      <c r="X42" s="47" t="str">
         <f t="shared" si="14"/>
-        <v>#N/A</v>
-      </c>
-      <c r="Y42" s="47" t="e">
+        <v>0000</v>
+      </c>
+      <c r="Y42" s="47" t="str">
         <f t="shared" si="15"/>
-        <v>#N/A</v>
-      </c>
-      <c r="Z42" s="47" t="e">
+        <v>0000</v>
+      </c>
+      <c r="Z42" s="47" t="str">
         <f t="shared" si="16"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AA42" s="47" t="e">
+        <v>0000</v>
+      </c>
+      <c r="AA42" s="47" t="str">
         <f t="shared" si="17"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AB42" s="47" t="e">
+        <v>0000</v>
+      </c>
+      <c r="AB42" s="47" t="str">
         <f t="shared" si="18"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AC42" s="47" t="e">
+        <v>0011</v>
+      </c>
+      <c r="AC42" s="47" t="str">
         <f t="shared" si="19"/>
-        <v>#N/A</v>
-      </c>
-      <c r="AE42" s="47" t="e">
+        <v>1010</v>
+      </c>
+      <c r="AE42" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!V42,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AF42" s="47" t="e">
+        <v>C</v>
+      </c>
+      <c r="AF42" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!W42,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AG42" s="47" t="e">
+        <v>0</v>
+      </c>
+      <c r="AG42" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!X42,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AH42" s="47" t="e">
+        <v>0</v>
+      </c>
+      <c r="AH42" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Y42,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AI42" s="47" t="e">
+        <v>0</v>
+      </c>
+      <c r="AI42" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!Z42,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AJ42" s="47" t="e">
+        <v>0</v>
+      </c>
+      <c r="AJ42" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AA42,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AK42" s="47" t="e">
+        <v>0</v>
+      </c>
+      <c r="AK42" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AB42,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AL42" s="47" t="e">
+        <v>3</v>
+      </c>
+      <c r="AL42" s="47" t="str">
         <f>INDEX('HEX GEN BACKEND'!M:M,MATCH('HEX GEN'!AC42,'HEX GEN BACKEND'!L:L,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="AN42" s="47" t="e">
+        <v>A</v>
+      </c>
+      <c r="AN42" s="47" t="str">
         <f t="shared" si="10"/>
-        <v>#N/A</v>
+        <v>C000003A</v>
       </c>
     </row>
     <row r="43" spans="1:40" x14ac:dyDescent="0.25">

</xml_diff>